<commit_message>
Updated Excel & crendential
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Module_Name</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>User99341</t>
+  </si>
+  <si>
+    <t>ToggleTc005_VerifyTheToggleButtonAndFunctionalityOfToggleButtonOnInstitutionPageRecord</t>
+  </si>
+  <si>
+    <t>ToggleTc006_CreateNewCustomSDG</t>
   </si>
 </sst>
 </file>
@@ -380,7 +386,403 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="121">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1692,22 +2094,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="84" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="83" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1724,10 +2126,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,319 +2292,419 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="80" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="106" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="107" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="108" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="77" priority="91" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="113" priority="109" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="92" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="112" priority="110" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="93" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="111" priority="111" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="74" priority="94" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="110" priority="112" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="95" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="109" priority="113" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="96" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="108" priority="114" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="71" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="97" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="98" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="99" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="68" priority="82" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="104" priority="100" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="83" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="103" priority="101" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="84" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="102" priority="102" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="65" priority="85" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="101" priority="103" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="86" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="100" priority="104" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="87" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="99" priority="105" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="88" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="89" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="90" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="59" priority="73" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="95" priority="91" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="74" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="94" priority="92" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="75" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="93" priority="93" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="56" priority="76" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="92" priority="94" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="77" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="78" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="90" priority="96" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="79" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="80" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="81" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="50" priority="55" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="86" priority="73" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="85" priority="74" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="57" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="84" priority="75" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="47" priority="58" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="83" priority="76" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="59" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="82" priority="77" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="60" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="81" priority="78" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="80" priority="58" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="79" priority="59" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="78" priority="60" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="77" priority="61" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="76" priority="62" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="75" priority="63" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="74" priority="52" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="73" priority="53" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="72" priority="54" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="71" priority="55" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="70" priority="56" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="69" priority="57" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="67" priority="47" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="66" priority="48" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="65" priority="49" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="64" priority="50" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="63" priority="51" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="62" priority="40" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="60" priority="42" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="59" priority="43" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="58" priority="44" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="57" priority="45" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="56" priority="34" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="55" priority="35" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="54" priority="36" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="53" priority="37" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="52" priority="38" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="51" priority="39" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="31" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="32" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="33" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="28" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="29" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="30" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="25" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="26" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="27" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="22" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="23" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="24" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="19" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="20" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="21" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="35" priority="16" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="18" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="12" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C10">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C12">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E12">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Added tc006 & tc007 of Toggle
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="8190" windowWidth="16380" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Modules" r:id="rId1" sheetId="1"/>
-    <sheet name="TestCases" r:id="rId2" sheetId="10"/>
-    <sheet name="Users" r:id="rId3" sheetId="3"/>
+    <sheet name="Modules" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="10" r:id="rId2"/>
+    <sheet name="Users" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Module_Name</t>
   </si>
@@ -172,20 +172,21 @@
     <t>ToggleTc005_VerifyTheRetainAndDefaultSelectionOfToggleButton</t>
   </si>
   <si>
-    <t>Pass</t>
+    <t>ToggleTc007_VerifyToAddNewToggleButtonWithMaxAndSpecialCharacter</t>
+  </si>
+  <si>
+    <t>ToggleTc008_CreateNewToggleButtonAsADefaultButton</t>
   </si>
   <si>
     <t>Fail: The following asserts failed:
-	Able to Enter Value : Custom SDG to label : SDG Name (Toggle.java:639)	Screenshot Name: ToggleTc006_CreateNewCustomSDG2020_12_17_06_53_48.png	 did not expect to find [true] but found [false],
-	Able to Enter Value : Custom SDG to label : SDG Tag (Toggle.java:639)	Screenshot Name: ToggleTc006_CreateNewCustomSDG2020_12_17_06_53_50.png	 did not expect to find [true] but found [false],
-	Able to Enter Value : navpeII__Pipeline__c to label : sObjectName (Toggle.java:639)	Screenshot Name: ToggleTc006_CreateNewCustomSDG2020_12_17_06_53_53.png	 did not expect to find [true] but found [false]</t>
+	After Save Active Deals with All Stages !@#$%^&amp;*() @#$%^&amp;*Deals:Custom SDG should be selected  (Toggle.java:871)	Screenshot Name: ToggleTc008_CreateNewToggleButtonAsADefaultButton2020_12_21_03_48_12.png	 did not expect to find [true] but found [false],
+	After Save Active Deals with All Stages !@#$%^&amp;*() @#$%^&amp;*Deals:Custom SDG should be selected  (Toggle.java:900)	Screenshot Name: ToggleTc008_CreateNewToggleButtonAsADefaultButton2020_12_21_03_48_47.png	 did not expect to find [true] but found [false]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,54 +353,54 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="112">
+  <dxfs count="130">
     <dxf>
       <font>
         <b/>
@@ -698,6 +699,78 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -725,6 +798,78 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -833,6 +978,60 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1617,7 +1816,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1702,10 +1901,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1740,7 +1939,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1775,7 +1974,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1869,21 +2068,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1900,7 +2099,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1952,29 +2151,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="10" max="1025" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="1" max="7" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="8:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1982,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1990,7 +2189,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="15.75" r="3" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2" t="s">
         <v>30</v>
       </c>
@@ -1998,7 +2197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H4" s="2" t="s">
         <v>31</v>
       </c>
@@ -2008,54 +2207,54 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule dxfId="111" operator="equal" priority="6" type="cellIs">
+    <cfRule type="cellIs" dxfId="129" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule dxfId="110" operator="equal" priority="7" type="cellIs">
+    <cfRule type="cellIs" dxfId="128" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule dxfId="109" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="127" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule dxfId="108" operator="equal" priority="2" type="cellIs">
+    <cfRule type="cellIs" dxfId="126" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="I2:I4" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="87.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="18" r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2072,7 +2271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -2087,7 +2286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="15.75" r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -2102,7 +2301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -2117,7 +2316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="15.75" r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -2132,7 +2331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="15.75" r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -2147,7 +2346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="15.75" r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
@@ -2164,7 +2363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="15.75" r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
@@ -2181,7 +2380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
@@ -2198,7 +2397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
@@ -2215,7 +2414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -2232,7 +2431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -2249,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>45</v>
       </c>
@@ -2257,444 +2456,544 @@
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7">
-    <cfRule dxfId="107" operator="equal" priority="115" type="cellIs">
+    <cfRule type="cellIs" dxfId="125" priority="133" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="106" operator="equal" priority="116" type="cellIs">
+    <cfRule type="cellIs" dxfId="124" priority="134" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="105" operator="equal" priority="117" type="cellIs">
+    <cfRule type="cellIs" dxfId="123" priority="135" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule dxfId="104" operator="containsText" priority="118" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="122" priority="136" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule dxfId="103" operator="containsText" priority="119" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="121" priority="137" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule dxfId="102" operator="containsText" priority="120" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="120" priority="138" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule dxfId="101" operator="containsText" priority="121" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="119" priority="139" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule dxfId="100" operator="containsText" priority="122" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="118" priority="140" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule dxfId="99" operator="containsText" priority="123" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="117" priority="141" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule dxfId="98" operator="equal" priority="106" type="cellIs">
+    <cfRule type="cellIs" dxfId="116" priority="124" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="97" operator="equal" priority="107" type="cellIs">
+    <cfRule type="cellIs" dxfId="115" priority="125" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="96" operator="equal" priority="108" type="cellIs">
+    <cfRule type="cellIs" dxfId="114" priority="126" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule dxfId="95" operator="containsText" priority="109" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="113" priority="127" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule dxfId="94" operator="containsText" priority="110" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="112" priority="128" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule dxfId="93" operator="containsText" priority="111" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="111" priority="129" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule dxfId="92" operator="containsText" priority="112" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="110" priority="130" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule dxfId="91" operator="containsText" priority="113" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="109" priority="131" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule dxfId="90" operator="containsText" priority="114" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="108" priority="132" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule dxfId="89" operator="equal" priority="97" type="cellIs">
+    <cfRule type="cellIs" dxfId="107" priority="115" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="88" operator="equal" priority="98" type="cellIs">
+    <cfRule type="cellIs" dxfId="106" priority="116" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="87" operator="equal" priority="99" type="cellIs">
+    <cfRule type="cellIs" dxfId="105" priority="117" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule dxfId="86" operator="containsText" priority="100" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="104" priority="118" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule dxfId="85" operator="containsText" priority="101" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="103" priority="119" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule dxfId="84" operator="containsText" priority="102" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="102" priority="120" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule dxfId="83" operator="containsText" priority="103" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="101" priority="121" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule dxfId="82" operator="containsText" priority="104" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="100" priority="122" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule dxfId="81" operator="containsText" priority="105" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="99" priority="123" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule dxfId="80" operator="equal" priority="88" type="cellIs">
+    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="79" operator="equal" priority="89" type="cellIs">
+    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="78" operator="equal" priority="90" type="cellIs">
+    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule dxfId="77" operator="containsText" priority="82" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="95" priority="100" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule dxfId="76" operator="containsText" priority="83" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="94" priority="101" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule dxfId="75" operator="containsText" priority="84" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="93" priority="102" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule dxfId="74" operator="containsText" priority="85" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="92" priority="103" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule dxfId="73" operator="containsText" priority="86" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="91" priority="104" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule dxfId="72" operator="containsText" priority="87" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="90" priority="105" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule dxfId="71" operator="containsText" priority="67" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="89" priority="85" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule dxfId="70" operator="containsText" priority="68" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="88" priority="86" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule dxfId="69" operator="containsText" priority="69" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule dxfId="68" operator="containsText" priority="70" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="86" priority="88" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule dxfId="67" operator="containsText" priority="71" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule dxfId="66" operator="containsText" priority="72" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="84" priority="90" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule dxfId="65" operator="containsText" priority="61" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="83" priority="79" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule dxfId="64" operator="containsText" priority="62" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="82" priority="80" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule dxfId="63" operator="containsText" priority="63" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="81" priority="81" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule dxfId="62" operator="containsText" priority="64" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="80" priority="82" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule dxfId="61" operator="containsText" priority="65" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule dxfId="60" operator="containsText" priority="66" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule dxfId="59" operator="containsText" priority="55" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="77" priority="73" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule dxfId="58" operator="containsText" priority="56" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="76" priority="74" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule dxfId="57" operator="containsText" priority="57" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="75" priority="75" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule dxfId="56" operator="containsText" priority="58" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="74" priority="76" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule dxfId="55" operator="containsText" priority="59" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule dxfId="54" operator="containsText" priority="60" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="72" priority="78" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule dxfId="53" operator="containsText" priority="49" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="71" priority="67" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule dxfId="52" operator="containsText" priority="50" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule dxfId="51" operator="containsText" priority="51" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule dxfId="50" operator="containsText" priority="52" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule dxfId="49" operator="containsText" priority="53" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule dxfId="48" operator="containsText" priority="54" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule dxfId="47" operator="containsText" priority="43" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="65" priority="61" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule dxfId="46" operator="containsText" priority="44" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="64" priority="62" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule dxfId="45" operator="containsText" priority="45" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule dxfId="44" operator="containsText" priority="46" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="62" priority="64" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule dxfId="43" operator="containsText" priority="47" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule dxfId="42" operator="containsText" priority="48" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="60" priority="66" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule dxfId="41" operator="equal" priority="40" type="cellIs">
+    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="40" operator="equal" priority="41" type="cellIs">
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="39" operator="equal" priority="42" type="cellIs">
+    <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule dxfId="38" operator="equal" priority="37" type="cellIs">
+    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="37" operator="equal" priority="38" type="cellIs">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="36" operator="equal" priority="39" type="cellIs">
+    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule dxfId="35" operator="equal" priority="34" type="cellIs">
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="34" operator="equal" priority="35" type="cellIs">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="33" operator="equal" priority="36" type="cellIs">
+    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule dxfId="32" operator="equal" priority="31" type="cellIs">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="31" operator="equal" priority="32" type="cellIs">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="30" operator="equal" priority="33" type="cellIs">
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule dxfId="29" operator="equal" priority="28" type="cellIs">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="28" operator="equal" priority="29" type="cellIs">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="27" operator="equal" priority="30" type="cellIs">
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule dxfId="26" operator="equal" priority="25" type="cellIs">
+    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="25" operator="equal" priority="26" type="cellIs">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="24" operator="equal" priority="27" type="cellIs">
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule dxfId="23" operator="containsText" priority="19" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
     </cfRule>
-    <cfRule dxfId="22" operator="containsText" priority="20" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
     </cfRule>
-    <cfRule dxfId="21" operator="containsText" priority="21" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule dxfId="20" operator="containsText" priority="22" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
     </cfRule>
-    <cfRule dxfId="19" operator="containsText" priority="23" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
     </cfRule>
-    <cfRule dxfId="18" operator="containsText" priority="24" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule dxfId="17" operator="equal" priority="16" type="cellIs">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="16" operator="equal" priority="17" type="cellIs">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="15" operator="equal" priority="18" type="cellIs">
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule dxfId="14" operator="containsText" priority="10" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
     </cfRule>
-    <cfRule dxfId="13" operator="containsText" priority="11" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
     </cfRule>
-    <cfRule dxfId="12" operator="containsText" priority="12" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule dxfId="11" operator="containsText" priority="13" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
     </cfRule>
-    <cfRule dxfId="10" operator="containsText" priority="14" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
     </cfRule>
-    <cfRule dxfId="9" operator="containsText" priority="15" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule dxfId="8" operator="equal" priority="7" type="cellIs">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule dxfId="7" operator="equal" priority="8" type="cellIs">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule dxfId="6" operator="equal" priority="9" type="cellIs">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule dxfId="5" operator="containsText" priority="1" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
     </cfRule>
-    <cfRule dxfId="4" operator="containsText" priority="2" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
     </cfRule>
-    <cfRule dxfId="3" operator="containsText" priority="3" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule dxfId="2" operator="containsText" priority="4" text="Skip:" type="containsText">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
     </cfRule>
-    <cfRule dxfId="1" operator="containsText" priority="5" text="Fail" type="containsText">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="containsText" priority="6" text="Pass" type="containsText">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C2:C13" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C15">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E13" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation showDropDown="1" showErrorMessage="1" showInputMessage="1" sqref="C1">
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="D3" pane="bottomLeft" sqref="D3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.42578125" collapsed="true"/>
-    <col min="6" max="1025" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="4" width="19" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="1025" width="19" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2777,9 +3076,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E3"/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test case file
Signed-off-by: Ankit Jaiswal <ajaiswal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B825DC83-0209-478E-B65A-B755973E0C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>Module_Name</t>
   </si>
@@ -181,12 +182,26 @@
     <t>Fail: The following asserts failed:
 	After Save Active Deals with All Stages !@#$%^&amp;*() @#$%^&amp;*Deals:Custom SDG should be selected  (Toggle.java:871)	Screenshot Name: ToggleTc008_CreateNewToggleButtonAsADefaultButton2020_12_21_03_48_12.png	 did not expect to find [true] but found [false],
 	After Save Active Deals with All Stages !@#$%^&amp;*() @#$%^&amp;*Deals:Custom SDG should be selected  (Toggle.java:900)	Screenshot Name: ToggleTc008_CreateNewToggleButtonAsADefaultButton2020_12_21_03_48_47.png	 did not expect to find [true] but found [false]</t>
+  </si>
+  <si>
+    <t>FSTc002_verifyDefaultFieldSet</t>
+  </si>
+  <si>
+    <t>FSTc003_createFieldSet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail: Element not found: Linghting Pop-Up Close Icon
+Reason: Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.xpath: //a[text()='Close']' (tried for 10 second(s) with 500 milliseconds interval)
+Cause: </t>
+  </si>
+  <si>
+    <t>FSTc004_CreatePreconditionData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,7 +373,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -393,14 +408,413 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="2"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="130">
+  <dxfs count="166">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2158,7 +2572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2207,27 +2621,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="129" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="128" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="127" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="126" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2238,11 +2652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,272 +2913,449 @@
         <v>10</v>
       </c>
     </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="125" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="169" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="170" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="171" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="122" priority="136" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="158" priority="172" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="137" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="157" priority="173" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="138" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="156" priority="174" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="119" priority="139" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="155" priority="175" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="140" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="154" priority="176" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="141" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="153" priority="177" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="116" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="160" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="161" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="162" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="113" priority="127" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="149" priority="163" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="128" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="148" priority="164" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="129" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="147" priority="165" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="110" priority="130" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="146" priority="166" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="131" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="145" priority="167" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="132" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="144" priority="168" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="107" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="151" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="152" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="153" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="104" priority="118" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="140" priority="154" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="119" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="139" priority="155" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="120" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="138" priority="156" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="101" priority="121" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="137" priority="157" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="122" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="136" priority="158" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="123" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="135" priority="159" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="142" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="143" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="144" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="95" priority="100" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="131" priority="136" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="101" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="130" priority="137" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="102" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="129" priority="138" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="92" priority="103" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="128" priority="139" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="104" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="127" priority="140" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="105" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="126" priority="141" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="89" priority="85" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="125" priority="121" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="86" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="124" priority="122" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="123" priority="123" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="86" priority="88" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="122" priority="124" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="121" priority="125" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="90" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="120" priority="126" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="83" priority="79" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="119" priority="115" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="80" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="118" priority="116" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="81" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="117" priority="117" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="80" priority="82" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="116" priority="118" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="115" priority="119" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="114" priority="120" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
+    <cfRule type="containsText" dxfId="113" priority="109" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="110" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="111" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="containsText" dxfId="110" priority="112" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="113" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="114" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="107" priority="103" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="104" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="105" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="104" priority="106" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="107" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="108" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="101" priority="97" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="98" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="99" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="98" priority="100" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="102" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="95" priority="94" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="95" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="96" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="92" priority="91" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="93" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="89" priority="88" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="89" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="90" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="86" priority="85" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="86" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="87" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="83" priority="82" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="83" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="84" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="80" priority="79" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="80" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="81" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
     <cfRule type="containsText" dxfId="77" priority="73" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="76" priority="74" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="75" priority="75" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
+      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
     <cfRule type="containsText" dxfId="74" priority="76" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="72" priority="78" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="71" priority="67" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="65" priority="61" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="62" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="62" priority="64" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="66" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
+      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="71" priority="70" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="71" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="72" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
+  <conditionalFormatting sqref="D12">
+    <cfRule type="containsText" dxfId="68" priority="64" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
+  <conditionalFormatting sqref="D13">
+    <cfRule type="containsText" dxfId="59" priority="55" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="56" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="containsText" dxfId="56" priority="58" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="60" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
     <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
@@ -2775,29 +3366,29 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="D14">
+    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="containsText" dxfId="47" priority="49" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
     <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
@@ -2808,128 +3399,29 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+  <conditionalFormatting sqref="D15">
     <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
     <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E18">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
@@ -2940,38 +3432,38 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D16:D18">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D18">
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C18" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E18" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2981,7 +3473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3076,7 +3568,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updated TestCases for Toggle TC007-TC010
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B825DC83-0209-478E-B65A-B755973E0C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <t>Module_Name</t>
   </si>
@@ -179,29 +178,25 @@
     <t>ToggleTc008_CreateNewToggleButtonAsADefaultButton</t>
   </si>
   <si>
-    <t>Fail: The following asserts failed:
-	After Save Active Deals with All Stages !@#$%^&amp;*() @#$%^&amp;*Deals:Custom SDG should be selected  (Toggle.java:871)	Screenshot Name: ToggleTc008_CreateNewToggleButtonAsADefaultButton2020_12_21_03_48_12.png	 did not expect to find [true] but found [false],
-	After Save Active Deals with All Stages !@#$%^&amp;*() @#$%^&amp;*Deals:Custom SDG should be selected  (Toggle.java:900)	Screenshot Name: ToggleTc008_CreateNewToggleButtonAsADefaultButton2020_12_21_03_48_47.png	 did not expect to find [true] but found [false]</t>
-  </si>
-  <si>
     <t>FSTc002_verifyDefaultFieldSet</t>
   </si>
   <si>
     <t>FSTc003_createFieldSet</t>
   </si>
   <si>
-    <t xml:space="preserve">Fail: Element not found: Linghting Pop-Up Close Icon
-Reason: Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.xpath: //a[text()='Close']' (tried for 10 second(s) with 500 milliseconds interval)
-Cause: </t>
-  </si>
-  <si>
     <t>FSTc004_CreatePreconditionData</t>
+  </si>
+  <si>
+    <t>ToggleTc009_VerifyTheToggleButtonAndFunctionalityOfToggleButtonOnDealPageRecord</t>
+  </si>
+  <si>
+    <t>ToggleTc010_VerifyTheRetainAndDefaultSelectionOfToggleButton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,7 +245,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +262,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -373,7 +374,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,14 +412,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="166">
+  <dxfs count="178">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -519,78 +631,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -686,6 +726,105 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2572,7 +2711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2621,27 +2760,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="165" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="164" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="163" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="162" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2652,11 +2791,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,7 +2825,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="8"/>
@@ -2761,7 +2900,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="8">
@@ -2907,7 +3046,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>10</v>
@@ -2915,10 +3054,12 @@
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
@@ -2930,10 +3071,12 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
@@ -2944,526 +3087,534 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>54</v>
+      <c r="A18" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="161" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="187" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="188" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="189" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="158" priority="172" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="170" priority="190" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="173" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="169" priority="191" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="174" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="168" priority="192" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="155" priority="175" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="167" priority="193" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="176" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="166" priority="194" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="177" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="165" priority="195" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="152" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="178" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="179" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="180" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="149" priority="163" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="161" priority="181" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="164" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="160" priority="182" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="165" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="159" priority="183" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="146" priority="166" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="158" priority="184" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="167" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="157" priority="185" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="168" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="156" priority="186" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="143" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="169" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="170" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="171" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="140" priority="154" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="152" priority="172" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="155" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="151" priority="173" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="156" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="150" priority="174" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="137" priority="157" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="149" priority="175" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="158" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="148" priority="176" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="159" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="147" priority="177" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="134" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="160" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="161" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="162" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="131" priority="136" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="143" priority="154" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="137" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="142" priority="155" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="138" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="141" priority="156" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="128" priority="139" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="140" priority="157" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="140" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="139" priority="158" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="141" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="138" priority="159" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="125" priority="121" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="137" priority="139" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="122" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="136" priority="140" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="123" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="135" priority="141" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="122" priority="124" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="134" priority="142" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="125" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="133" priority="143" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="126" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="132" priority="144" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="119" priority="115" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="131" priority="133" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="116" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="130" priority="134" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="117" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="129" priority="135" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="116" priority="118" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="128" priority="136" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="119" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="127" priority="137" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="120" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="126" priority="138" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="113" priority="109" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="125" priority="127" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="110" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="124" priority="128" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="111" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="123" priority="129" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="110" priority="112" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="122" priority="130" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="113" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="121" priority="131" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="114" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="120" priority="132" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="107" priority="103" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="119" priority="121" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="104" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="118" priority="122" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="105" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="117" priority="123" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="104" priority="106" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="116" priority="124" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="107" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="115" priority="125" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="108" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="114" priority="126" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="101" priority="97" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="113" priority="115" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="98" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="112" priority="116" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="99" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="111" priority="117" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="98" priority="100" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="110" priority="118" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="109" priority="119" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="102" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="108" priority="120" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="95" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="112" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="113" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="114" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="92" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="109" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="110" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="111" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="89" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="106" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="107" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="108" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="86" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="104" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="105" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="83" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="100" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="101" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="102" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="80" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="98" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="99" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="containsText" dxfId="77" priority="73" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="89" priority="91" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="74" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="75" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="87" priority="93" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="containsText" dxfId="74" priority="76" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="86" priority="94" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="85" priority="95" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="78" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="84" priority="96" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="71" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="89" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="90" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="68" priority="64" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="80" priority="82" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="77" priority="85" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="76" priority="86" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="75" priority="87" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="79" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="80" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="81" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="59" priority="55" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="71" priority="73" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="56" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="69" priority="75" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="56" priority="58" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="68" priority="76" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="67" priority="77" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="60" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="66" priority="78" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="71" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="72" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D14:D20">
+    <cfRule type="containsText" dxfId="62" priority="64" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="60" priority="66" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="47" priority="49" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D14:D20">
+    <cfRule type="containsText" dxfId="59" priority="67" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="58" priority="68" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="57" priority="69" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="62" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E18">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D18">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D18">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="18" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C18" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C20">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E18" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3473,7 +3624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3568,7 +3719,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
excel for task watchlist
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
   <si>
     <t>Module_Name</t>
   </si>
@@ -191,6 +191,30 @@
   </si>
   <si>
     <t>ToggleTc010_VerifyTheRetainAndDefaultSelectionOfToggleButton</t>
+  </si>
+  <si>
+    <t>TWtc004_AddWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc005_AddUnderEvalContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc006_AddWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc007_AddUnderEvalContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc008_AddMultipleWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc009_AddMultipleWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc010_RemoveContactFromWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc011_RemoveContactFromWatchlistContactAndVerifyImpact</t>
   </si>
 </sst>
 </file>
@@ -422,7 +446,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="178">
+  <dxfs count="169">
     <dxf>
       <font>
         <b/>
@@ -496,6 +520,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -568,6 +619,141 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -604,6 +790,42 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -631,6 +853,78 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -730,6 +1024,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -856,6 +1177,114 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -928,6 +1357,366 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -1252,6 +2041,61 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9D18E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9D18E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1419,952 +2263,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFABAB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA9D18E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFABAB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA9D18E"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2760,22 +2658,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="177" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="176" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="175" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="174" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2792,10 +2690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D20"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,12 +2798,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
+      <c r="A7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
@@ -2918,11 +2814,9 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2933,13 +2827,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2950,13 +2842,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
@@ -2967,13 +2857,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B11" s="8"/>
       <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
@@ -2984,13 +2872,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
@@ -3001,13 +2887,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
@@ -3018,15 +2902,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -3035,9 +2917,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>49</v>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -3052,9 +2934,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
@@ -3071,7 +2953,7 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B17" s="8">
         <v>1</v>
@@ -3087,11 +2969,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
@@ -3103,10 +2987,12 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
@@ -3118,10 +3004,12 @@
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D20" t="s">
@@ -3131,491 +3019,687 @@
         <v>10</v>
       </c>
     </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="146" priority="205" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="206" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="207" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="containsText" dxfId="143" priority="208" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="142" priority="209" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="141" priority="210" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="containsText" dxfId="140" priority="211" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="212" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="138" priority="213" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="137" priority="196" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="197" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="198" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="containsText" dxfId="134" priority="199" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="200" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="201" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="containsText" dxfId="131" priority="202" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="203" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="204" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="cellIs" dxfId="128" priority="187" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="188" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="189" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="containsText" dxfId="125" priority="190" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="191" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="192" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="containsText" dxfId="122" priority="193" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="194" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="195" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="119" priority="178" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="179" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="180" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="containsText" dxfId="116" priority="172" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="173" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="174" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="containsText" dxfId="113" priority="175" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="176" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="177" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="110" priority="157" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="158" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="159" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="107" priority="160" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="161" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="162" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="104" priority="151" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="152" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="153" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="101" priority="154" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="155" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="156" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="containsText" dxfId="98" priority="145" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="146" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="147" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="containsText" dxfId="95" priority="148" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="149" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="150" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="92" priority="139" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="140" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="141" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="89" priority="142" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="143" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="144" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="86" priority="133" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="134" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="135" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="containsText" dxfId="83" priority="136" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="137" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="138" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="80" priority="130" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="131" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="132" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="77" priority="127" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="128" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="129" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="74" priority="124" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="125" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="126" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="71" priority="121" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="122" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="123" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="68" priority="118" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="119" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="120" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="65" priority="115" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="116" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="117" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="containsText" dxfId="62" priority="109" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="110" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="111" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="containsText" dxfId="59" priority="112" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="113" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="114" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="56" priority="106" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="107" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="108" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="containsText" dxfId="53" priority="100" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="101" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="102" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="containsText" dxfId="50" priority="103" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="104" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="105" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="47" priority="97" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="98" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="99" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="containsText" dxfId="44" priority="91" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="92" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="93" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="containsText" dxfId="41" priority="94" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="95" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="96" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="38" priority="88" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="89" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="90" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D28">
+    <cfRule type="containsText" dxfId="35" priority="82" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="83" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="84" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D28">
+    <cfRule type="containsText" dxfId="32" priority="85" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="86" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="87" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="29" priority="79" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="80" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="81" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E28">
+    <cfRule type="cellIs" dxfId="26" priority="43" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="44" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="45" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="35" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:E14">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="173" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="170" priority="190" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="191" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="192" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="167" priority="193" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="194" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="195" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="164" priority="178" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="179" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="180" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="161" priority="181" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D8:D14">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="182" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="183" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="158" priority="184" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D8:D14">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="185" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="186" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="155" priority="169" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="170" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="171" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="152" priority="172" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="173" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="174" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="149" priority="175" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="176" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="177" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="146" priority="160" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="161" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="162" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="143" priority="154" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="155" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="156" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="140" priority="157" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="158" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="159" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="137" priority="139" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="140" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="141" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="134" priority="142" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="143" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="144" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="131" priority="133" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="134" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="135" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="128" priority="136" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="137" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="138" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="125" priority="127" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="128" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="129" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="122" priority="130" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="131" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="132" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="119" priority="121" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="122" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="123" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="116" priority="124" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="125" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="126" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="113" priority="115" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="116" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="117" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="110" priority="118" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="119" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="120" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="107" priority="112" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="113" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="114" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="104" priority="109" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="110" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="111" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="101" priority="106" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="107" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="108" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="104" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="105" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="95" priority="100" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="101" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="102" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="98" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="99" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="containsText" dxfId="89" priority="91" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="93" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="containsText" dxfId="86" priority="94" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="95" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="96" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="89" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="90" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="80" priority="82" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="77" priority="85" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="86" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="87" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="74" priority="79" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="80" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="81" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="71" priority="73" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="75" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="68" priority="76" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="77" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="78" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="71" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="72" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D20">
-    <cfRule type="containsText" dxfId="62" priority="64" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="66" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D20">
-    <cfRule type="containsText" dxfId="59" priority="67" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="68" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="69" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="62" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E20">
-    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="18" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C20">
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C28">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E28">
       <formula1>"High,Low"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added tc012-tc013 for toggle & updated TestCases
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>Module_Name</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>TWtc011_RemoveContactFromWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>ToggleTc011_VerifyToAddNewToggleButtonWithMaxAndSpecialCharacter</t>
+  </si>
+  <si>
+    <t>ToggleTc012_CreateNewToggleButtonAsADefaultButton</t>
   </si>
 </sst>
 </file>
@@ -448,6 +454,60 @@
   </cellStyles>
   <dxfs count="169">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -520,6 +580,150 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -2065,204 +2269,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFA9D18E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF548235"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDEEBF7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2658,22 +2664,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="149" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="148" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="147" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2690,10 +2696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,11 +3111,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
-        <v>50</v>
+      <c r="A26" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
@@ -3121,10 +3127,10 @@
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
@@ -3135,8 +3141,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>52</v>
+      <c r="A28" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="14" t="s">
@@ -3149,544 +3155,607 @@
         <v>10</v>
       </c>
     </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="146" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="214" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="215" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="216" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="143" priority="208" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="161" priority="217" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="209" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="160" priority="218" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="210" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="159" priority="219" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="140" priority="211" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="158" priority="220" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="212" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="157" priority="221" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="213" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="156" priority="222" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="137" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="205" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="206" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="207" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="134" priority="199" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="152" priority="208" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="200" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="151" priority="209" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="201" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="150" priority="210" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="131" priority="202" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="149" priority="211" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="203" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="148" priority="212" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="204" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="147" priority="213" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="128" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="196" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="197" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="198" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="125" priority="190" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="143" priority="199" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="191" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="142" priority="200" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="192" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="141" priority="201" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="122" priority="193" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="140" priority="202" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="194" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="139" priority="203" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="195" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="138" priority="204" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="119" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="187" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="188" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="189" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="116" priority="172" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="134" priority="181" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="173" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="133" priority="182" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="174" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="132" priority="183" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="113" priority="175" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="131" priority="184" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="176" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="130" priority="185" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="177" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="129" priority="186" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="110" priority="157" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="128" priority="166" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="158" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="127" priority="167" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="159" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="126" priority="168" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="107" priority="160" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="125" priority="169" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="161" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="124" priority="170" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="162" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="123" priority="171" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="104" priority="151" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="122" priority="160" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="152" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="121" priority="161" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="153" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="120" priority="162" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="101" priority="154" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="119" priority="163" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="155" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="118" priority="164" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="156" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="117" priority="165" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="98" priority="145" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="116" priority="154" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="146" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="115" priority="155" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="147" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="114" priority="156" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="95" priority="148" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="113" priority="157" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="149" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="112" priority="158" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="150" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="111" priority="159" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="92" priority="139" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="110" priority="148" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="140" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="109" priority="149" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="141" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="108" priority="150" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="89" priority="142" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="107" priority="151" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="143" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="106" priority="152" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="144" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="105" priority="153" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="86" priority="133" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="104" priority="142" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="134" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="103" priority="143" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="135" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="102" priority="144" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="83" priority="136" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="101" priority="145" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="137" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="100" priority="146" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="138" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="99" priority="147" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="80" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="139" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="140" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="141" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="77" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="136" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="137" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="138" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="74" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="133" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="134" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="135" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="71" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="130" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="131" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="132" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="68" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="127" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="128" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="129" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="65" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="124" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="125" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="126" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="containsText" dxfId="62" priority="109" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="80" priority="118" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="110" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="79" priority="119" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="111" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="78" priority="120" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="containsText" dxfId="59" priority="112" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="77" priority="121" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="113" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="76" priority="122" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="114" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="75" priority="123" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="56" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="115" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="116" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="117" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="53" priority="100" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="71" priority="109" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="101" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="70" priority="110" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="102" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="69" priority="111" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="50" priority="103" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="68" priority="112" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="104" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="67" priority="113" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="105" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="66" priority="114" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="47" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="106" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="107" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="108" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="44" priority="91" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="62" priority="100" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="92" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="61" priority="101" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="93" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="60" priority="102" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="41" priority="94" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="59" priority="103" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="95" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="58" priority="104" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="96" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="57" priority="105" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="38" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="97" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="98" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="99" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D28">
-    <cfRule type="containsText" dxfId="35" priority="82" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D22:D25 D28:D30">
+    <cfRule type="containsText" dxfId="53" priority="91" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="83" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="52" priority="92" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="84" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="51" priority="93" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D28">
-    <cfRule type="containsText" dxfId="32" priority="85" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D22:D25 D28:D30">
+    <cfRule type="containsText" dxfId="50" priority="94" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="86" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="49" priority="95" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="87" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="48" priority="96" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="29" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="88" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="89" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="90" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E28">
-    <cfRule type="cellIs" dxfId="26" priority="43" operator="equal">
+  <conditionalFormatting sqref="E28:E30">
+    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E14">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="31" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="30" priority="24" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D14">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D14">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D27">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D27">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Skip:">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",D26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",D26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E27">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -3694,11 +3763,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C28">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C30">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E30">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
updated excel task watchlist
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BC41F9-EFE5-48EE-B1CD-B6A2600E44D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Modules" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="10" r:id="rId2"/>
-    <sheet name="Users" sheetId="3" r:id="rId3"/>
+    <sheet name="Modules" r:id="rId1" sheetId="1"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="10"/>
+    <sheet name="Users" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="85">
   <si>
     <t>Module_Name</t>
   </si>
@@ -246,12 +245,49 @@
   </si>
   <si>
     <t>FSTc009_changeTheFieldPositionAndCheckImpact</t>
+  </si>
+  <si>
+    <t>TWtc012_AddContactFromWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc013_AddContactFromWatchlistContactAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc014_SetStatusAsWatchlistAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc015_SaveTaskAgainAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc016_CreateNewTaskWithWatchlistAndVerifyImpact</t>
+  </si>
+  <si>
+    <t>TWtc017_AddWatchlistContactInStandardTask</t>
+  </si>
+  <si>
+    <t>TWtc018_EnableContactTransfer</t>
+  </si>
+  <si>
+    <t>TWtc019_TransferContact_Action</t>
+  </si>
+  <si>
+    <t>TWtc019_TransferContact_Impact</t>
+  </si>
+  <si>
+    <t>TWtc020_1_UpdateWatchlistLabels_Action</t>
+  </si>
+  <si>
+    <t>TWtc020_2_UpdateWatchlistLabels_Action</t>
+  </si>
+  <si>
+    <t>TWtc021_DeleteContactAndVerifyImpact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,60 +460,96 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle name="Hyperlink 2" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="223">
+  <dxfs count="229">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -506,6 +578,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2892,7 +2991,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2977,10 +3076,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -3015,7 +3114,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3050,7 +3149,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3144,21 +3243,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -3175,7 +3274,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -3227,29 +3326,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H1:J4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="7" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="1025" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row ht="15.75" r="1" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3257,23 +3356,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row ht="15.75" r="3" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row ht="15.75" r="4" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H4" s="2" t="s">
         <v>30</v>
       </c>
@@ -3283,54 +3382,54 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="222" priority="6" operator="equal">
+    <cfRule dxfId="228" operator="equal" priority="6" type="cellIs">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="221" priority="7" operator="equal">
+    <cfRule dxfId="227" operator="equal" priority="7" type="cellIs">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="220" priority="1" operator="equal">
+    <cfRule dxfId="226" operator="equal" priority="1" type="cellIs">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="219" priority="2" operator="equal">
+    <cfRule dxfId="225" operator="equal" priority="2" type="cellIs">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="I2:I4" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="87.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="18" r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -3347,7 +3446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>36</v>
       </c>
@@ -3362,7 +3461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -3377,7 +3476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -3392,7 +3491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
@@ -3407,7 +3506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
@@ -3422,7 +3521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>52</v>
       </c>
@@ -3437,7 +3536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>53</v>
       </c>
@@ -3452,7 +3551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
@@ -3467,7 +3566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
@@ -3482,7 +3581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>56</v>
       </c>
@@ -3497,7 +3596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>57</v>
       </c>
@@ -3512,7 +3611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
@@ -3527,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>59</v>
       </c>
@@ -3542,13 +3641,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
+    <row ht="15.75" r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
@@ -3559,13 +3656,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B16" s="8"/>
       <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
@@ -3576,13 +3671,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="17" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="8">
-        <v>1</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B17" s="8"/>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -3593,13 +3686,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="18" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="8">
-        <v>1</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B18" s="8"/>
       <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
@@ -3610,13 +3701,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="19" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
@@ -3627,13 +3716,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="20" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B20" s="8"/>
       <c r="C20" s="3" t="s">
         <v>7</v>
       </c>
@@ -3644,13 +3731,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="21" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="8">
-        <v>1</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B21" s="8"/>
       <c r="C21" s="3" t="s">
         <v>7</v>
       </c>
@@ -3661,15 +3746,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="22" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="8">
-        <v>1</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B22" s="8"/>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
@@ -3678,13 +3761,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="23" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="8">
-        <v>1</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B23" s="8"/>
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
@@ -3695,13 +3776,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="24" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="8">
-        <v>1</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B24" s="8"/>
       <c r="C24" s="3" t="s">
         <v>7</v>
       </c>
@@ -3712,13 +3791,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="25" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B25" s="8"/>
       <c r="C25" s="3" t="s">
         <v>7</v>
       </c>
@@ -3729,9 +3806,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="26" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="3" t="s">
@@ -3744,11 +3821,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="8"/>
+    <row ht="15.75" r="27" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
       <c r="C27" s="3" t="s">
         <v>7</v>
       </c>
@@ -3759,12 +3838,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="14" t="s">
+    <row ht="15.75" r="28" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
@@ -3774,12 +3855,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="29" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
@@ -3789,12 +3872,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="30" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
@@ -3804,12 +3889,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="31" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
@@ -3819,12 +3906,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="32" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
@@ -3834,12 +3923,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="33" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D33" t="s">
@@ -3849,13 +3940,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="34" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="14" t="s">
-        <v>7</v>
+        <v>45</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -3864,12 +3957,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="35" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="8">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
@@ -3879,12 +3974,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="36" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="8">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
@@ -3894,857 +3991,1006 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="37" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>9</v>
       </c>
     </row>
+    <row customHeight="1" ht="15" r="38" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="39" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="40" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="41" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="42" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="43" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="44" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="45" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="46" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="47" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="48" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="49" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="218" priority="277" operator="equal">
+  <conditionalFormatting sqref="E28">
+    <cfRule dxfId="215" operator="equal" priority="268" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="278" operator="equal">
+    <cfRule dxfId="214" operator="equal" priority="269" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="279" operator="equal">
+    <cfRule dxfId="213" operator="equal" priority="270" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="215" priority="280" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="281" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="282" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="212" priority="283" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="284" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="285" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="209" priority="268" operator="equal">
+  <conditionalFormatting sqref="D28">
+    <cfRule dxfId="212" operator="containsText" priority="271" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D28)))</formula>
+    </cfRule>
+    <cfRule dxfId="211" operator="containsText" priority="272" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D28)))</formula>
+    </cfRule>
+    <cfRule dxfId="210" operator="containsText" priority="273" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule dxfId="209" operator="containsText" priority="274" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D28)))</formula>
+    </cfRule>
+    <cfRule dxfId="208" operator="containsText" priority="275" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D28)))</formula>
+    </cfRule>
+    <cfRule dxfId="207" operator="containsText" priority="276" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule dxfId="206" operator="equal" priority="259" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="269" operator="equal">
+    <cfRule dxfId="205" operator="equal" priority="260" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="270" operator="equal">
+    <cfRule dxfId="204" operator="equal" priority="261" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="206" priority="271" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="272" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="273" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="203" priority="274" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="275" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="276" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="200" priority="259" operator="equal">
+  <conditionalFormatting sqref="D29">
+    <cfRule dxfId="203" operator="containsText" priority="262" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D29)))</formula>
+    </cfRule>
+    <cfRule dxfId="202" operator="containsText" priority="263" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D29)))</formula>
+    </cfRule>
+    <cfRule dxfId="201" operator="containsText" priority="264" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule dxfId="200" operator="containsText" priority="265" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D29)))</formula>
+    </cfRule>
+    <cfRule dxfId="199" operator="containsText" priority="266" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D29)))</formula>
+    </cfRule>
+    <cfRule dxfId="198" operator="containsText" priority="267" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule dxfId="197" operator="equal" priority="250" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="260" operator="equal">
+    <cfRule dxfId="196" operator="equal" priority="251" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="261" operator="equal">
+    <cfRule dxfId="195" operator="equal" priority="252" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="197" priority="262" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="263" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="264" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="194" priority="265" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="266" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="267" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="191" priority="250" operator="equal">
+  <conditionalFormatting sqref="D30">
+    <cfRule dxfId="194" operator="containsText" priority="244" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D30)))</formula>
+    </cfRule>
+    <cfRule dxfId="193" operator="containsText" priority="245" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D30)))</formula>
+    </cfRule>
+    <cfRule dxfId="192" operator="containsText" priority="246" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule dxfId="191" operator="containsText" priority="247" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D30)))</formula>
+    </cfRule>
+    <cfRule dxfId="190" operator="containsText" priority="248" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D30)))</formula>
+    </cfRule>
+    <cfRule dxfId="189" operator="containsText" priority="249" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule dxfId="188" operator="containsText" priority="229" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
+    </cfRule>
+    <cfRule dxfId="187" operator="containsText" priority="230" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
+    </cfRule>
+    <cfRule dxfId="186" operator="containsText" priority="231" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule dxfId="185" operator="containsText" priority="232" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
+    </cfRule>
+    <cfRule dxfId="184" operator="containsText" priority="233" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
+    </cfRule>
+    <cfRule dxfId="183" operator="containsText" priority="234" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule dxfId="182" operator="containsText" priority="223" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
+    </cfRule>
+    <cfRule dxfId="181" operator="containsText" priority="224" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
+    </cfRule>
+    <cfRule dxfId="180" operator="containsText" priority="225" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule dxfId="179" operator="containsText" priority="226" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
+    </cfRule>
+    <cfRule dxfId="178" operator="containsText" priority="227" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
+    </cfRule>
+    <cfRule dxfId="177" operator="containsText" priority="228" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule dxfId="176" operator="containsText" priority="217" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+    </cfRule>
+    <cfRule dxfId="175" operator="containsText" priority="218" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+    </cfRule>
+    <cfRule dxfId="174" operator="containsText" priority="219" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule dxfId="173" operator="containsText" priority="220" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
+    </cfRule>
+    <cfRule dxfId="172" operator="containsText" priority="221" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
+    </cfRule>
+    <cfRule dxfId="171" operator="containsText" priority="222" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule dxfId="170" operator="containsText" priority="211" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
+    </cfRule>
+    <cfRule dxfId="169" operator="containsText" priority="212" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
+    </cfRule>
+    <cfRule dxfId="168" operator="containsText" priority="213" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule dxfId="167" operator="containsText" priority="214" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
+    </cfRule>
+    <cfRule dxfId="166" operator="containsText" priority="215" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
+    </cfRule>
+    <cfRule dxfId="165" operator="containsText" priority="216" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule dxfId="164" operator="containsText" priority="205" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
+    </cfRule>
+    <cfRule dxfId="163" operator="containsText" priority="206" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
+    </cfRule>
+    <cfRule dxfId="162" operator="containsText" priority="207" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule dxfId="161" operator="containsText" priority="208" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
+    </cfRule>
+    <cfRule dxfId="160" operator="containsText" priority="209" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
+    </cfRule>
+    <cfRule dxfId="159" operator="containsText" priority="210" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule dxfId="158" operator="equal" priority="202" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="251" operator="equal">
+    <cfRule dxfId="157" operator="equal" priority="203" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="252" operator="equal">
+    <cfRule dxfId="156" operator="equal" priority="204" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="188" priority="244" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="245" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="246" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="185" priority="247" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="248" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="249" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="182" priority="229" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="230" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="231" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="179" priority="232" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="233" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="234" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="176" priority="223" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="224" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="225" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="173" priority="226" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="227" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="228" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="170" priority="217" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="218" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="219" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="167" priority="220" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="221" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="222" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="164" priority="211" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="212" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="213" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="161" priority="214" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="215" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="216" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="158" priority="205" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="206" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="207" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="155" priority="208" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="209" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="210" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="152" priority="202" operator="equal">
+  <conditionalFormatting sqref="E3">
+    <cfRule dxfId="155" operator="equal" priority="199" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="203" operator="equal">
+    <cfRule dxfId="154" operator="equal" priority="200" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="204" operator="equal">
+    <cfRule dxfId="153" operator="equal" priority="201" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="149" priority="199" operator="equal">
+  <conditionalFormatting sqref="E4">
+    <cfRule dxfId="152" operator="equal" priority="196" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="200" operator="equal">
+    <cfRule dxfId="151" operator="equal" priority="197" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="201" operator="equal">
+    <cfRule dxfId="150" operator="equal" priority="198" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="146" priority="196" operator="equal">
+  <conditionalFormatting sqref="E5">
+    <cfRule dxfId="149" operator="equal" priority="193" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="197" operator="equal">
+    <cfRule dxfId="148" operator="equal" priority="194" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="198" operator="equal">
+    <cfRule dxfId="147" operator="equal" priority="195" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="143" priority="193" operator="equal">
+  <conditionalFormatting sqref="E6">
+    <cfRule dxfId="146" operator="equal" priority="190" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="194" operator="equal">
+    <cfRule dxfId="145" operator="equal" priority="191" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="195" operator="equal">
+    <cfRule dxfId="144" operator="equal" priority="192" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="140" priority="190" operator="equal">
+  <conditionalFormatting sqref="E31">
+    <cfRule dxfId="143" operator="equal" priority="187" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="191" operator="equal">
+    <cfRule dxfId="142" operator="equal" priority="188" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="192" operator="equal">
+    <cfRule dxfId="141" operator="equal" priority="189" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="137" priority="187" operator="equal">
+  <conditionalFormatting sqref="D31">
+    <cfRule dxfId="140" operator="containsText" priority="181" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D31)))</formula>
+    </cfRule>
+    <cfRule dxfId="139" operator="containsText" priority="182" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D31)))</formula>
+    </cfRule>
+    <cfRule dxfId="138" operator="containsText" priority="183" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule dxfId="137" operator="containsText" priority="184" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D31)))</formula>
+    </cfRule>
+    <cfRule dxfId="136" operator="containsText" priority="185" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D31)))</formula>
+    </cfRule>
+    <cfRule dxfId="135" operator="containsText" priority="186" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule dxfId="134" operator="equal" priority="178" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="188" operator="equal">
+    <cfRule dxfId="133" operator="equal" priority="179" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="189" operator="equal">
+    <cfRule dxfId="132" operator="equal" priority="180" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="containsText" dxfId="134" priority="181" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="182" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="183" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="containsText" dxfId="131" priority="184" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="185" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="186" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="128" priority="178" operator="equal">
+  <conditionalFormatting sqref="D32">
+    <cfRule dxfId="131" operator="containsText" priority="172" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D32)))</formula>
+    </cfRule>
+    <cfRule dxfId="130" operator="containsText" priority="173" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D32)))</formula>
+    </cfRule>
+    <cfRule dxfId="129" operator="containsText" priority="174" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule dxfId="128" operator="containsText" priority="175" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D32)))</formula>
+    </cfRule>
+    <cfRule dxfId="127" operator="containsText" priority="176" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D32)))</formula>
+    </cfRule>
+    <cfRule dxfId="126" operator="containsText" priority="177" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule dxfId="125" operator="equal" priority="169" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="179" operator="equal">
+    <cfRule dxfId="124" operator="equal" priority="170" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="180" operator="equal">
+    <cfRule dxfId="123" operator="equal" priority="171" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="125" priority="172" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="173" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="174" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="122" priority="175" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="176" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="177" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="119" priority="169" operator="equal">
+  <conditionalFormatting sqref="D33">
+    <cfRule dxfId="122" operator="containsText" priority="163" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D33)))</formula>
+    </cfRule>
+    <cfRule dxfId="121" operator="containsText" priority="164" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D33)))</formula>
+    </cfRule>
+    <cfRule dxfId="120" operator="containsText" priority="165" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule dxfId="119" operator="containsText" priority="166" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D33)))</formula>
+    </cfRule>
+    <cfRule dxfId="118" operator="containsText" priority="167" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D33)))</formula>
+    </cfRule>
+    <cfRule dxfId="117" operator="containsText" priority="168" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule dxfId="116" operator="equal" priority="160" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="170" operator="equal">
+    <cfRule dxfId="115" operator="equal" priority="161" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="171" operator="equal">
+    <cfRule dxfId="114" operator="equal" priority="162" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="116" priority="163" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="164" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="165" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="113" priority="166" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="167" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="168" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="110" priority="160" operator="equal">
+  <conditionalFormatting sqref="D34:D37 D40:D42">
+    <cfRule dxfId="113" operator="containsText" priority="154" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="112" operator="containsText" priority="155" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="111" operator="containsText" priority="156" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:D37 D40:D42">
+    <cfRule dxfId="110" operator="containsText" priority="157" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="109" operator="containsText" priority="158" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="108" operator="containsText" priority="159" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule dxfId="107" operator="equal" priority="151" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="161" operator="equal">
+    <cfRule dxfId="106" operator="equal" priority="152" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="162" operator="equal">
+    <cfRule dxfId="105" operator="equal" priority="153" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D25 D28:D30">
-    <cfRule type="containsText" dxfId="107" priority="154" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="155" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="156" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D25 D28:D30">
-    <cfRule type="containsText" dxfId="104" priority="157" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="158" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="159" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="101" priority="151" operator="equal">
+  <conditionalFormatting sqref="E40:E42">
+    <cfRule dxfId="104" operator="equal" priority="115" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="152" operator="equal">
+    <cfRule dxfId="103" operator="equal" priority="116" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="153" operator="equal">
+    <cfRule dxfId="102" operator="equal" priority="117" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E30">
-    <cfRule type="cellIs" dxfId="98" priority="115" operator="equal">
+  <conditionalFormatting sqref="E36">
+    <cfRule dxfId="101" operator="equal" priority="106" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="116" operator="equal">
+    <cfRule dxfId="100" operator="equal" priority="107" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="117" operator="equal">
+    <cfRule dxfId="99" operator="equal" priority="108" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="95" priority="106" operator="equal">
+  <conditionalFormatting sqref="E37">
+    <cfRule dxfId="98" operator="equal" priority="97" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="107" operator="equal">
+    <cfRule dxfId="97" operator="equal" priority="98" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="108" operator="equal">
+    <cfRule dxfId="96" operator="equal" priority="99" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
+  <conditionalFormatting sqref="E8:E27">
+    <cfRule dxfId="95" operator="equal" priority="73" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="98" operator="equal">
+    <cfRule dxfId="94" operator="equal" priority="74" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="99" operator="equal">
+    <cfRule dxfId="93" operator="equal" priority="75" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E14">
-    <cfRule type="cellIs" dxfId="89" priority="73" operator="equal">
+  <conditionalFormatting sqref="D7">
+    <cfRule dxfId="92" operator="containsText" priority="85" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
+    </cfRule>
+    <cfRule dxfId="91" operator="containsText" priority="86" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
+    </cfRule>
+    <cfRule dxfId="90" operator="containsText" priority="87" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule dxfId="89" operator="containsText" priority="88" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
+    </cfRule>
+    <cfRule dxfId="88" operator="containsText" priority="89" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
+    </cfRule>
+    <cfRule dxfId="87" operator="containsText" priority="90" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule dxfId="86" operator="equal" priority="82" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="74" operator="equal">
+    <cfRule dxfId="85" operator="equal" priority="83" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="75" operator="equal">
+    <cfRule dxfId="84" operator="equal" priority="84" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="83" priority="88" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="89" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="90" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
+  <conditionalFormatting sqref="D8:D27">
+    <cfRule dxfId="83" operator="containsText" priority="76" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="82" operator="containsText" priority="77" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="81" operator="containsText" priority="78" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D27">
+    <cfRule dxfId="80" operator="containsText" priority="79" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="79" operator="containsText" priority="80" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="78" operator="containsText" priority="81" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D39">
+    <cfRule dxfId="77" operator="containsText" priority="67" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="76" operator="containsText" priority="68" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="75" operator="containsText" priority="69" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D39">
+    <cfRule dxfId="74" operator="containsText" priority="70" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="73" operator="containsText" priority="71" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="72" operator="containsText" priority="72" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38:E39">
+    <cfRule dxfId="71" operator="equal" priority="64" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="83" operator="equal">
+    <cfRule dxfId="70" operator="equal" priority="65" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="84" operator="equal">
+    <cfRule dxfId="69" operator="equal" priority="66" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D14">
-    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D14">
-    <cfRule type="containsText" dxfId="74" priority="79" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="81" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D27">
-    <cfRule type="containsText" dxfId="71" priority="67" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D27">
-    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
-    <cfRule type="cellIs" dxfId="65" priority="64" operator="equal">
+  <conditionalFormatting sqref="D43">
+    <cfRule dxfId="68" operator="containsText" priority="58" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D43)))</formula>
+    </cfRule>
+    <cfRule dxfId="67" operator="containsText" priority="59" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D43)))</formula>
+    </cfRule>
+    <cfRule dxfId="66" operator="containsText" priority="60" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule dxfId="65" operator="containsText" priority="61" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D43)))</formula>
+    </cfRule>
+    <cfRule dxfId="64" operator="containsText" priority="62" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D43)))</formula>
+    </cfRule>
+    <cfRule dxfId="63" operator="containsText" priority="63" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule dxfId="62" operator="equal" priority="55" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
+    <cfRule dxfId="61" operator="equal" priority="56" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="66" operator="equal">
+    <cfRule dxfId="60" operator="equal" priority="57" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="containsText" dxfId="62" priority="58" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="containsText" dxfId="59" priority="61" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="63" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
+  <conditionalFormatting sqref="D44">
+    <cfRule dxfId="59" operator="containsText" priority="49" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D44)))</formula>
+    </cfRule>
+    <cfRule dxfId="58" operator="containsText" priority="50" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D44)))</formula>
+    </cfRule>
+    <cfRule dxfId="57" operator="containsText" priority="51" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule dxfId="56" operator="containsText" priority="52" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D44)))</formula>
+    </cfRule>
+    <cfRule dxfId="55" operator="containsText" priority="53" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D44)))</formula>
+    </cfRule>
+    <cfRule dxfId="54" operator="containsText" priority="54" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule dxfId="53" operator="equal" priority="46" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
+    <cfRule dxfId="52" operator="equal" priority="47" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+    <cfRule dxfId="51" operator="equal" priority="48" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+  <conditionalFormatting sqref="D45">
+    <cfRule dxfId="50" operator="containsText" priority="40" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D45)))</formula>
+    </cfRule>
+    <cfRule dxfId="49" operator="containsText" priority="41" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D45)))</formula>
+    </cfRule>
+    <cfRule dxfId="48" operator="containsText" priority="42" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule dxfId="47" operator="containsText" priority="43" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D45)))</formula>
+    </cfRule>
+    <cfRule dxfId="46" operator="containsText" priority="44" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D45)))</formula>
+    </cfRule>
+    <cfRule dxfId="45" operator="containsText" priority="45" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule dxfId="44" operator="equal" priority="37" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+    <cfRule dxfId="43" operator="equal" priority="38" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
+    <cfRule dxfId="42" operator="equal" priority="39" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+  <conditionalFormatting sqref="D46">
+    <cfRule dxfId="41" operator="containsText" priority="31" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="40" operator="containsText" priority="32" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="39" operator="containsText" priority="33" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule dxfId="38" operator="containsText" priority="34" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="37" operator="containsText" priority="35" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="36" operator="containsText" priority="36" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule dxfId="35" operator="equal" priority="28" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+    <cfRule dxfId="34" operator="equal" priority="29" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
+    <cfRule dxfId="33" operator="equal" priority="30" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+  <conditionalFormatting sqref="D47">
+    <cfRule dxfId="32" operator="containsText" priority="22" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D47)))</formula>
+    </cfRule>
+    <cfRule dxfId="31" operator="containsText" priority="23" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D47)))</formula>
+    </cfRule>
+    <cfRule dxfId="30" operator="containsText" priority="24" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule dxfId="29" operator="containsText" priority="25" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D47)))</formula>
+    </cfRule>
+    <cfRule dxfId="28" operator="containsText" priority="26" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D47)))</formula>
+    </cfRule>
+    <cfRule dxfId="27" operator="containsText" priority="27" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule dxfId="26" operator="equal" priority="19" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule dxfId="25" operator="equal" priority="20" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+    <cfRule dxfId="24" operator="equal" priority="21" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+  <conditionalFormatting sqref="D48">
+    <cfRule dxfId="23" operator="containsText" priority="13" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D48)))</formula>
+    </cfRule>
+    <cfRule dxfId="22" operator="containsText" priority="14" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D48)))</formula>
+    </cfRule>
+    <cfRule dxfId="21" operator="containsText" priority="15" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule dxfId="20" operator="containsText" priority="16" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D48)))</formula>
+    </cfRule>
+    <cfRule dxfId="19" operator="containsText" priority="17" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D48)))</formula>
+    </cfRule>
+    <cfRule dxfId="18" operator="containsText" priority="18" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule dxfId="17" operator="equal" priority="10" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule dxfId="16" operator="equal" priority="11" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+    <cfRule dxfId="15" operator="equal" priority="12" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+  <conditionalFormatting sqref="D49">
+    <cfRule dxfId="14" operator="containsText" priority="4" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="13" operator="containsText" priority="5" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="12" operator="containsText" priority="6" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule dxfId="11" operator="containsText" priority="7" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="10" operator="containsText" priority="8" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="9" operator="containsText" priority="9" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule dxfId="8" operator="equal" priority="1" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule dxfId="7" operator="equal" priority="2" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule dxfId="6" operator="equal" priority="3" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation showDropDown="1" showErrorMessage="1" showInputMessage="1" sqref="C1">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C37" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C2:C49" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E37" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E49" type="list">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="D3" pane="bottomLeft" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="19" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="1025" width="19" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="6" max="1025" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4827,9 +5073,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="javascript:srcUp(%27%2F0054x000001Z8z4%3Fnoredirect%3D1%26isUserEntityOverride%3D1%26isdtp%3Dp1%27);" xr:uid="{B90EC40D-7451-41E9-8B2E-CC1DDED80C77}"/>
+    <hyperlink display="javascript:srcUp(%27%2F0054x000001Z8z4%3Fnoredirect%3D1%26isUserEntityOverride%3D1%26isdtp%3Dp1%27);" r:id="rId1" ref="E3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Module 3 TC004 & TC005 Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406606CD-8257-4FDC-BE48-6AC6385058D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Modules" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="10" r:id="rId2"/>
-    <sheet name="Users" sheetId="3" r:id="rId3"/>
+    <sheet name="Modules" r:id="rId1" sheetId="1"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="10"/>
+    <sheet name="Users" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="108">
   <si>
     <t>Module_Name</t>
   </si>
@@ -278,9 +277,6 @@
     <t>FSTc015_createFieldsForPackageObject</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>FSTc014_CreatedataForPackageObject</t>
   </si>
   <si>
@@ -336,12 +332,38 @@
   </si>
   <si>
     <t>FSTc019_addProfileImageFieldOnLayOut</t>
+  </si>
+  <si>
+    <t>Module3</t>
+  </si>
+  <si>
+    <t>Module3Tc004_OpentheNavigationMenuAndVerifyTheMenuItems</t>
+  </si>
+  <si>
+    <t>Fail: timeout: Timed out receiving message from renderer: 10.000
+  (Session info: chrome=88.0.4324.104)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:25:53'
+System info: host: 'DESKTOP-K4MTBVJ', ip: '192.168.0.104', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_141'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 88.0.4324.104, chrome: {chromedriverVersion: 87.0.4280.20 (c99e81631faa0..., userDataDir: C:\Users\sibaram\AppData\Lo...}, goog:chromeOptions: {debuggerAddress: localhost:63888}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:virtualAuthenticators: true}
+Session ID: 1b41886e1662c3724adefb794bc06a38</t>
+  </si>
+  <si>
+    <t>Module3Tc005_VerifyTheURLNavigationFromNavigationMenu</t>
+  </si>
+  <si>
+    <t>Fail: 7</t>
+  </si>
+  <si>
+    <t>Fail: The following asserts failed:
+	Url Not Verified for : Navatar Setup Actual : https://pe4604.lightning.force.com/lightning/page/home	 Expected : /lightning/n/navmnaI__Navatar_Setup (Module3.java:434)	Screenshot Name: Module3Tc005_VerifyTheURLNavigationFromNavigationMenu2021_02_05_06_50_23.png	 did not expect to find [true] but found [false]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -514,63 +536,207 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle name="Hyperlink 2" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="313">
+  <dxfs count="342">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -599,6 +765,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -698,6 +891,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -896,6 +1116,78 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF548235"/>
@@ -950,6 +1242,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3974,8 +4293,22 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9D18E"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -4060,10 +4393,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -4098,7 +4431,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4133,7 +4466,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4227,21 +4560,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -4258,7 +4591,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -4310,29 +4643,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H1:J5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="7" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="1025" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row ht="15.75" r="1" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4340,15 +4673,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row ht="15.75" r="3" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
@@ -4356,7 +4689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="4" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H4" s="2" t="s">
         <v>30</v>
       </c>
@@ -4364,56 +4697,74 @@
         <v>7</v>
       </c>
     </row>
+    <row ht="15.75" r="5" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="312" priority="6" operator="equal">
+    <cfRule dxfId="341" operator="equal" priority="8" type="cellIs">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="311" priority="7" operator="equal">
+    <cfRule dxfId="340" operator="equal" priority="9" type="cellIs">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="310" priority="1" operator="equal">
+    <cfRule dxfId="339" operator="equal" priority="3" type="cellIs">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="309" priority="2" operator="equal">
+    <cfRule dxfId="338" operator="equal" priority="4" type="cellIs">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule dxfId="337" operator="equal" priority="1" type="cellIs">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule dxfId="336" operator="equal" priority="2" type="cellIs">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="I2:I5" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="87.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="18" r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -4430,7 +4781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>36</v>
       </c>
@@ -4445,7 +4796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -4460,7 +4811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
@@ -4475,7 +4826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
@@ -4490,7 +4841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
@@ -4505,7 +4856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>48</v>
       </c>
@@ -4520,7 +4871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -4535,7 +4886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>50</v>
       </c>
@@ -4550,7 +4901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
@@ -4565,7 +4916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
@@ -4580,7 +4931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>53</v>
       </c>
@@ -4595,7 +4946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>54</v>
       </c>
@@ -4610,7 +4961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>55</v>
       </c>
@@ -4625,7 +4976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>66</v>
       </c>
@@ -4640,7 +4991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>67</v>
       </c>
@@ -4655,7 +5006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="17" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>68</v>
       </c>
@@ -4670,7 +5021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="18" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>69</v>
       </c>
@@ -4685,7 +5036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="19" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>70</v>
       </c>
@@ -4700,7 +5051,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="20" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>71</v>
       </c>
@@ -4715,7 +5066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="21" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>72</v>
       </c>
@@ -4730,7 +5081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="22" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>73</v>
       </c>
@@ -4745,7 +5096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="23" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>74</v>
       </c>
@@ -4760,7 +5111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="24" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>75</v>
       </c>
@@ -4775,7 +5126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="25" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>76</v>
       </c>
@@ -4790,7 +5141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="26" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>77</v>
       </c>
@@ -4805,9 +5156,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="27" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="3" t="s">
@@ -4820,9 +5171,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="28" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="3" t="s">
@@ -4835,9 +5186,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="29" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="3" t="s">
@@ -4850,9 +5201,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="30" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="3" t="s">
@@ -4865,9 +5216,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="31" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="3" t="s">
@@ -4880,9 +5231,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="32" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="3" t="s">
@@ -4895,9 +5246,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="33" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="3" t="s">
@@ -4910,7 +5261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="34" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>31</v>
       </c>
@@ -4927,7 +5278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="35" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
@@ -4944,7 +5295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="36" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
@@ -4961,7 +5312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="37" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>34</v>
       </c>
@@ -4978,9 +5329,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="38" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="8">
         <v>1</v>
@@ -4995,7 +5346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="39" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>43</v>
       </c>
@@ -5012,7 +5363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="40" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>42</v>
       </c>
@@ -5029,7 +5380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="41" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>44</v>
       </c>
@@ -5046,9 +5397,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="42" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="8">
         <v>1</v>
@@ -5063,9 +5414,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="43" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="8">
         <v>1</v>
@@ -5080,9 +5431,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="44" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" s="8">
         <v>1</v>
@@ -5097,11 +5448,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="45" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B45" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="B45" s="8">
+        <v>1</v>
+      </c>
       <c r="C45" s="3" t="s">
         <v>7</v>
       </c>
@@ -5112,12 +5465,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="46" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>7</v>
@@ -5129,12 +5482,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="47" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>7</v>
@@ -5146,12 +5499,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="14" t="s">
+    <row customHeight="1" ht="15" r="48" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="8">
+        <v>4</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D48" t="s">
@@ -5161,24 +5516,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="49" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="14" t="s">
-        <v>7</v>
+        <v>105</v>
+      </c>
+      <c r="B49" s="8">
+        <v>4</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>47</v>
+    <row customHeight="1" ht="15" r="50" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="14" t="s">
@@ -5191,9 +5548,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="51" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="14" t="s">
@@ -5206,9 +5563,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="52" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="14" t="s">
@@ -5221,9 +5578,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="53" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="14" t="s">
@@ -5236,9 +5593,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="54" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="14" t="s">
@@ -5251,9 +5608,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="55" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="14" t="s">
@@ -5266,9 +5623,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="56" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="14" t="s">
@@ -5281,9 +5638,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="57" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="14" t="s">
@@ -5296,9 +5653,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="58" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="14" t="s">
@@ -5311,9 +5668,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="59" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="14" t="s">
@@ -5326,9 +5683,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="60" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="14" t="s">
@@ -5341,9 +5698,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="61" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="14" t="s">
@@ -5356,9 +5713,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="16" t="s">
-        <v>84</v>
+    <row customHeight="1" ht="15" r="62" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="14" t="s">
@@ -5371,9 +5728,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>82</v>
+    <row customHeight="1" ht="15" r="63" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="14" t="s">
@@ -5386,9 +5743,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>92</v>
+    <row customHeight="1" ht="15" r="64" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="14" t="s">
@@ -5401,1217 +5758,1313 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="65" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="66" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="67" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D67" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>9</v>
       </c>
     </row>
+    <row customHeight="1" ht="15" r="68" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="69" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E6 E45">
-    <cfRule type="cellIs" dxfId="308" priority="373" operator="equal">
+    <cfRule dxfId="335" operator="equal" priority="397" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="307" priority="374" operator="equal">
+    <cfRule dxfId="334" operator="equal" priority="398" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="306" priority="375" operator="equal">
+    <cfRule dxfId="333" operator="equal" priority="399" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 D44:D45">
-    <cfRule type="containsText" dxfId="305" priority="412" operator="containsText" text="Skip:">
+    <cfRule dxfId="332" operator="containsText" priority="436" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="304" priority="413" operator="containsText" text="Fail">
+    <cfRule dxfId="331" operator="containsText" priority="437" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="303" priority="414" operator="containsText" text="Pass">
+    <cfRule dxfId="330" operator="containsText" priority="438" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="302" priority="415" operator="containsText" text="Skip:">
+    <cfRule dxfId="329" operator="containsText" priority="439" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="416" operator="containsText" text="Fail">
+    <cfRule dxfId="328" operator="containsText" priority="440" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="300" priority="417" operator="containsText" text="Pass">
+    <cfRule dxfId="327" operator="containsText" priority="441" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="299" priority="406" operator="containsText" text="Skip:">
+    <cfRule dxfId="326" operator="containsText" priority="430" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="298" priority="407" operator="containsText" text="Fail">
+    <cfRule dxfId="325" operator="containsText" priority="431" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="297" priority="408" operator="containsText" text="Pass">
+    <cfRule dxfId="324" operator="containsText" priority="432" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="296" priority="409" operator="containsText" text="Skip:">
+    <cfRule dxfId="323" operator="containsText" priority="433" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="295" priority="410" operator="containsText" text="Fail">
+    <cfRule dxfId="322" operator="containsText" priority="434" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="294" priority="411" operator="containsText" text="Pass">
+    <cfRule dxfId="321" operator="containsText" priority="435" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="293" priority="400" operator="containsText" text="Skip:">
+    <cfRule dxfId="320" operator="containsText" priority="424" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="292" priority="401" operator="containsText" text="Fail">
+    <cfRule dxfId="319" operator="containsText" priority="425" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="291" priority="402" operator="containsText" text="Pass">
+    <cfRule dxfId="318" operator="containsText" priority="426" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="290" priority="403" operator="containsText" text="Skip:">
+    <cfRule dxfId="317" operator="containsText" priority="427" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="404" operator="containsText" text="Fail">
+    <cfRule dxfId="316" operator="containsText" priority="428" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="288" priority="405" operator="containsText" text="Pass">
+    <cfRule dxfId="315" operator="containsText" priority="429" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="287" priority="394" operator="containsText" text="Skip:">
+    <cfRule dxfId="314" operator="containsText" priority="418" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="395" operator="containsText" text="Fail">
+    <cfRule dxfId="313" operator="containsText" priority="419" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="396" operator="containsText" text="Pass">
+    <cfRule dxfId="312" operator="containsText" priority="420" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="284" priority="397" operator="containsText" text="Skip:">
+    <cfRule dxfId="311" operator="containsText" priority="421" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="283" priority="398" operator="containsText" text="Fail">
+    <cfRule dxfId="310" operator="containsText" priority="422" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="399" operator="containsText" text="Pass">
+    <cfRule dxfId="309" operator="containsText" priority="423" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="281" priority="388" operator="containsText" text="Skip:">
+    <cfRule dxfId="308" operator="containsText" priority="412" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="280" priority="389" operator="containsText" text="Fail">
+    <cfRule dxfId="307" operator="containsText" priority="413" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="390" operator="containsText" text="Pass">
+    <cfRule dxfId="306" operator="containsText" priority="414" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="278" priority="391" operator="containsText" text="Skip:">
+    <cfRule dxfId="305" operator="containsText" priority="415" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="392" operator="containsText" text="Fail">
+    <cfRule dxfId="304" operator="containsText" priority="416" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="276" priority="393" operator="containsText" text="Pass">
+    <cfRule dxfId="303" operator="containsText" priority="417" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="275" priority="385" operator="equal">
+    <cfRule dxfId="302" operator="equal" priority="409" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="274" priority="386" operator="equal">
+    <cfRule dxfId="301" operator="equal" priority="410" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="273" priority="387" operator="equal">
+    <cfRule dxfId="300" operator="equal" priority="411" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="272" priority="382" operator="equal">
+    <cfRule dxfId="299" operator="equal" priority="406" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="271" priority="383" operator="equal">
+    <cfRule dxfId="298" operator="equal" priority="407" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="270" priority="384" operator="equal">
+    <cfRule dxfId="297" operator="equal" priority="408" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="269" priority="379" operator="equal">
+    <cfRule dxfId="296" operator="equal" priority="403" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="268" priority="380" operator="equal">
+    <cfRule dxfId="295" operator="equal" priority="404" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="267" priority="381" operator="equal">
+    <cfRule dxfId="294" operator="equal" priority="405" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="266" priority="376" operator="equal">
+    <cfRule dxfId="293" operator="equal" priority="400" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="265" priority="377" operator="equal">
+    <cfRule dxfId="292" operator="equal" priority="401" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="264" priority="378" operator="equal">
+    <cfRule dxfId="291" operator="equal" priority="402" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="263" priority="268" operator="containsText" text="Skip:">
+    <cfRule dxfId="290" operator="containsText" priority="292" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="269" operator="containsText" text="Fail">
+    <cfRule dxfId="289" operator="containsText" priority="293" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="270" operator="containsText" text="Pass">
+    <cfRule dxfId="288" operator="containsText" priority="294" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="260" priority="271" operator="containsText" text="Skip:">
+    <cfRule dxfId="287" operator="containsText" priority="295" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="272" operator="containsText" text="Fail">
+    <cfRule dxfId="286" operator="containsText" priority="296" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="273" operator="containsText" text="Pass">
+    <cfRule dxfId="285" operator="containsText" priority="297" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="257" priority="265" operator="equal">
+    <cfRule dxfId="284" operator="equal" priority="289" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="256" priority="266" operator="equal">
+    <cfRule dxfId="283" operator="equal" priority="290" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="267" operator="equal">
+    <cfRule dxfId="282" operator="equal" priority="291" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D50">
-    <cfRule type="containsText" dxfId="254" priority="337" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D50:D52">
+    <cfRule dxfId="281" operator="containsText" priority="361" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="280" operator="containsText" priority="362" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="279" operator="containsText" priority="363" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50:D52">
+    <cfRule dxfId="278" operator="containsText" priority="364" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="277" operator="containsText" priority="365" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D50)))</formula>
+    </cfRule>
+    <cfRule dxfId="276" operator="containsText" priority="366" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:E33">
+    <cfRule dxfId="275" operator="equal" priority="280" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="274" operator="equal" priority="281" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="273" operator="equal" priority="282" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:E52">
+    <cfRule dxfId="272" operator="equal" priority="322" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="271" operator="equal" priority="323" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="270" operator="equal" priority="324" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule dxfId="269" operator="equal" priority="235" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="268" operator="equal" priority="236" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="267" operator="equal" priority="237" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D33">
+    <cfRule dxfId="266" operator="containsText" priority="283" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="265" operator="containsText" priority="284" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="264" operator="containsText" priority="285" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D33">
+    <cfRule dxfId="263" operator="containsText" priority="286" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="262" operator="containsText" priority="287" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
+    </cfRule>
+    <cfRule dxfId="261" operator="containsText" priority="288" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule dxfId="260" operator="containsText" priority="265" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="259" operator="containsText" priority="266" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="258" operator="containsText" priority="267" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule dxfId="257" operator="containsText" priority="268" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="256" operator="containsText" priority="269" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
+    </cfRule>
+    <cfRule dxfId="255" operator="containsText" priority="270" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule dxfId="254" operator="equal" priority="262" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="253" operator="equal" priority="263" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="252" operator="equal" priority="264" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule dxfId="251" operator="containsText" priority="256" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="250" operator="containsText" priority="257" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="249" operator="containsText" priority="258" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule dxfId="248" operator="containsText" priority="259" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="247" operator="containsText" priority="260" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
+    </cfRule>
+    <cfRule dxfId="246" operator="containsText" priority="261" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54">
+    <cfRule dxfId="245" operator="equal" priority="253" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="244" operator="equal" priority="254" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="243" operator="equal" priority="255" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule dxfId="242" operator="containsText" priority="247" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="241" operator="containsText" priority="248" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="240" operator="containsText" priority="249" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule dxfId="239" operator="containsText" priority="250" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="238" operator="containsText" priority="251" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
+    </cfRule>
+    <cfRule dxfId="237" operator="containsText" priority="252" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule dxfId="236" operator="equal" priority="244" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="235" operator="equal" priority="245" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="234" operator="equal" priority="246" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule dxfId="233" operator="containsText" priority="238" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="232" operator="containsText" priority="239" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="231" operator="containsText" priority="240" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule dxfId="230" operator="containsText" priority="241" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="229" operator="containsText" priority="242" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
+    </cfRule>
+    <cfRule dxfId="228" operator="containsText" priority="243" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule dxfId="227" operator="containsText" priority="229" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="226" operator="containsText" priority="230" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="225" operator="containsText" priority="231" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule dxfId="224" operator="containsText" priority="232" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="223" operator="containsText" priority="233" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
+    </cfRule>
+    <cfRule dxfId="222" operator="containsText" priority="234" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule dxfId="221" operator="equal" priority="226" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="220" operator="equal" priority="227" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="219" operator="equal" priority="228" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule dxfId="218" operator="containsText" priority="220" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="217" operator="containsText" priority="221" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="216" operator="containsText" priority="222" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule dxfId="215" operator="containsText" priority="223" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="214" operator="containsText" priority="224" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
+    </cfRule>
+    <cfRule dxfId="213" operator="containsText" priority="225" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule dxfId="212" operator="equal" priority="217" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="211" operator="equal" priority="218" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="210" operator="equal" priority="219" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule dxfId="209" operator="containsText" priority="211" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="208" operator="containsText" priority="212" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="207" operator="containsText" priority="213" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule dxfId="206" operator="containsText" priority="214" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="205" operator="containsText" priority="215" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
+    </cfRule>
+    <cfRule dxfId="204" operator="containsText" priority="216" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule dxfId="203" operator="equal" priority="208" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="202" operator="equal" priority="209" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="201" operator="equal" priority="210" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule dxfId="200" operator="containsText" priority="202" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="199" operator="containsText" priority="203" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="198" operator="containsText" priority="204" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule dxfId="197" operator="containsText" priority="205" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="196" operator="containsText" priority="206" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
+    </cfRule>
+    <cfRule dxfId="195" operator="containsText" priority="207" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E60">
+    <cfRule dxfId="194" operator="equal" priority="199" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="193" operator="equal" priority="200" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="192" operator="equal" priority="201" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule dxfId="191" operator="containsText" priority="193" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="190" operator="containsText" priority="194" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="189" operator="containsText" priority="195" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule dxfId="188" operator="containsText" priority="196" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="187" operator="containsText" priority="197" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
+    </cfRule>
+    <cfRule dxfId="186" operator="containsText" priority="198" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61">
+    <cfRule dxfId="185" operator="equal" priority="190" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="184" operator="equal" priority="191" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="183" operator="equal" priority="192" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule dxfId="182" operator="containsText" priority="184" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="181" operator="containsText" priority="185" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="180" operator="containsText" priority="186" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule dxfId="179" operator="containsText" priority="187" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="178" operator="containsText" priority="188" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D62)))</formula>
+    </cfRule>
+    <cfRule dxfId="177" operator="containsText" priority="189" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
+    <cfRule dxfId="176" operator="equal" priority="181" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="175" operator="equal" priority="182" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="174" operator="equal" priority="183" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:D64">
+    <cfRule dxfId="173" operator="containsText" priority="175" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="172" operator="containsText" priority="176" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="171" operator="containsText" priority="177" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:D64">
+    <cfRule dxfId="170" operator="containsText" priority="178" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="169" operator="containsText" priority="179" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
+    </cfRule>
+    <cfRule dxfId="168" operator="containsText" priority="180" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63:E64">
+    <cfRule dxfId="167" operator="equal" priority="172" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="166" operator="equal" priority="173" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="165" operator="equal" priority="174" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule dxfId="164" operator="containsText" priority="166" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="163" operator="containsText" priority="167" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="162" operator="containsText" priority="168" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule dxfId="161" operator="containsText" priority="169" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="160" operator="containsText" priority="170" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
+    </cfRule>
+    <cfRule dxfId="159" operator="containsText" priority="171" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule dxfId="158" operator="equal" priority="163" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="157" operator="equal" priority="164" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="156" operator="equal" priority="165" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule dxfId="155" operator="equal" priority="154" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="154" operator="equal" priority="155" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="153" operator="equal" priority="156" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule dxfId="152" operator="containsText" priority="157" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="151" operator="containsText" priority="158" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="150" operator="containsText" priority="159" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule dxfId="149" operator="containsText" priority="160" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="148" operator="containsText" priority="161" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
+    </cfRule>
+    <cfRule dxfId="147" operator="containsText" priority="162" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule dxfId="146" operator="equal" priority="145" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="145" operator="equal" priority="146" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="144" operator="equal" priority="147" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule dxfId="143" operator="containsText" priority="148" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="142" operator="containsText" priority="149" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="141" operator="containsText" priority="150" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule dxfId="140" operator="containsText" priority="151" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="139" operator="containsText" priority="152" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
+    </cfRule>
+    <cfRule dxfId="138" operator="containsText" priority="153" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule dxfId="137" operator="equal" priority="142" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="136" operator="equal" priority="143" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="135" operator="equal" priority="144" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule dxfId="134" operator="containsText" priority="136" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="133" operator="containsText" priority="137" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="132" operator="containsText" priority="138" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule dxfId="131" operator="containsText" priority="139" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="130" operator="containsText" priority="140" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
+    </cfRule>
+    <cfRule dxfId="129" operator="containsText" priority="141" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule dxfId="128" operator="equal" priority="133" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="127" operator="equal" priority="134" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="126" operator="equal" priority="135" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule dxfId="125" operator="containsText" priority="127" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="124" operator="containsText" priority="128" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="123" operator="containsText" priority="129" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule dxfId="122" operator="containsText" priority="130" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="121" operator="containsText" priority="131" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
+    </cfRule>
+    <cfRule dxfId="120" operator="containsText" priority="132" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule dxfId="119" operator="equal" priority="124" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="118" operator="equal" priority="125" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="117" operator="equal" priority="126" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule dxfId="116" operator="containsText" priority="118" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="115" operator="containsText" priority="119" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="114" operator="containsText" priority="120" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule dxfId="113" operator="containsText" priority="121" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="112" operator="containsText" priority="122" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
+    </cfRule>
+    <cfRule dxfId="111" operator="containsText" priority="123" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule dxfId="110" operator="equal" priority="115" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="109" operator="equal" priority="116" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="108" operator="equal" priority="117" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule dxfId="107" operator="containsText" priority="109" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="106" operator="containsText" priority="110" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="105" operator="containsText" priority="111" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule dxfId="104" operator="containsText" priority="112" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="103" operator="containsText" priority="113" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
+    </cfRule>
+    <cfRule dxfId="102" operator="containsText" priority="114" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule dxfId="101" operator="equal" priority="106" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="100" operator="equal" priority="107" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="99" operator="equal" priority="108" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:D43">
+    <cfRule dxfId="98" operator="containsText" priority="100" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="97" operator="containsText" priority="101" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="96" operator="containsText" priority="102" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:D43">
+    <cfRule dxfId="95" operator="containsText" priority="103" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="94" operator="containsText" priority="104" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
+    </cfRule>
+    <cfRule dxfId="93" operator="containsText" priority="105" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule dxfId="92" operator="equal" priority="97" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="91" operator="equal" priority="98" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="90" operator="equal" priority="99" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule dxfId="89" operator="equal" priority="94" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="88" operator="equal" priority="95" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="87" operator="equal" priority="96" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule dxfId="86" operator="equal" priority="85" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="85" operator="equal" priority="86" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="84" operator="equal" priority="87" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule dxfId="83" operator="containsText" priority="88" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="82" operator="containsText" priority="89" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="81" operator="containsText" priority="90" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule dxfId="80" operator="containsText" priority="91" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="79" operator="containsText" priority="92" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
+    </cfRule>
+    <cfRule dxfId="78" operator="containsText" priority="93" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule dxfId="77" operator="containsText" priority="79" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="76" operator="containsText" priority="80" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="75" operator="containsText" priority="81" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66">
+    <cfRule dxfId="74" operator="containsText" priority="82" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="73" operator="containsText" priority="83" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D66)))</formula>
+    </cfRule>
+    <cfRule dxfId="72" operator="containsText" priority="84" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule dxfId="71" operator="equal" priority="76" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="70" operator="equal" priority="77" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="69" operator="equal" priority="78" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule dxfId="68" operator="containsText" priority="70" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="67" operator="containsText" priority="71" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="66" operator="containsText" priority="72" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule dxfId="65" operator="containsText" priority="73" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="64" operator="containsText" priority="74" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D67)))</formula>
+    </cfRule>
+    <cfRule dxfId="63" operator="containsText" priority="75" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule dxfId="62" operator="equal" priority="67" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="61" operator="equal" priority="68" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="60" operator="equal" priority="69" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule dxfId="59" operator="equal" priority="58" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="58" operator="equal" priority="59" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="57" operator="equal" priority="60" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule dxfId="56" operator="equal" priority="43" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="55" operator="equal" priority="44" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="54" operator="equal" priority="45" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46:D47">
+    <cfRule dxfId="53" operator="containsText" priority="49" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="52" operator="containsText" priority="50" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="51" operator="containsText" priority="51" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46:D47">
+    <cfRule dxfId="50" operator="containsText" priority="52" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="49" operator="containsText" priority="53" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
+    </cfRule>
+    <cfRule dxfId="48" operator="containsText" priority="54" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule dxfId="47" operator="equal" priority="46" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="46" operator="equal" priority="47" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="45" operator="equal" priority="48" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule dxfId="44" operator="containsText" priority="37" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="43" operator="containsText" priority="38" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="42" operator="containsText" priority="39" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule dxfId="41" operator="containsText" priority="40" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="40" operator="containsText" priority="41" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D68)))</formula>
+    </cfRule>
+    <cfRule dxfId="39" operator="containsText" priority="42" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule dxfId="38" operator="equal" priority="34" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="37" operator="equal" priority="35" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="36" operator="equal" priority="36" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69">
+    <cfRule dxfId="35" operator="containsText" priority="28" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="34" operator="containsText" priority="29" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="33" operator="containsText" priority="30" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69">
+    <cfRule dxfId="32" operator="containsText" priority="31" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="31" operator="containsText" priority="32" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D69)))</formula>
+    </cfRule>
+    <cfRule dxfId="30" operator="containsText" priority="33" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule dxfId="29" operator="equal" priority="25" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="28" operator="equal" priority="26" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="27" operator="equal" priority="27" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule dxfId="26" operator="equal" priority="16" type="cellIs">
+      <formula>"LOW"</formula>
+    </cfRule>
+    <cfRule dxfId="25" operator="equal" priority="17" type="cellIs">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule dxfId="24" operator="equal" priority="18" type="cellIs">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule dxfId="23" operator="containsText" priority="10" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="338" operator="containsText" text="Fail">
+    <cfRule dxfId="22" operator="containsText" priority="11" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="252" priority="339" operator="containsText" text="Pass">
+    <cfRule dxfId="21" operator="containsText" priority="12" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D50">
-    <cfRule type="containsText" dxfId="251" priority="340" operator="containsText" text="Skip:">
+  <conditionalFormatting sqref="D48">
+    <cfRule dxfId="20" operator="containsText" priority="13" text="Skip:" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Skip:",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="341" operator="containsText" text="Fail">
+    <cfRule dxfId="19" operator="containsText" priority="14" text="Fail" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Fail",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="342" operator="containsText" text="Pass">
+    <cfRule dxfId="18" operator="containsText" priority="15" text="Pass" type="containsText">
       <formula>NOT(ISERROR(SEARCH("Pass",D48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E33">
-    <cfRule type="cellIs" dxfId="248" priority="256" operator="equal">
+  <conditionalFormatting sqref="E49">
+    <cfRule dxfId="17" operator="equal" priority="7" type="cellIs">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="257" operator="equal">
+    <cfRule dxfId="16" operator="equal" priority="8" type="cellIs">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="258" operator="equal">
+    <cfRule dxfId="15" operator="equal" priority="9" type="cellIs">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48:E50">
-    <cfRule type="cellIs" dxfId="245" priority="298" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="244" priority="299" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="300" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="242" priority="211" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="212" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="213" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D33">
-    <cfRule type="containsText" dxfId="239" priority="259" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="260" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="261" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D33">
-    <cfRule type="containsText" dxfId="236" priority="262" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="235" priority="263" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="264" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="233" priority="241" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="242" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="231" priority="243" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="230" priority="244" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="245" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="246" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="227" priority="238" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="239" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="240" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="containsText" dxfId="224" priority="232" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="223" priority="233" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="234" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="containsText" dxfId="221" priority="235" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="236" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="237" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="218" priority="229" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="230" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="231" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="215" priority="223" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="224" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="225" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="212" priority="226" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="227" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="228" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="209" priority="220" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="221" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="222" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="206" priority="214" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="215" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="216" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="203" priority="217" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="218" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="219" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="200" priority="205" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="206" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="207" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="197" priority="208" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="209" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="210" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
-    <cfRule type="cellIs" dxfId="194" priority="202" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="203" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="204" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="191" priority="196" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="197" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="198" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="188" priority="199" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="200" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="201" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="185" priority="193" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="194" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="195" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="182" priority="187" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="188" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="189" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="179" priority="190" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="191" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="192" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" dxfId="176" priority="184" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="185" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="186" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="173" priority="178" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="179" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="180" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="170" priority="181" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="182" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="183" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" dxfId="167" priority="175" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="176" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="177" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="containsText" dxfId="164" priority="169" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="170" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="171" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="containsText" dxfId="161" priority="172" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="173" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="174" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="158" priority="166" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="167" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="168" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="containsText" dxfId="155" priority="160" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="161" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="162" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="containsText" dxfId="152" priority="163" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="164" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="165" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="149" priority="157" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="158" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="159" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61:D62">
-    <cfRule type="containsText" dxfId="146" priority="151" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="152" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="153" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61:D62">
-    <cfRule type="containsText" dxfId="143" priority="154" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="155" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="156" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E62">
-    <cfRule type="cellIs" dxfId="140" priority="148" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="149" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="150" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="containsText" dxfId="137" priority="142" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="143" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="144" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="containsText" dxfId="134" priority="145" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="146" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="147" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
-    <cfRule type="cellIs" dxfId="131" priority="139" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="140" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="141" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="128" priority="130" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="131" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="132" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="125" priority="133" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="134" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="135" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="122" priority="136" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="137" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="138" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="119" priority="121" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="122" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="123" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="116" priority="124" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="125" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="126" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="113" priority="127" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="128" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="129" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="110" priority="118" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="119" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="120" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="107" priority="112" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="113" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="114" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="104" priority="115" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="116" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="117" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="101" priority="109" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="110" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="111" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="98" priority="103" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="104" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="105" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="95" priority="106" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="107" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="108" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="92" priority="100" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="101" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="102" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="95" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="96" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="86" priority="97" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="98" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="99" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="83" priority="91" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="92" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="93" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="80" priority="85" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="86" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="87" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="77" priority="88" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="89" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="90" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="74" priority="82" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="83" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="84" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D43">
-    <cfRule type="containsText" dxfId="71" priority="76" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="77" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="78" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41:D43">
-    <cfRule type="containsText" dxfId="68" priority="79" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="80" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="81" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="65" priority="73" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="74" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="75" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="59" priority="61" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="56" priority="64" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="65" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="66" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="53" priority="67" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="68" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="69" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="containsText" dxfId="50" priority="55" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="57" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="containsText" dxfId="47" priority="58" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="59" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="60" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="containsText" dxfId="41" priority="46" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="47" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="48" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="containsText" dxfId="38" priority="49" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="51" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46:D47">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46:D47">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D66)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D66)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D66)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D66)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D66)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D66)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D67)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D67)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Skip:">
-      <formula>NOT(ISERROR(SEARCH("Skip:",D67)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",D67)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",D67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"LOW"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Low"</formula>
+  <conditionalFormatting sqref="D49">
+    <cfRule dxfId="11" operator="containsText" priority="1" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="10" operator="containsText" priority="2" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="9" operator="containsText" priority="3" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule dxfId="5" operator="containsText" priority="4" text="Skip:" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Skip:",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="4" operator="containsText" priority="5" text="Fail" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Fail",D49)))</formula>
+    </cfRule>
+    <cfRule dxfId="3" operator="containsText" priority="6" text="Pass" type="containsText">
+      <formula>NOT(ISERROR(SEARCH("Pass",D49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation showDropDown="1" showErrorMessage="1" showInputMessage="1" sqref="C1">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C67" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C2:C69" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E67" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E69" type="list">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="D3" pane="bottomLeft" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="19" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="1025" width="19" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="6" max="1025" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6694,9 +7147,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="javascript:srcUp(%27%2F0054x000001Z8z4%3Fnoredirect%3D1%26isUserEntityOverride%3D1%26isdtp%3Dp1%27);" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink display="javascript:srcUp(%27%2F0054x000001Z8z4%3Fnoredirect%3D1%26isUserEntityOverride%3D1%26isdtp%3Dp1%27);" r:id="rId1" ref="E3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change excel format only
Signed-off-by: vineet <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vineet Kumar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="315">
   <si>
     <t>Module_Name</t>
   </si>
@@ -725,9 +725,6 @@
   </si>
   <si>
     <t>Module3Tc067_1_ChangetheUserIndustryAsHealthCareAndVerifyImpactonNavigationMenu</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Module3Tc067_2_ChangetheUserIndustryAsHealthCareAndVerifyImpactonNavigationMenu</t>
@@ -1160,7 +1157,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1201,9 +1198,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1211,7 +1205,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="751">
+  <dxfs count="753">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9D18E"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -9809,7 +9817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -9831,7 +9839,7 @@
     </row>
     <row r="2" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>7</v>
@@ -9850,7 +9858,7 @@
         <v>84</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>232</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9871,52 +9879,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I3:I5">
-    <cfRule type="cellIs" dxfId="750" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="752" priority="18" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I5">
-    <cfRule type="cellIs" dxfId="749" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="751" priority="19" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="748" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="750" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="747" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="749" priority="14" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="746" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="748" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="745" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="747" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="744" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="746" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="743" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="745" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" dxfId="742" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="744" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" dxfId="741" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="743" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9935,14 +9943,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -11032,7 +11040,7 @@
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="3" t="s">
@@ -11332,7 +11340,7 @@
     </row>
     <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="3" t="s">
@@ -11347,7 +11355,7 @@
     </row>
     <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="3" t="s">
@@ -11392,7 +11400,7 @@
     </row>
     <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="3" t="s">
@@ -11407,7 +11415,7 @@
     </row>
     <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="3" t="s">
@@ -11422,7 +11430,7 @@
     </row>
     <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="3" t="s">
@@ -11437,7 +11445,7 @@
     </row>
     <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="3" t="s">
@@ -11452,7 +11460,7 @@
     </row>
     <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="3" t="s">
@@ -11467,7 +11475,7 @@
     </row>
     <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="3" t="s">
@@ -11482,7 +11490,7 @@
     </row>
     <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="3" t="s">
@@ -11497,7 +11505,7 @@
     </row>
     <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="3" t="s">
@@ -11512,7 +11520,7 @@
     </row>
     <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="3" t="s">
@@ -11527,7 +11535,7 @@
     </row>
     <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="3" t="s">
@@ -11542,7 +11550,7 @@
     </row>
     <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="3" t="s">
@@ -11557,7 +11565,7 @@
     </row>
     <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="3" t="s">
@@ -11572,7 +11580,7 @@
     </row>
     <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="3" t="s">
@@ -11587,7 +11595,7 @@
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="3" t="s">
@@ -11602,7 +11610,7 @@
     </row>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="3" t="s">
@@ -11617,7 +11625,7 @@
     </row>
     <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="3" t="s">
@@ -11632,7 +11640,7 @@
     </row>
     <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="3" t="s">
@@ -11647,7 +11655,7 @@
     </row>
     <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="3" t="s">
@@ -11662,7 +11670,7 @@
     </row>
     <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="3" t="s">
@@ -11677,7 +11685,7 @@
     </row>
     <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B116" s="8"/>
       <c r="C116" s="3" t="s">
@@ -11692,7 +11700,7 @@
     </row>
     <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="3" t="s">
@@ -11707,7 +11715,7 @@
     </row>
     <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B118" s="8"/>
       <c r="C118" s="3" t="s">
@@ -11722,7 +11730,7 @@
     </row>
     <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="3" t="s">
@@ -11737,7 +11745,7 @@
     </row>
     <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="3" t="s">
@@ -11815,7 +11823,7 @@
         <v>159</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>7</v>
@@ -11832,7 +11840,7 @@
         <v>160</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>7</v>
@@ -11866,7 +11874,7 @@
         <v>162</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>7</v>
@@ -11883,7 +11891,7 @@
         <v>163</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>7</v>
@@ -11900,7 +11908,7 @@
         <v>164</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>7</v>
@@ -11917,7 +11925,7 @@
         <v>165</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>7</v>
@@ -11931,7 +11939,7 @@
     </row>
     <row r="132" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B132" s="8">
         <v>1</v>
@@ -11948,7 +11956,7 @@
     </row>
     <row r="133" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B133" s="8">
         <v>1</v>
@@ -12288,7 +12296,7 @@
     </row>
     <row r="153" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B153" s="8">
         <v>23</v>
@@ -12305,7 +12313,7 @@
     </row>
     <row r="154" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B154" s="8">
         <v>23</v>
@@ -13087,7 +13095,7 @@
     </row>
     <row r="200" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B200" s="8">
         <v>67</v>
@@ -13104,7 +13112,7 @@
     </row>
     <row r="201" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B201" s="8">
         <v>68</v>
@@ -13121,7 +13129,7 @@
     </row>
     <row r="202" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B202" s="8">
         <v>68</v>
@@ -13138,7 +13146,7 @@
     </row>
     <row r="203" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B203" s="8">
         <v>69</v>
@@ -13155,7 +13163,7 @@
     </row>
     <row r="204" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B204" s="8">
         <v>69</v>
@@ -13172,7 +13180,7 @@
     </row>
     <row r="205" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B205" s="8">
         <v>70</v>
@@ -13189,7 +13197,7 @@
     </row>
     <row r="206" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B206" s="8">
         <v>71</v>
@@ -13206,7 +13214,7 @@
     </row>
     <row r="207" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B207" s="8">
         <v>72</v>
@@ -13223,7 +13231,7 @@
     </row>
     <row r="208" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B208" s="8">
         <v>73</v>
@@ -13240,7 +13248,7 @@
     </row>
     <row r="209" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B209" s="8">
         <v>74</v>
@@ -13257,7 +13265,7 @@
     </row>
     <row r="210" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B210" s="8">
         <v>75</v>
@@ -13274,7 +13282,7 @@
     </row>
     <row r="211" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B211" s="8">
         <v>76</v>
@@ -13291,7 +13299,7 @@
     </row>
     <row r="212" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B212" s="8">
         <v>76</v>
@@ -13308,7 +13316,7 @@
     </row>
     <row r="213" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B213" s="8">
         <v>77</v>
@@ -13325,7 +13333,7 @@
     </row>
     <row r="214" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B214" s="8">
         <v>77</v>
@@ -13342,7 +13350,7 @@
     </row>
     <row r="215" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B215" s="8">
         <v>78</v>
@@ -13359,7 +13367,7 @@
     </row>
     <row r="216" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B216" s="8">
         <v>78</v>
@@ -13376,7 +13384,7 @@
     </row>
     <row r="217" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B217" s="8">
         <v>79</v>
@@ -13393,7 +13401,7 @@
     </row>
     <row r="218" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B218" s="8">
         <v>80</v>
@@ -13410,7 +13418,7 @@
     </row>
     <row r="219" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B219" s="8">
         <v>81</v>
@@ -13427,7 +13435,7 @@
     </row>
     <row r="220" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B220" s="8">
         <v>82</v>
@@ -13444,7 +13452,7 @@
     </row>
     <row r="221" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B221" s="8">
         <v>83</v>
@@ -13461,7 +13469,7 @@
     </row>
     <row r="222" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B222" s="8">
         <v>84</v>
@@ -13478,7 +13486,7 @@
     </row>
     <row r="223" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B223" s="8">
         <v>85</v>
@@ -13495,10 +13503,10 @@
     </row>
     <row r="224" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>7</v>
@@ -13512,7 +13520,7 @@
     </row>
     <row r="225" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B225" s="8">
         <v>88</v>
@@ -13529,7 +13537,7 @@
     </row>
     <row r="226" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B226" s="8">
         <v>89</v>
@@ -13546,7 +13554,7 @@
     </row>
     <row r="227" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B227" s="8">
         <v>90</v>
@@ -13563,7 +13571,7 @@
     </row>
     <row r="228" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B228" s="8">
         <v>91</v>
@@ -13580,7 +13588,7 @@
     </row>
     <row r="229" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B229" s="8">
         <v>93</v>
@@ -13597,7 +13605,7 @@
     </row>
     <row r="230" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B230" s="8">
         <v>94</v>
@@ -13614,7 +13622,7 @@
     </row>
     <row r="231" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B231" s="8">
         <v>95</v>
@@ -13868,7 +13876,7 @@
       </c>
     </row>
     <row r="246" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="16" t="s">
+      <c r="A246" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B246" s="8">
@@ -13885,7 +13893,7 @@
       </c>
     </row>
     <row r="247" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
+      <c r="A247" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B247" s="8">
@@ -13902,7 +13910,7 @@
       </c>
     </row>
     <row r="248" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
+      <c r="A248" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B248" s="8">
@@ -13919,7 +13927,7 @@
       </c>
     </row>
     <row r="249" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
+      <c r="A249" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B249" s="8">
@@ -13936,7 +13944,7 @@
       </c>
     </row>
     <row r="250" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" t="s">
+      <c r="A250" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B250" s="8">
@@ -13953,7 +13961,7 @@
       </c>
     </row>
     <row r="251" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
+      <c r="A251" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B251" s="8">
@@ -13970,7 +13978,7 @@
       </c>
     </row>
     <row r="252" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A252" t="s">
+      <c r="A252" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B252" s="8">
@@ -13987,7 +13995,7 @@
       </c>
     </row>
     <row r="253" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A253" t="s">
+      <c r="A253" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B253" s="8">
@@ -14004,7 +14012,7 @@
       </c>
     </row>
     <row r="254" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A254" t="s">
+      <c r="A254" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B254" s="8">
@@ -14021,7 +14029,7 @@
       </c>
     </row>
     <row r="255" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A255" t="s">
+      <c r="A255" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B255" s="8">
@@ -14038,7 +14046,7 @@
       </c>
     </row>
     <row r="256" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A256" t="s">
+      <c r="A256" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B256" s="8">
@@ -14055,7 +14063,7 @@
       </c>
     </row>
     <row r="257" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A257" t="s">
+      <c r="A257" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B257" s="8">
@@ -14072,7 +14080,7 @@
       </c>
     </row>
     <row r="258" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A258" t="s">
+      <c r="A258" s="7" t="s">
         <v>192</v>
       </c>
       <c r="B258" s="8">
@@ -14089,7 +14097,7 @@
       </c>
     </row>
     <row r="259" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A259" t="s">
+      <c r="A259" s="7" t="s">
         <v>193</v>
       </c>
       <c r="B259" s="8">
@@ -14106,8 +14114,8 @@
       </c>
     </row>
     <row r="260" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A260" t="s">
-        <v>261</v>
+      <c r="A260" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="B260" s="8">
         <v>32</v>
@@ -14123,8 +14131,8 @@
       </c>
     </row>
     <row r="261" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A261" t="s">
-        <v>262</v>
+      <c r="A261" s="7" t="s">
+        <v>261</v>
       </c>
       <c r="B261" s="8"/>
       <c r="C261" s="14" t="s">
@@ -14138,8 +14146,8 @@
       </c>
     </row>
     <row r="262" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A262" t="s">
-        <v>263</v>
+      <c r="A262" s="7" t="s">
+        <v>262</v>
       </c>
       <c r="B262" s="8"/>
       <c r="C262" s="14" t="s">
@@ -14155,2719 +14163,2719 @@
   </sheetData>
   <autoFilter ref="A1:E262"/>
   <conditionalFormatting sqref="E6 E75:E93 E121 E95:E102">
-    <cfRule type="cellIs" dxfId="740" priority="1717" operator="equal">
+    <cfRule type="cellIs" dxfId="742" priority="1717" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="739" priority="1718" operator="equal">
+    <cfRule type="cellIs" dxfId="741" priority="1718" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="738" priority="1719" operator="equal">
+    <cfRule type="cellIs" dxfId="740" priority="1719" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 D131 D80:D93 D95:D102">
-    <cfRule type="containsText" dxfId="737" priority="1756" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="739" priority="1756" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="736" priority="1757" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="738" priority="1757" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="735" priority="1758" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="737" priority="1758" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="734" priority="1759" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="736" priority="1759" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="733" priority="1760" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="735" priority="1760" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="732" priority="1761" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="734" priority="1761" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="731" priority="1750" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="733" priority="1750" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="730" priority="1751" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="732" priority="1751" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="729" priority="1752" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="731" priority="1752" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="728" priority="1753" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="730" priority="1753" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="727" priority="1754" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="729" priority="1754" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="726" priority="1755" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="728" priority="1755" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="725" priority="1744" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="727" priority="1744" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="724" priority="1745" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="726" priority="1745" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="723" priority="1746" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="725" priority="1746" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="722" priority="1747" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="724" priority="1747" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="721" priority="1748" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="723" priority="1748" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="720" priority="1749" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="722" priority="1749" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="719" priority="1738" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="721" priority="1738" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="718" priority="1739" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="720" priority="1739" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="717" priority="1740" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="719" priority="1740" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="716" priority="1741" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="718" priority="1741" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="715" priority="1742" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="717" priority="1742" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="714" priority="1743" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="716" priority="1743" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="713" priority="1732" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="715" priority="1732" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="712" priority="1733" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="714" priority="1733" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="711" priority="1734" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="713" priority="1734" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="710" priority="1735" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="712" priority="1735" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="709" priority="1736" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="711" priority="1736" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="708" priority="1737" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="710" priority="1737" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="707" priority="1729" operator="equal">
+    <cfRule type="cellIs" dxfId="709" priority="1729" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="706" priority="1730" operator="equal">
+    <cfRule type="cellIs" dxfId="708" priority="1730" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="705" priority="1731" operator="equal">
+    <cfRule type="cellIs" dxfId="707" priority="1731" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="704" priority="1726" operator="equal">
+    <cfRule type="cellIs" dxfId="706" priority="1726" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="703" priority="1727" operator="equal">
+    <cfRule type="cellIs" dxfId="705" priority="1727" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="702" priority="1728" operator="equal">
+    <cfRule type="cellIs" dxfId="704" priority="1728" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="701" priority="1723" operator="equal">
+    <cfRule type="cellIs" dxfId="703" priority="1723" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="700" priority="1724" operator="equal">
+    <cfRule type="cellIs" dxfId="702" priority="1724" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="699" priority="1725" operator="equal">
+    <cfRule type="cellIs" dxfId="701" priority="1725" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="698" priority="1720" operator="equal">
+    <cfRule type="cellIs" dxfId="700" priority="1720" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="697" priority="1721" operator="equal">
+    <cfRule type="cellIs" dxfId="699" priority="1721" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="696" priority="1722" operator="equal">
+    <cfRule type="cellIs" dxfId="698" priority="1722" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="695" priority="1612" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="697" priority="1612" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="694" priority="1613" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="696" priority="1613" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="693" priority="1614" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="695" priority="1614" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="692" priority="1615" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="694" priority="1615" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="691" priority="1616" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="693" priority="1616" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="690" priority="1617" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="692" priority="1617" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="689" priority="1609" operator="equal">
+    <cfRule type="cellIs" dxfId="691" priority="1609" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="688" priority="1610" operator="equal">
+    <cfRule type="cellIs" dxfId="690" priority="1610" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="687" priority="1611" operator="equal">
+    <cfRule type="cellIs" dxfId="689" priority="1611" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D232:D234">
-    <cfRule type="containsText" dxfId="686" priority="1681" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="688" priority="1681" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="685" priority="1682" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="687" priority="1682" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="684" priority="1683" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="686" priority="1683" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D232:D234">
-    <cfRule type="containsText" dxfId="683" priority="1684" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="685" priority="1684" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="682" priority="1685" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="684" priority="1685" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="681" priority="1686" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="683" priority="1686" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E67">
-    <cfRule type="cellIs" dxfId="680" priority="1600" operator="equal">
+    <cfRule type="cellIs" dxfId="682" priority="1600" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="679" priority="1601" operator="equal">
+    <cfRule type="cellIs" dxfId="681" priority="1601" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="678" priority="1602" operator="equal">
+    <cfRule type="cellIs" dxfId="680" priority="1602" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E232:E234">
-    <cfRule type="cellIs" dxfId="677" priority="1642" operator="equal">
+    <cfRule type="cellIs" dxfId="679" priority="1642" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="676" priority="1643" operator="equal">
+    <cfRule type="cellIs" dxfId="678" priority="1643" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="675" priority="1644" operator="equal">
+    <cfRule type="cellIs" dxfId="677" priority="1644" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E238">
-    <cfRule type="cellIs" dxfId="674" priority="1555" operator="equal">
+    <cfRule type="cellIs" dxfId="676" priority="1555" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="673" priority="1556" operator="equal">
+    <cfRule type="cellIs" dxfId="675" priority="1556" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="672" priority="1557" operator="equal">
+    <cfRule type="cellIs" dxfId="674" priority="1557" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D67 D121">
-    <cfRule type="containsText" dxfId="671" priority="1603" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="673" priority="1603" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="670" priority="1604" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="672" priority="1604" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="669" priority="1605" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="671" priority="1605" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D67 D121">
-    <cfRule type="containsText" dxfId="668" priority="1606" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="670" priority="1606" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="667" priority="1607" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="669" priority="1607" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="666" priority="1608" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="668" priority="1608" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D235">
-    <cfRule type="containsText" dxfId="665" priority="1585" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="667" priority="1585" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D235)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="664" priority="1586" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="666" priority="1586" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D235)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="663" priority="1587" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="665" priority="1587" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D235">
-    <cfRule type="containsText" dxfId="662" priority="1588" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="664" priority="1588" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D235)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="661" priority="1589" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="663" priority="1589" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D235)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="660" priority="1590" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="662" priority="1590" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E235">
-    <cfRule type="cellIs" dxfId="659" priority="1582" operator="equal">
+    <cfRule type="cellIs" dxfId="661" priority="1582" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="658" priority="1583" operator="equal">
+    <cfRule type="cellIs" dxfId="660" priority="1583" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="657" priority="1584" operator="equal">
+    <cfRule type="cellIs" dxfId="659" priority="1584" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D236">
-    <cfRule type="containsText" dxfId="656" priority="1576" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="658" priority="1576" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D236)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="655" priority="1577" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="657" priority="1577" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D236)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="654" priority="1578" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="656" priority="1578" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D236">
-    <cfRule type="containsText" dxfId="653" priority="1579" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="655" priority="1579" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D236)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="652" priority="1580" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="654" priority="1580" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D236)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="651" priority="1581" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="653" priority="1581" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E236">
-    <cfRule type="cellIs" dxfId="650" priority="1573" operator="equal">
+    <cfRule type="cellIs" dxfId="652" priority="1573" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="649" priority="1574" operator="equal">
+    <cfRule type="cellIs" dxfId="651" priority="1574" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="648" priority="1575" operator="equal">
+    <cfRule type="cellIs" dxfId="650" priority="1575" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D237">
-    <cfRule type="containsText" dxfId="647" priority="1567" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="649" priority="1567" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D237)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="646" priority="1568" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="648" priority="1568" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D237)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="645" priority="1569" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="647" priority="1569" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D237">
-    <cfRule type="containsText" dxfId="644" priority="1570" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="646" priority="1570" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D237)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="643" priority="1571" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="645" priority="1571" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D237)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="642" priority="1572" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="644" priority="1572" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E237">
-    <cfRule type="cellIs" dxfId="641" priority="1564" operator="equal">
+    <cfRule type="cellIs" dxfId="643" priority="1564" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="640" priority="1565" operator="equal">
+    <cfRule type="cellIs" dxfId="642" priority="1565" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="639" priority="1566" operator="equal">
+    <cfRule type="cellIs" dxfId="641" priority="1566" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D238">
-    <cfRule type="containsText" dxfId="638" priority="1558" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="640" priority="1558" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="637" priority="1559" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="639" priority="1559" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="636" priority="1560" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="638" priority="1560" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D238">
-    <cfRule type="containsText" dxfId="635" priority="1561" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="637" priority="1561" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="634" priority="1562" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="636" priority="1562" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="633" priority="1563" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="635" priority="1563" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D239">
-    <cfRule type="containsText" dxfId="632" priority="1549" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="634" priority="1549" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="631" priority="1550" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="633" priority="1550" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="630" priority="1551" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="632" priority="1551" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D239">
-    <cfRule type="containsText" dxfId="629" priority="1552" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="631" priority="1552" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="628" priority="1553" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="630" priority="1553" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="627" priority="1554" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="629" priority="1554" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E239">
-    <cfRule type="cellIs" dxfId="626" priority="1546" operator="equal">
+    <cfRule type="cellIs" dxfId="628" priority="1546" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="625" priority="1547" operator="equal">
+    <cfRule type="cellIs" dxfId="627" priority="1547" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="624" priority="1548" operator="equal">
+    <cfRule type="cellIs" dxfId="626" priority="1548" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D240">
-    <cfRule type="containsText" dxfId="623" priority="1540" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="625" priority="1540" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="622" priority="1541" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="624" priority="1541" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="621" priority="1542" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="623" priority="1542" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D240">
-    <cfRule type="containsText" dxfId="620" priority="1543" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="622" priority="1543" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="619" priority="1544" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="621" priority="1544" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="618" priority="1545" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="620" priority="1545" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E240">
-    <cfRule type="cellIs" dxfId="617" priority="1537" operator="equal">
+    <cfRule type="cellIs" dxfId="619" priority="1537" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="616" priority="1538" operator="equal">
+    <cfRule type="cellIs" dxfId="618" priority="1538" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="615" priority="1539" operator="equal">
+    <cfRule type="cellIs" dxfId="617" priority="1539" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D241">
-    <cfRule type="containsText" dxfId="614" priority="1531" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="616" priority="1531" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="613" priority="1532" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="615" priority="1532" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="612" priority="1533" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="614" priority="1533" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D241">
-    <cfRule type="containsText" dxfId="611" priority="1534" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="613" priority="1534" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="610" priority="1535" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="612" priority="1535" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="609" priority="1536" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="611" priority="1536" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E241">
-    <cfRule type="cellIs" dxfId="608" priority="1528" operator="equal">
+    <cfRule type="cellIs" dxfId="610" priority="1528" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="607" priority="1529" operator="equal">
+    <cfRule type="cellIs" dxfId="609" priority="1529" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="606" priority="1530" operator="equal">
+    <cfRule type="cellIs" dxfId="608" priority="1530" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D242">
-    <cfRule type="containsText" dxfId="605" priority="1522" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="607" priority="1522" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D242)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="604" priority="1523" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="606" priority="1523" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D242)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="603" priority="1524" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="605" priority="1524" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D242)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D242">
-    <cfRule type="containsText" dxfId="602" priority="1525" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="604" priority="1525" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D242)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="601" priority="1526" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="603" priority="1526" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D242)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="600" priority="1527" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="602" priority="1527" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D242)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E242">
-    <cfRule type="cellIs" dxfId="599" priority="1519" operator="equal">
+    <cfRule type="cellIs" dxfId="601" priority="1519" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="598" priority="1520" operator="equal">
+    <cfRule type="cellIs" dxfId="600" priority="1520" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="597" priority="1521" operator="equal">
+    <cfRule type="cellIs" dxfId="599" priority="1521" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D243">
-    <cfRule type="containsText" dxfId="596" priority="1513" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="598" priority="1513" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D243)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="595" priority="1514" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="597" priority="1514" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D243)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="594" priority="1515" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="596" priority="1515" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D243)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D243">
-    <cfRule type="containsText" dxfId="593" priority="1516" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="595" priority="1516" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D243)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="592" priority="1517" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="594" priority="1517" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D243)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="591" priority="1518" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="593" priority="1518" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D243)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E243">
-    <cfRule type="cellIs" dxfId="590" priority="1510" operator="equal">
+    <cfRule type="cellIs" dxfId="592" priority="1510" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="589" priority="1511" operator="equal">
+    <cfRule type="cellIs" dxfId="591" priority="1511" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="588" priority="1512" operator="equal">
+    <cfRule type="cellIs" dxfId="590" priority="1512" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D244">
-    <cfRule type="containsText" dxfId="587" priority="1504" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="589" priority="1504" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D244)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="586" priority="1505" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="588" priority="1505" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D244)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="585" priority="1506" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="587" priority="1506" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D244)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D244">
-    <cfRule type="containsText" dxfId="584" priority="1507" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="586" priority="1507" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D244)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="583" priority="1508" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="585" priority="1508" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D244)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="582" priority="1509" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="584" priority="1509" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D244)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E244">
-    <cfRule type="cellIs" dxfId="581" priority="1501" operator="equal">
+    <cfRule type="cellIs" dxfId="583" priority="1501" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="580" priority="1502" operator="equal">
+    <cfRule type="cellIs" dxfId="582" priority="1502" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="579" priority="1503" operator="equal">
+    <cfRule type="cellIs" dxfId="581" priority="1503" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D245:D246">
-    <cfRule type="containsText" dxfId="578" priority="1495" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="580" priority="1495" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D245)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="577" priority="1496" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="579" priority="1496" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D245)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="576" priority="1497" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="578" priority="1497" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D245:D246">
-    <cfRule type="containsText" dxfId="575" priority="1498" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="577" priority="1498" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D245)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="574" priority="1499" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="576" priority="1499" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D245)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="573" priority="1500" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="575" priority="1500" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E245:E246">
-    <cfRule type="cellIs" dxfId="572" priority="1492" operator="equal">
+    <cfRule type="cellIs" dxfId="574" priority="1492" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="571" priority="1493" operator="equal">
+    <cfRule type="cellIs" dxfId="573" priority="1493" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="570" priority="1494" operator="equal">
+    <cfRule type="cellIs" dxfId="572" priority="1494" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D247">
-    <cfRule type="containsText" dxfId="569" priority="1486" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="571" priority="1486" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="568" priority="1487" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="570" priority="1487" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="567" priority="1488" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="569" priority="1488" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D247">
-    <cfRule type="containsText" dxfId="566" priority="1489" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="568" priority="1489" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="565" priority="1490" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="567" priority="1490" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="564" priority="1491" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="566" priority="1491" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E247">
-    <cfRule type="cellIs" dxfId="563" priority="1483" operator="equal">
+    <cfRule type="cellIs" dxfId="565" priority="1483" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="562" priority="1484" operator="equal">
+    <cfRule type="cellIs" dxfId="564" priority="1484" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="561" priority="1485" operator="equal">
+    <cfRule type="cellIs" dxfId="563" priority="1485" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E122">
-    <cfRule type="cellIs" dxfId="560" priority="1474" operator="equal">
+    <cfRule type="cellIs" dxfId="562" priority="1474" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="559" priority="1475" operator="equal">
+    <cfRule type="cellIs" dxfId="561" priority="1475" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="558" priority="1476" operator="equal">
+    <cfRule type="cellIs" dxfId="560" priority="1476" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D122">
-    <cfRule type="containsText" dxfId="557" priority="1477" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="559" priority="1477" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D122)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="556" priority="1478" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="558" priority="1478" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D122)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="555" priority="1479" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="557" priority="1479" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D122">
-    <cfRule type="containsText" dxfId="554" priority="1480" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="556" priority="1480" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D122)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="553" priority="1481" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="555" priority="1481" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D122)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="552" priority="1482" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="554" priority="1482" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E123">
-    <cfRule type="cellIs" dxfId="551" priority="1465" operator="equal">
+    <cfRule type="cellIs" dxfId="553" priority="1465" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="550" priority="1466" operator="equal">
+    <cfRule type="cellIs" dxfId="552" priority="1466" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="549" priority="1467" operator="equal">
+    <cfRule type="cellIs" dxfId="551" priority="1467" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="containsText" dxfId="548" priority="1468" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="550" priority="1468" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D123)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="547" priority="1469" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="549" priority="1469" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D123)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="546" priority="1470" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="548" priority="1470" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="containsText" dxfId="545" priority="1471" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="547" priority="1471" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D123)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="544" priority="1472" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="546" priority="1472" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D123)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="543" priority="1473" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="545" priority="1473" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E124">
-    <cfRule type="cellIs" dxfId="542" priority="1462" operator="equal">
+    <cfRule type="cellIs" dxfId="544" priority="1462" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="541" priority="1463" operator="equal">
+    <cfRule type="cellIs" dxfId="543" priority="1463" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="540" priority="1464" operator="equal">
+    <cfRule type="cellIs" dxfId="542" priority="1464" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D124">
-    <cfRule type="containsText" dxfId="539" priority="1456" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="541" priority="1456" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D124)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="538" priority="1457" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="540" priority="1457" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D124)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="537" priority="1458" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="539" priority="1458" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D124">
-    <cfRule type="containsText" dxfId="536" priority="1459" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="538" priority="1459" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D124)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="535" priority="1460" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="537" priority="1460" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D124)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="534" priority="1461" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="536" priority="1461" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E125">
-    <cfRule type="cellIs" dxfId="533" priority="1453" operator="equal">
+    <cfRule type="cellIs" dxfId="535" priority="1453" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="532" priority="1454" operator="equal">
+    <cfRule type="cellIs" dxfId="534" priority="1454" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="531" priority="1455" operator="equal">
+    <cfRule type="cellIs" dxfId="533" priority="1455" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D125">
-    <cfRule type="containsText" dxfId="530" priority="1447" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="532" priority="1447" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D125)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="529" priority="1448" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="531" priority="1448" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D125)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="528" priority="1449" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="530" priority="1449" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D125">
-    <cfRule type="containsText" dxfId="527" priority="1450" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="529" priority="1450" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D125)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="526" priority="1451" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="528" priority="1451" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D125)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="525" priority="1452" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="527" priority="1452" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E126">
-    <cfRule type="cellIs" dxfId="524" priority="1444" operator="equal">
+    <cfRule type="cellIs" dxfId="526" priority="1444" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="523" priority="1445" operator="equal">
+    <cfRule type="cellIs" dxfId="525" priority="1445" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="522" priority="1446" operator="equal">
+    <cfRule type="cellIs" dxfId="524" priority="1446" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D126">
-    <cfRule type="containsText" dxfId="521" priority="1438" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="523" priority="1438" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D126)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="520" priority="1439" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="522" priority="1439" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D126)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="519" priority="1440" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="521" priority="1440" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D126">
-    <cfRule type="containsText" dxfId="518" priority="1441" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="520" priority="1441" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D126)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="517" priority="1442" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="519" priority="1442" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D126)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="516" priority="1443" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="518" priority="1443" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E127">
-    <cfRule type="cellIs" dxfId="515" priority="1435" operator="equal">
+    <cfRule type="cellIs" dxfId="517" priority="1435" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="514" priority="1436" operator="equal">
+    <cfRule type="cellIs" dxfId="516" priority="1436" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="513" priority="1437" operator="equal">
+    <cfRule type="cellIs" dxfId="515" priority="1437" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="containsText" dxfId="512" priority="1429" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="514" priority="1429" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D127)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="511" priority="1430" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="513" priority="1430" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D127)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="510" priority="1431" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="512" priority="1431" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D127)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="containsText" dxfId="509" priority="1432" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="511" priority="1432" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D127)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="508" priority="1433" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="510" priority="1433" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D127)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="507" priority="1434" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="509" priority="1434" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D127)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E128">
-    <cfRule type="cellIs" dxfId="506" priority="1426" operator="equal">
+    <cfRule type="cellIs" dxfId="508" priority="1426" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="505" priority="1427" operator="equal">
+    <cfRule type="cellIs" dxfId="507" priority="1427" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="504" priority="1428" operator="equal">
+    <cfRule type="cellIs" dxfId="506" priority="1428" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D128:D130">
-    <cfRule type="containsText" dxfId="503" priority="1420" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="505" priority="1420" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D128)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="502" priority="1421" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="504" priority="1421" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D128)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="501" priority="1422" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="503" priority="1422" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D128)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D128:D130">
-    <cfRule type="containsText" dxfId="500" priority="1423" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="502" priority="1423" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D128)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="499" priority="1424" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="501" priority="1424" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D128)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="498" priority="1425" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="500" priority="1425" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D128)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E129">
-    <cfRule type="cellIs" dxfId="497" priority="1417" operator="equal">
+    <cfRule type="cellIs" dxfId="499" priority="1417" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="496" priority="1418" operator="equal">
+    <cfRule type="cellIs" dxfId="498" priority="1418" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="495" priority="1419" operator="equal">
+    <cfRule type="cellIs" dxfId="497" priority="1419" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="cellIs" dxfId="494" priority="1414" operator="equal">
+    <cfRule type="cellIs" dxfId="496" priority="1414" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="493" priority="1415" operator="equal">
+    <cfRule type="cellIs" dxfId="495" priority="1415" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="492" priority="1416" operator="equal">
+    <cfRule type="cellIs" dxfId="494" priority="1416" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D248">
-    <cfRule type="containsText" dxfId="491" priority="1399" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="493" priority="1399" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="490" priority="1400" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="492" priority="1400" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="489" priority="1401" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="491" priority="1401" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D248">
-    <cfRule type="containsText" dxfId="488" priority="1402" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="490" priority="1402" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="487" priority="1403" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="489" priority="1403" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="486" priority="1404" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="488" priority="1404" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E248">
-    <cfRule type="cellIs" dxfId="485" priority="1396" operator="equal">
+    <cfRule type="cellIs" dxfId="487" priority="1396" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="484" priority="1397" operator="equal">
+    <cfRule type="cellIs" dxfId="486" priority="1397" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="483" priority="1398" operator="equal">
+    <cfRule type="cellIs" dxfId="485" priority="1398" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D249">
-    <cfRule type="containsText" dxfId="482" priority="1390" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="484" priority="1390" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D249)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="481" priority="1391" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="483" priority="1391" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D249)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="480" priority="1392" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="482" priority="1392" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D249)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D249">
-    <cfRule type="containsText" dxfId="479" priority="1393" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="481" priority="1393" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D249)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="478" priority="1394" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="480" priority="1394" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D249)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="477" priority="1395" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="479" priority="1395" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D249)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E249">
-    <cfRule type="cellIs" dxfId="476" priority="1387" operator="equal">
+    <cfRule type="cellIs" dxfId="478" priority="1387" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="475" priority="1388" operator="equal">
+    <cfRule type="cellIs" dxfId="477" priority="1388" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="474" priority="1389" operator="equal">
+    <cfRule type="cellIs" dxfId="476" priority="1389" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131">
-    <cfRule type="cellIs" dxfId="473" priority="1378" operator="equal">
+    <cfRule type="cellIs" dxfId="475" priority="1378" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="472" priority="1379" operator="equal">
+    <cfRule type="cellIs" dxfId="474" priority="1379" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="471" priority="1380" operator="equal">
+    <cfRule type="cellIs" dxfId="473" priority="1380" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D250">
-    <cfRule type="containsText" dxfId="470" priority="1357" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="472" priority="1357" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D250)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="469" priority="1358" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="471" priority="1358" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D250)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="468" priority="1359" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="470" priority="1359" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D250">
-    <cfRule type="containsText" dxfId="467" priority="1360" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="469" priority="1360" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D250)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="466" priority="1361" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="468" priority="1361" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D250)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="465" priority="1362" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="467" priority="1362" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E250">
-    <cfRule type="cellIs" dxfId="464" priority="1354" operator="equal">
+    <cfRule type="cellIs" dxfId="466" priority="1354" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="463" priority="1355" operator="equal">
+    <cfRule type="cellIs" dxfId="465" priority="1355" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="462" priority="1356" operator="equal">
+    <cfRule type="cellIs" dxfId="464" priority="1356" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D251">
-    <cfRule type="containsText" dxfId="461" priority="1348" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="463" priority="1348" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D251)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="460" priority="1349" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="462" priority="1349" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D251)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="459" priority="1350" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="461" priority="1350" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D251">
-    <cfRule type="containsText" dxfId="458" priority="1351" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="460" priority="1351" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D251)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="457" priority="1352" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="459" priority="1352" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D251)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="456" priority="1353" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="458" priority="1353" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E251">
-    <cfRule type="cellIs" dxfId="455" priority="1345" operator="equal">
+    <cfRule type="cellIs" dxfId="457" priority="1345" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="454" priority="1346" operator="equal">
+    <cfRule type="cellIs" dxfId="456" priority="1346" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="453" priority="1347" operator="equal">
+    <cfRule type="cellIs" dxfId="455" priority="1347" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D252">
-    <cfRule type="containsText" dxfId="452" priority="1252" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="454" priority="1252" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D252)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="451" priority="1253" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="453" priority="1253" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D252)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="450" priority="1254" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="452" priority="1254" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D252">
-    <cfRule type="containsText" dxfId="449" priority="1255" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="451" priority="1255" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D252)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="448" priority="1256" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="450" priority="1256" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D252)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="447" priority="1257" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="449" priority="1257" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E252">
-    <cfRule type="cellIs" dxfId="446" priority="1249" operator="equal">
+    <cfRule type="cellIs" dxfId="448" priority="1249" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="445" priority="1250" operator="equal">
+    <cfRule type="cellIs" dxfId="447" priority="1250" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="444" priority="1251" operator="equal">
+    <cfRule type="cellIs" dxfId="446" priority="1251" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D253">
-    <cfRule type="containsText" dxfId="443" priority="1243" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="445" priority="1243" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D253)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="442" priority="1244" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="444" priority="1244" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D253)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="441" priority="1245" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="443" priority="1245" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D253)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D253">
-    <cfRule type="containsText" dxfId="440" priority="1246" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="442" priority="1246" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D253)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="439" priority="1247" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="441" priority="1247" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D253)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="438" priority="1248" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="440" priority="1248" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D253)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E253">
-    <cfRule type="cellIs" dxfId="437" priority="1240" operator="equal">
+    <cfRule type="cellIs" dxfId="439" priority="1240" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="436" priority="1241" operator="equal">
+    <cfRule type="cellIs" dxfId="438" priority="1241" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="435" priority="1242" operator="equal">
+    <cfRule type="cellIs" dxfId="437" priority="1242" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D254">
-    <cfRule type="containsText" dxfId="434" priority="1234" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="436" priority="1234" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="433" priority="1235" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="435" priority="1235" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="432" priority="1236" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="434" priority="1236" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D254">
-    <cfRule type="containsText" dxfId="431" priority="1237" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="433" priority="1237" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="430" priority="1238" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="432" priority="1238" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="429" priority="1239" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="431" priority="1239" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E254">
-    <cfRule type="cellIs" dxfId="428" priority="1231" operator="equal">
+    <cfRule type="cellIs" dxfId="430" priority="1231" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="427" priority="1232" operator="equal">
+    <cfRule type="cellIs" dxfId="429" priority="1232" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="426" priority="1233" operator="equal">
+    <cfRule type="cellIs" dxfId="428" priority="1233" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D255">
-    <cfRule type="containsText" dxfId="425" priority="1225" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="427" priority="1225" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="424" priority="1226" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="426" priority="1226" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="423" priority="1227" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="425" priority="1227" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D255">
-    <cfRule type="containsText" dxfId="422" priority="1228" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="424" priority="1228" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="421" priority="1229" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="423" priority="1229" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="420" priority="1230" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="422" priority="1230" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E255">
-    <cfRule type="cellIs" dxfId="419" priority="1222" operator="equal">
+    <cfRule type="cellIs" dxfId="421" priority="1222" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="418" priority="1223" operator="equal">
+    <cfRule type="cellIs" dxfId="420" priority="1223" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="417" priority="1224" operator="equal">
+    <cfRule type="cellIs" dxfId="419" priority="1224" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D256">
-    <cfRule type="containsText" dxfId="416" priority="1216" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="418" priority="1216" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="415" priority="1217" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="417" priority="1217" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="414" priority="1218" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="416" priority="1218" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D256">
-    <cfRule type="containsText" dxfId="413" priority="1219" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="415" priority="1219" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="412" priority="1220" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="414" priority="1220" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="411" priority="1221" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="413" priority="1221" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E256">
-    <cfRule type="cellIs" dxfId="410" priority="1213" operator="equal">
+    <cfRule type="cellIs" dxfId="412" priority="1213" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="409" priority="1214" operator="equal">
+    <cfRule type="cellIs" dxfId="411" priority="1214" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="408" priority="1215" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="1215" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D257">
-    <cfRule type="containsText" dxfId="407" priority="1207" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="409" priority="1207" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D257)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="406" priority="1208" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="408" priority="1208" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D257)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="405" priority="1209" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="407" priority="1209" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D257)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D257">
-    <cfRule type="containsText" dxfId="404" priority="1210" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="406" priority="1210" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D257)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="403" priority="1211" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="405" priority="1211" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D257)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="402" priority="1212" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="404" priority="1212" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D257)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E257">
-    <cfRule type="cellIs" dxfId="401" priority="1204" operator="equal">
+    <cfRule type="cellIs" dxfId="403" priority="1204" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="400" priority="1205" operator="equal">
+    <cfRule type="cellIs" dxfId="402" priority="1205" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="399" priority="1206" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="1206" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E74">
-    <cfRule type="cellIs" dxfId="398" priority="976" operator="equal">
+    <cfRule type="cellIs" dxfId="400" priority="976" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="397" priority="977" operator="equal">
+    <cfRule type="cellIs" dxfId="399" priority="977" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="396" priority="978" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="978" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68:D74">
-    <cfRule type="containsText" dxfId="395" priority="979" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="397" priority="979" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="394" priority="980" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="396" priority="980" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="393" priority="981" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="395" priority="981" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68:D74">
-    <cfRule type="containsText" dxfId="392" priority="982" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="394" priority="982" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="391" priority="983" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="393" priority="983" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="390" priority="984" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="392" priority="984" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75:D78">
-    <cfRule type="containsText" dxfId="389" priority="754" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="391" priority="754" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="388" priority="755" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="390" priority="755" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="387" priority="756" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="389" priority="756" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75:D78">
-    <cfRule type="containsText" dxfId="386" priority="757" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="388" priority="757" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="385" priority="758" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="387" priority="758" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="384" priority="759" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="386" priority="759" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="containsText" dxfId="383" priority="745" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="385" priority="745" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="382" priority="746" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="384" priority="746" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="381" priority="747" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="383" priority="747" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="containsText" dxfId="380" priority="748" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="382" priority="748" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="379" priority="749" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="381" priority="749" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="378" priority="750" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="380" priority="750" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D258">
-    <cfRule type="containsText" dxfId="377" priority="739" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="379" priority="739" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D258)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="376" priority="740" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="378" priority="740" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D258)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="375" priority="741" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="377" priority="741" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D258">
-    <cfRule type="containsText" dxfId="374" priority="742" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="376" priority="742" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D258)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="373" priority="743" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="375" priority="743" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D258)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="372" priority="744" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="374" priority="744" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E258">
-    <cfRule type="cellIs" dxfId="371" priority="736" operator="equal">
+    <cfRule type="cellIs" dxfId="373" priority="736" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="370" priority="737" operator="equal">
+    <cfRule type="cellIs" dxfId="372" priority="737" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="369" priority="738" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="738" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D259">
-    <cfRule type="containsText" dxfId="368" priority="730" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="370" priority="730" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D259)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="367" priority="731" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="369" priority="731" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D259)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="366" priority="732" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="368" priority="732" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D259)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D259">
-    <cfRule type="containsText" dxfId="365" priority="733" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="367" priority="733" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D259)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="364" priority="734" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="366" priority="734" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D259)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="363" priority="735" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="365" priority="735" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D259)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E259">
-    <cfRule type="cellIs" dxfId="362" priority="727" operator="equal">
+    <cfRule type="cellIs" dxfId="364" priority="727" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="361" priority="728" operator="equal">
+    <cfRule type="cellIs" dxfId="363" priority="728" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="360" priority="729" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="729" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D137:D141 D143">
-    <cfRule type="containsText" dxfId="359" priority="610" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="361" priority="610" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D137)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="358" priority="611" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="360" priority="611" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D137)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="612" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="359" priority="612" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D137)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132:E133">
-    <cfRule type="cellIs" dxfId="356" priority="604" operator="equal">
+    <cfRule type="cellIs" dxfId="358" priority="604" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="355" priority="605" operator="equal">
+    <cfRule type="cellIs" dxfId="357" priority="605" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="354" priority="606" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="606" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D132:D133">
-    <cfRule type="containsText" dxfId="353" priority="607" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="355" priority="607" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D132)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="352" priority="608" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="354" priority="608" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D132)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="351" priority="609" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="353" priority="609" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E135">
-    <cfRule type="cellIs" dxfId="350" priority="592" operator="equal">
+    <cfRule type="cellIs" dxfId="352" priority="592" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="349" priority="593" operator="equal">
+    <cfRule type="cellIs" dxfId="351" priority="593" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="348" priority="594" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="594" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D134:D135">
-    <cfRule type="containsText" dxfId="347" priority="598" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="349" priority="598" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D134)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="346" priority="599" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="348" priority="599" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D134)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="600" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="347" priority="600" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D134)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D134:D135">
-    <cfRule type="containsText" dxfId="344" priority="601" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="346" priority="601" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D134)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="343" priority="602" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="345" priority="602" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D134)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="603" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="344" priority="603" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D134)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="cellIs" dxfId="341" priority="595" operator="equal">
+    <cfRule type="cellIs" dxfId="343" priority="595" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="340" priority="596" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="596" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="339" priority="597" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="597" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E136">
-    <cfRule type="cellIs" dxfId="338" priority="589" operator="equal">
+    <cfRule type="cellIs" dxfId="340" priority="589" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="337" priority="590" operator="equal">
+    <cfRule type="cellIs" dxfId="339" priority="590" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="336" priority="591" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="591" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="containsText" dxfId="335" priority="583" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="337" priority="583" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D136)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="584" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="336" priority="584" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D136)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="585" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="335" priority="585" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D136)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="containsText" dxfId="332" priority="586" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="334" priority="586" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D136)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="331" priority="587" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="333" priority="587" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D136)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="588" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="332" priority="588" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D136)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E137">
-    <cfRule type="cellIs" dxfId="329" priority="580" operator="equal">
+    <cfRule type="cellIs" dxfId="331" priority="580" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="328" priority="581" operator="equal">
+    <cfRule type="cellIs" dxfId="330" priority="581" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="327" priority="582" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="582" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E138">
-    <cfRule type="cellIs" dxfId="326" priority="577" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="577" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="325" priority="578" operator="equal">
+    <cfRule type="cellIs" dxfId="327" priority="578" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="324" priority="579" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="579" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E139">
-    <cfRule type="cellIs" dxfId="323" priority="574" operator="equal">
+    <cfRule type="cellIs" dxfId="325" priority="574" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="322" priority="575" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="575" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="321" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="576" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E140:E141">
-    <cfRule type="cellIs" dxfId="320" priority="571" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="571" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="319" priority="572" operator="equal">
+    <cfRule type="cellIs" dxfId="321" priority="572" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="318" priority="573" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="573" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E143">
-    <cfRule type="cellIs" dxfId="317" priority="568" operator="equal">
+    <cfRule type="cellIs" dxfId="319" priority="568" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="316" priority="569" operator="equal">
+    <cfRule type="cellIs" dxfId="318" priority="569" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="315" priority="570" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="570" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D142">
-    <cfRule type="containsText" dxfId="314" priority="565" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="316" priority="565" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="566" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="315" priority="566" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="312" priority="567" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="314" priority="567" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E142">
-    <cfRule type="cellIs" dxfId="311" priority="562" operator="equal">
+    <cfRule type="cellIs" dxfId="313" priority="562" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="310" priority="563" operator="equal">
+    <cfRule type="cellIs" dxfId="312" priority="563" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="309" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="564" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144:D145">
-    <cfRule type="containsText" dxfId="308" priority="559" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="310" priority="559" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="307" priority="560" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="309" priority="560" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="306" priority="561" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="308" priority="561" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144">
-    <cfRule type="cellIs" dxfId="305" priority="556" operator="equal">
+    <cfRule type="cellIs" dxfId="307" priority="556" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="304" priority="557" operator="equal">
+    <cfRule type="cellIs" dxfId="306" priority="557" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="303" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="558" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145">
-    <cfRule type="cellIs" dxfId="302" priority="553" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="553" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="301" priority="554" operator="equal">
+    <cfRule type="cellIs" dxfId="303" priority="554" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="300" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="555" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D146">
-    <cfRule type="containsText" dxfId="299" priority="550" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="301" priority="550" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D146)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="298" priority="551" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="300" priority="551" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D146)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="297" priority="552" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="299" priority="552" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E146">
-    <cfRule type="cellIs" dxfId="296" priority="547" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="547" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="295" priority="548" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="548" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="294" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="549" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147:D150">
-    <cfRule type="containsText" dxfId="293" priority="544" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="295" priority="544" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D147)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="292" priority="545" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="294" priority="545" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D147)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="291" priority="546" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="293" priority="546" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D147)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E147:E231">
-    <cfRule type="cellIs" dxfId="290" priority="541" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="541" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="542" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="542" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="288" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="543" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D153">
-    <cfRule type="containsText" dxfId="287" priority="535" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="289" priority="535" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="536" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="288" priority="536" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="537" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="287" priority="537" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="containsText" dxfId="284" priority="529" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="286" priority="529" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="283" priority="530" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="285" priority="530" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="531" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="284" priority="531" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D152">
-    <cfRule type="containsText" dxfId="281" priority="523" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="283" priority="523" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="280" priority="524" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="282" priority="524" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="525" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="281" priority="525" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D156">
-    <cfRule type="containsText" dxfId="278" priority="517" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="280" priority="517" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="518" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="279" priority="518" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="276" priority="519" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="278" priority="519" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D155">
-    <cfRule type="containsText" dxfId="275" priority="511" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="277" priority="511" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="512" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="276" priority="512" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="513" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="275" priority="513" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D158">
-    <cfRule type="containsText" dxfId="272" priority="505" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="274" priority="505" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="271" priority="506" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="273" priority="506" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="507" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="272" priority="507" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D157">
-    <cfRule type="containsText" dxfId="269" priority="499" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="271" priority="499" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="268" priority="500" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="270" priority="500" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="267" priority="501" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="269" priority="501" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159:D161">
-    <cfRule type="containsText" dxfId="266" priority="493" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="268" priority="493" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="494" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="267" priority="494" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="264" priority="495" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="266" priority="495" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162:D163">
-    <cfRule type="containsText" dxfId="263" priority="481" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="265" priority="481" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="482" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="264" priority="482" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="483" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="263" priority="483" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164">
-    <cfRule type="containsText" dxfId="260" priority="472" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="262" priority="472" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="473" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="261" priority="473" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="474" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="260" priority="474" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D165">
-    <cfRule type="containsText" dxfId="257" priority="466" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="259" priority="466" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="256" priority="467" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="258" priority="467" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="255" priority="468" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="257" priority="468" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="containsText" dxfId="254" priority="460" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="256" priority="460" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="461" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="255" priority="461" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="252" priority="462" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="254" priority="462" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D167">
-    <cfRule type="containsText" dxfId="251" priority="454" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="253" priority="454" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="455" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="252" priority="455" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="456" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="251" priority="456" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="containsText" dxfId="248" priority="448" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="250" priority="448" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="247" priority="449" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="249" priority="449" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="450" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="248" priority="450" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D169">
-    <cfRule type="containsText" dxfId="245" priority="442" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="247" priority="442" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D169)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="443" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="246" priority="443" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D169)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="243" priority="444" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="245" priority="444" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="containsText" dxfId="242" priority="436" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="244" priority="436" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D170)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="437" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="243" priority="437" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D170)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="438" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="242" priority="438" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D171">
-    <cfRule type="containsText" dxfId="239" priority="430" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="241" priority="430" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D171)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="431" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="240" priority="431" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D171)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="432" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="239" priority="432" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D171)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="containsText" dxfId="236" priority="424" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="238" priority="424" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D172)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="235" priority="425" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="237" priority="425" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D172)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="426" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="236" priority="426" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D173">
-    <cfRule type="containsText" dxfId="233" priority="418" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="235" priority="418" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D173)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="419" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="234" priority="419" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D173)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="231" priority="420" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="233" priority="420" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D173)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D174">
-    <cfRule type="containsText" dxfId="230" priority="412" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="232" priority="412" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D174)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="413" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="231" priority="413" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D174)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="414" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="230" priority="414" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D174)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175:D176">
-    <cfRule type="containsText" dxfId="227" priority="406" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="229" priority="406" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D175)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="407" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="228" priority="407" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D175)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="408" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="227" priority="408" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D175)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D177">
-    <cfRule type="containsText" dxfId="224" priority="397" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="226" priority="397" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D177)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="223" priority="398" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="225" priority="398" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D177)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="399" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="224" priority="399" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D177)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D178">
-    <cfRule type="containsText" dxfId="221" priority="391" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="223" priority="391" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D178)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="392" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="222" priority="392" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D178)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="393" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="221" priority="393" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D178)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="containsText" dxfId="218" priority="385" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="220" priority="385" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="386" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="219" priority="386" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="387" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="218" priority="387" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D180">
-    <cfRule type="containsText" dxfId="215" priority="379" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="217" priority="379" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="380" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="216" priority="380" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="381" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="215" priority="381" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D181">
-    <cfRule type="containsText" dxfId="212" priority="373" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="214" priority="373" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D181)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="374" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="213" priority="374" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D181)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="375" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="212" priority="375" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D181)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D182">
-    <cfRule type="containsText" dxfId="209" priority="367" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="211" priority="367" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D182)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="368" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="210" priority="368" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D182)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="369" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="209" priority="369" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D182)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="containsText" dxfId="206" priority="361" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="208" priority="361" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D183)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="362" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="207" priority="362" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D183)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="363" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="206" priority="363" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D183)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D184">
-    <cfRule type="containsText" dxfId="203" priority="355" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="205" priority="355" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="356" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="204" priority="356" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="357" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="203" priority="357" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D184)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D185">
-    <cfRule type="containsText" dxfId="200" priority="349" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="202" priority="349" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D185)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="350" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="201" priority="350" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D185)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="351" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="200" priority="351" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D185)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="containsText" dxfId="197" priority="343" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="199" priority="343" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D186)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="344" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="198" priority="344" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D186)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="345" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="197" priority="345" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D186)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D188">
-    <cfRule type="containsText" dxfId="194" priority="337" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="196" priority="337" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D188)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="338" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="195" priority="338" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D188)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="339" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="194" priority="339" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D188)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189">
-    <cfRule type="containsText" dxfId="191" priority="331" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="193" priority="331" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="332" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="192" priority="332" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="333" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="191" priority="333" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D189)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D187">
-    <cfRule type="containsText" dxfId="188" priority="325" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="190" priority="325" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="326" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="189" priority="326" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="327" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="188" priority="327" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D187)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D190">
-    <cfRule type="containsText" dxfId="185" priority="319" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="187" priority="319" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D190)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="320" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="186" priority="320" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D190)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="321" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="185" priority="321" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D190)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="containsText" dxfId="182" priority="313" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="184" priority="313" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D191)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="314" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="183" priority="314" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D191)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="315" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="182" priority="315" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D191)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D192">
-    <cfRule type="containsText" dxfId="179" priority="307" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="181" priority="307" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D192)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="308" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="180" priority="308" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D192)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="309" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="179" priority="309" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D192)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D194">
-    <cfRule type="containsText" dxfId="176" priority="301" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="178" priority="301" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D194)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="302" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="177" priority="302" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D194)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="303" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="176" priority="303" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D193">
-    <cfRule type="containsText" dxfId="173" priority="295" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="175" priority="295" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D193)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="296" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="174" priority="296" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D193)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="297" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="173" priority="297" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D193)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="containsText" dxfId="170" priority="289" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="172" priority="289" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D195)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="290" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="171" priority="290" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D195)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="291" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="170" priority="291" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D195)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D196:D207">
-    <cfRule type="containsText" dxfId="167" priority="283" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="169" priority="283" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D196)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="284" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="168" priority="284" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D196)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="285" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="167" priority="285" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D196)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D208:D218">
-    <cfRule type="containsText" dxfId="164" priority="244" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="166" priority="244" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="245" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="165" priority="245" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="246" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="164" priority="246" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D208)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D260">
-    <cfRule type="containsText" dxfId="161" priority="205" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="163" priority="205" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D260)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="206" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="162" priority="206" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D260)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="207" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="161" priority="207" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D260">
-    <cfRule type="containsText" dxfId="158" priority="208" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="160" priority="208" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D260)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="209" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="159" priority="209" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D260)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="210" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="158" priority="210" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E260">
-    <cfRule type="cellIs" dxfId="155" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="202" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="203" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="204" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D261">
-    <cfRule type="containsText" dxfId="152" priority="196" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="154" priority="196" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D261)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="197" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="153" priority="197" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D261)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="198" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="152" priority="198" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D261">
-    <cfRule type="containsText" dxfId="149" priority="199" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="151" priority="199" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D261)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="200" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="150" priority="200" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D261)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="201" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="149" priority="201" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E261">
-    <cfRule type="cellIs" dxfId="146" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="193" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="194" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="195" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D262">
-    <cfRule type="containsText" dxfId="143" priority="187" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="145" priority="187" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D262)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="188" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="144" priority="188" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D262)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="189" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="143" priority="189" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D262)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D262">
-    <cfRule type="containsText" dxfId="140" priority="190" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="142" priority="190" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D262)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="191" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="141" priority="191" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D262)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="192" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="140" priority="192" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D262)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E262">
-    <cfRule type="cellIs" dxfId="137" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="184" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="185" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="186" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E103">
-    <cfRule type="cellIs" dxfId="134" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="178" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="179" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="180" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="containsText" dxfId="131" priority="181" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="133" priority="181" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="182" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="132" priority="182" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="183" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="131" priority="183" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E104">
-    <cfRule type="cellIs" dxfId="128" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="172" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="173" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="174" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D104">
-    <cfRule type="containsText" dxfId="125" priority="175" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="127" priority="175" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="176" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="126" priority="176" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="177" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="125" priority="177" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="122" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="166" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="167" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="168" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="containsText" dxfId="119" priority="169" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="121" priority="169" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="170" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="120" priority="170" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="171" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="119" priority="171" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="116" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="160" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="161" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="162" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D107">
-    <cfRule type="containsText" dxfId="113" priority="163" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="115" priority="163" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="164" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="114" priority="164" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="165" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="113" priority="165" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="cellIs" dxfId="110" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="154" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="155" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="156" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="containsText" dxfId="107" priority="157" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="109" priority="157" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D108)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="158" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="108" priority="158" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D108)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="159" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="107" priority="159" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E110">
-    <cfRule type="cellIs" dxfId="104" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="148" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="149" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="150" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110">
-    <cfRule type="containsText" dxfId="101" priority="151" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="103" priority="151" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D110)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="152" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="102" priority="152" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D110)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="153" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="101" priority="153" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E111">
-    <cfRule type="cellIs" dxfId="98" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="142" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="143" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="144" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111">
-    <cfRule type="containsText" dxfId="95" priority="145" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="97" priority="145" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D111)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="146" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="96" priority="146" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D111)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="147" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="95" priority="147" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D111)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E112">
-    <cfRule type="cellIs" dxfId="92" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="136" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="137" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="138" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112">
-    <cfRule type="containsText" dxfId="89" priority="139" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="91" priority="139" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D112)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="140" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="90" priority="140" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D112)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="141" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="89" priority="141" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D219:D220">
-    <cfRule type="containsText" dxfId="86" priority="133" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="88" priority="133" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="134" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="87" priority="134" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="135" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="86" priority="135" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D219)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D221">
-    <cfRule type="containsText" dxfId="83" priority="124" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="85" priority="124" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D221)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="125" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="84" priority="125" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D221)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="126" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="83" priority="126" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D221)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D222:D225">
-    <cfRule type="containsText" dxfId="80" priority="118" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="82" priority="118" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="119" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="81" priority="119" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="120" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="80" priority="120" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D226">
-    <cfRule type="containsText" dxfId="77" priority="112" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="79" priority="112" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D226)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="113" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="78" priority="113" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D226)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="114" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="77" priority="114" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D227">
-    <cfRule type="containsText" dxfId="74" priority="106" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="76" priority="106" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D227)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="107" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="75" priority="107" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D227)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="108" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="74" priority="108" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D227)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D228:D231">
-    <cfRule type="containsText" dxfId="71" priority="100" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="73" priority="100" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D228)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="101" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="72" priority="101" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D228)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="102" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="71" priority="102" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109">
-    <cfRule type="cellIs" dxfId="68" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="74" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="75" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D109">
-    <cfRule type="containsText" dxfId="65" priority="76" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="67" priority="76" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="77" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="66" priority="77" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="78" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="65" priority="78" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E113">
-    <cfRule type="cellIs" dxfId="62" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="67" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="68" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="69" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D113">
-    <cfRule type="containsText" dxfId="59" priority="70" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="61" priority="70" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="71" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="60" priority="71" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="72" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E114">
-    <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="61" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="62" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="63" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="containsText" dxfId="53" priority="64" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="55" priority="64" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D114)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="65" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="54" priority="65" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D114)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="66" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="53" priority="66" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D114)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E115">
-    <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="57" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D115">
-    <cfRule type="containsText" dxfId="47" priority="58" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="49" priority="58" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D115)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="59" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D115)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="60" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E116">
-    <cfRule type="cellIs" dxfId="44" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="49" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="50" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="51" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D116">
-    <cfRule type="containsText" dxfId="41" priority="52" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="43" priority="52" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="53" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="42" priority="53" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="54" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="41" priority="54" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D116)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E117">
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="44" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D117">
-    <cfRule type="containsText" dxfId="35" priority="46" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="37" priority="46" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D117)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="36" priority="47" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D117)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="48" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118">
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D118">
-    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="31" priority="40" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D118)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="41" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D118)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="42" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D118)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E119">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="32" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="33" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D119">
-    <cfRule type="containsText" dxfId="23" priority="34" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="25" priority="34" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D119)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="35" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D119)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="36" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E120">
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D120">
-    <cfRule type="containsText" dxfId="17" priority="28" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="19" priority="28" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D120)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="29" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D120)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="30" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="17" priority="30" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E94">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D105">
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Skip:">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",D154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",D154)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16962,13 +16970,13 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
         <v>305</v>
-      </c>
-      <c r="D3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E3" t="s">
-        <v>306</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -16985,19 +16993,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>241</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>242</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>307</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>308</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
@@ -17006,10 +17014,10 @@
         <v>22</v>
       </c>
       <c r="H4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I4" t="s">
         <v>243</v>
-      </c>
-      <c r="I4" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added HSR and DSQ testcase
Signed-off-by: Ravi Kumar
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A37789-9F93-4E84-B093-01108076F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD6FF21-2FEE-4952-82B5-E4F8EF877966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -16858,7 +16858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A408" workbookViewId="0">
+    <sheetView topLeftCell="A408" workbookViewId="0">
       <selection activeCell="C422" sqref="C422:C423"/>
     </sheetView>
   </sheetViews>
@@ -29616,9 +29616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
executed tc01 round 4
Signed-off-by: sourabhnavatargroup <sourabhnavatargroup>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satya Roopa\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{60410B03-200B-43FB-95E7-07154F32B4F1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{690DA6BD-AA6D-4AE9-BECF-F9C88709472A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" r:id="rId1" sheetId="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8714" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7686" uniqueCount="1284">
   <si>
     <t>Module_Name</t>
   </si>
@@ -3744,75 +3744,6 @@
     <t>AcuityTaskCallAndEvent</t>
   </si>
   <si>
-    <t>navatariptesting+31820@gmail.com</t>
-  </si>
-  <si>
-    <t>User32952</t>
-  </si>
-  <si>
-    <t>navatariptesting+3232@gmail.com</t>
-  </si>
-  <si>
-    <t>User19558</t>
-  </si>
-  <si>
-    <t>navatariptesting+3009@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+98724@gmail.com</t>
-  </si>
-  <si>
-    <t>User55588</t>
-  </si>
-  <si>
-    <t>navatariptesting+87158@gmail.com</t>
-  </si>
-  <si>
-    <t>User48486</t>
-  </si>
-  <si>
-    <t>navatariptesting+55286@gmail.com</t>
-  </si>
-  <si>
-    <t>User53790</t>
-  </si>
-  <si>
-    <t>navatariptesting+29209@gmail.com</t>
-  </si>
-  <si>
-    <t>User95904</t>
-  </si>
-  <si>
-    <t>navatariptesting+25528@gmail.com</t>
-  </si>
-  <si>
-    <t>User17576</t>
-  </si>
-  <si>
-    <t>navatariptesting+43855@gmail.com</t>
-  </si>
-  <si>
-    <t>User14204</t>
-  </si>
-  <si>
-    <t>navatariptesting+43770@gmail.com</t>
-  </si>
-  <si>
-    <t>User99533</t>
-  </si>
-  <si>
-    <t>navatariptesting+16988@gmail.com</t>
-  </si>
-  <si>
-    <t>User44823</t>
-  </si>
-  <si>
-    <t>Connection</t>
-  </si>
-  <si>
-    <t>PE User 3</t>
-  </si>
-  <si>
     <t>navatariptesting+75817@gmail.com</t>
   </si>
   <si>
@@ -3879,9 +3810,6 @@
     <t>ATCETc010_VerifyUIOfAcuityTabOnDealRecord</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>ATCETc011_VerifyUIOfAcuityTabOnFundRecord</t>
   </si>
   <si>
@@ -3889,24 +3817,104 @@
   </si>
   <si>
     <t>ATCETc013_VerifyUIOfAcuityTabOnThemeRecord</t>
-  </si>
-  <si>
-    <t>Fail: The following asserts failed:
-	Not able to open PE Theme 1 reocrd 	Screenshot Name: ATCETc013_VerifyUIOfAcuityTabOnThemeRecord2023_02_15_07_45_30.png	 did not expect to find [true] but found [false]</t>
-  </si>
-  <si>
-    <t>Fail: The following asserts failed:
-	Not able to open PE Theme 1 reocrd 	Screenshot Name: ATCETc013_VerifyUIOfAcuityTabOnThemeRecord2023_02_15_07_49_09.png	 did not expect to find [true] but found [false]</t>
-  </si>
-  <si>
-    <t>Fail: The following asserts failed:
-	Section headers and Tooltip are not verified on acuity tab. [Expected Header Name : Interactions is not matched, Expected tooltip of header Name : Interactions is not matched] 	Screenshot Name: ATCETc013_VerifyUIOfAcuityTabOnThemeRecord2023_02_15_07_52_27.png	 did not expect to find [true] but found [false],
-	The header name and message are not verified on Interaction and Connection Section. [No items to display. message is not verified on Interaction section] 	Screenshot Name: ATCETc013_VerifyUIOfAcuityTabOnThemeRecord2023_02_15_07_52_28.png	 did not expect to find [true] but found [false]</t>
   </si>
   <si>
     <t>Fail: The following asserts failed:
 	Section headers and Tooltip are not verified on acuity tab. [Expected Header Name : Interactions is not matched, Expected tooltip of header Name : Interactions is not matched] 	Screenshot Name: ATCETc013_VerifyUIOfAcuityTabOnThemeRecord2023_02_15_07_57_24.png	 did not expect to find [true] but found [false],
 	The header name and message are not verified on Interaction and Connection Section. [No items to display. message is not verified on Interaction section] 	Screenshot Name: ATCETc013_VerifyUIOfAcuityTabOnThemeRecord2023_02_15_07_57_25.png	 did not expect to find [true] but found [false]</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Fail: unknown error: net::ERR_NAME_NOT_RESOLVED
+  (Session info: chrome=109.0.5414.120)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:25:53'
+System info: host: 'DESK0065', ip: '192.168.1.253', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '17.0.5'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 109.0.5414.120, chrome: {chromedriverVersion: 109.0.5414.74 (e7c5703604da..., userDataDir: C:\Users\SATYAR~1\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54659}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: 029898b863e04e74e71b50d58885b0b6</t>
+  </si>
+  <si>
+    <t>Fail: unknown error: net::ERR_NAME_NOT_RESOLVED
+  (Session info: chrome=109.0.5414.120)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:25:53'
+System info: host: 'DESK0065', ip: '192.168.1.253', os.name: 'Windows 8.1', os.arch: 'amd64', os.version: '6.3', java.version: '17.0.5'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 109.0.5414.120, chrome: {chromedriverVersion: 109.0.5414.74 (e7c5703604da..., userDataDir: C:\Users\SATYAR~1\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:54835}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: acce7d540e649e5c1fece90dcfc932b1</t>
+  </si>
+  <si>
+    <t>navatariptesting+77024@gmail.com</t>
+  </si>
+  <si>
+    <t>User48622</t>
+  </si>
+  <si>
+    <t>navatariptesting+31917@gmail.com</t>
+  </si>
+  <si>
+    <t>User10291</t>
+  </si>
+  <si>
+    <t>navatariptesting+25741@gmail.com</t>
+  </si>
+  <si>
+    <t>User51042</t>
+  </si>
+  <si>
+    <t>navatariptesting+73170@gmail.com</t>
+  </si>
+  <si>
+    <t>User98521</t>
+  </si>
+  <si>
+    <t>navatariptesting+47223@gmail.com</t>
+  </si>
+  <si>
+    <t>User75371</t>
+  </si>
+  <si>
+    <t>navatariptesting+97281@gmail.com</t>
+  </si>
+  <si>
+    <t>User68034</t>
+  </si>
+  <si>
+    <t>navatariptesting+91330@gmail.com</t>
+  </si>
+  <si>
+    <t>User18718</t>
+  </si>
+  <si>
+    <t>navatariptesting+22182@gmail.com</t>
+  </si>
+  <si>
+    <t>User64764</t>
+  </si>
+  <si>
+    <t>navatariptesting+11013@gmail.com</t>
+  </si>
+  <si>
+    <t>User10513</t>
+  </si>
+  <si>
+    <t>navatariptesting+22157@gmail.com</t>
+  </si>
+  <si>
+    <t>User76273</t>
+  </si>
+  <si>
+    <t>navatariptesting+49622@gmail.com</t>
+  </si>
+  <si>
+    <t>User19337</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -3914,7 +3922,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3986,6 +3994,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -21411,7 +21425,7 @@
   <dimension ref="H1:J25"/>
   <sheetViews>
     <sheetView topLeftCell="C5" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21563,7 +21577,7 @@
         <v>971</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>7</v>
+        <v>974</v>
       </c>
     </row>
     <row ht="15.75" r="19" spans="8:9" thickBot="1" x14ac:dyDescent="0.3">
@@ -21619,7 +21633,7 @@
         <v>1230</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>974</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -21858,8 +21872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1052"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1038" workbookViewId="0">
-      <selection activeCell="A1049" sqref="A1049"/>
+    <sheetView topLeftCell="A941" workbookViewId="0">
+      <selection activeCell="C946" sqref="C946"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34776,7 +34790,7 @@
       </c>
       <c r="B818" s="7"/>
       <c r="C818" s="3" t="s">
-        <v>974</v>
+        <v>7</v>
       </c>
       <c r="D818" t="s">
         <v>8</v>
@@ -36036,10 +36050,10 @@
       </c>
       <c r="B902" s="7"/>
       <c r="C902" s="3" t="s">
-        <v>974</v>
+        <v>7</v>
       </c>
       <c r="D902" t="s">
-        <v>1228</v>
+        <v>8</v>
       </c>
       <c r="E902" s="22" t="s">
         <v>9</v>
@@ -36606,10 +36620,10 @@
       </c>
       <c r="B940" s="7"/>
       <c r="C940" s="3" t="s">
-        <v>974</v>
+        <v>7</v>
       </c>
       <c r="D940" t="s">
-        <v>1228</v>
+        <v>8</v>
       </c>
       <c r="E940" s="22" t="s">
         <v>9</v>
@@ -36696,10 +36710,10 @@
       </c>
       <c r="B946" s="8"/>
       <c r="C946" s="3" t="s">
-        <v>7</v>
+        <v>974</v>
       </c>
       <c r="D946" t="s">
-        <v>8</v>
+        <v>1283</v>
       </c>
       <c r="E946" s="22" t="s">
         <v>9</v>
@@ -38102,7 +38116,7 @@
     </row>
     <row ht="15.75" r="1040" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1040" s="7" t="s">
-        <v>1266</v>
+        <v>1243</v>
       </c>
       <c r="B1040" s="7"/>
       <c r="C1040" s="3" t="s">
@@ -38117,7 +38131,7 @@
     </row>
     <row ht="15.75" r="1041" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1041" s="7" t="s">
-        <v>1267</v>
+        <v>1244</v>
       </c>
       <c r="B1041" s="7"/>
       <c r="C1041" s="3" t="s">
@@ -38132,7 +38146,7 @@
     </row>
     <row ht="15.75" r="1042" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1042" s="7" t="s">
-        <v>1268</v>
+        <v>1245</v>
       </c>
       <c r="B1042" s="7"/>
       <c r="C1042" s="3" t="s">
@@ -38147,7 +38161,7 @@
     </row>
     <row ht="15.75" r="1043" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1043" s="7" t="s">
-        <v>1269</v>
+        <v>1246</v>
       </c>
       <c r="B1043" s="7"/>
       <c r="C1043" s="3" t="s">
@@ -38162,7 +38176,7 @@
     </row>
     <row ht="15.75" r="1044" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1044" s="7" t="s">
-        <v>1270</v>
+        <v>1247</v>
       </c>
       <c r="B1044" s="7"/>
       <c r="C1044" s="3" t="s">
@@ -38177,7 +38191,7 @@
     </row>
     <row ht="15.75" r="1045" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1045" s="7" t="s">
-        <v>1271</v>
+        <v>1248</v>
       </c>
       <c r="B1045" s="7"/>
       <c r="C1045" s="3" t="s">
@@ -38192,7 +38206,7 @@
     </row>
     <row ht="15.75" r="1046" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1046" s="7" t="s">
-        <v>1272</v>
+        <v>1249</v>
       </c>
       <c r="B1046" s="7"/>
       <c r="C1046" s="3" t="s">
@@ -38207,7 +38221,7 @@
     </row>
     <row ht="15.75" r="1047" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1047" s="7" t="s">
-        <v>1273</v>
+        <v>1250</v>
       </c>
       <c r="B1047" s="7"/>
       <c r="C1047" s="3" t="s">
@@ -38222,7 +38236,7 @@
     </row>
     <row ht="15.75" r="1048" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1048" s="7" t="s">
-        <v>1274</v>
+        <v>1251</v>
       </c>
       <c r="B1048" s="7"/>
       <c r="C1048" s="3" t="s">
@@ -38237,7 +38251,7 @@
     </row>
     <row ht="15.75" r="1049" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1049" s="7" t="s">
-        <v>1275</v>
+        <v>1252</v>
       </c>
       <c r="B1049" s="7"/>
       <c r="C1049" s="3" t="s">
@@ -38252,7 +38266,7 @@
     </row>
     <row ht="15.75" r="1050" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1050" s="7" t="s">
-        <v>1277</v>
+        <v>1253</v>
       </c>
       <c r="B1050" s="7"/>
       <c r="C1050" s="3" t="s">
@@ -38267,7 +38281,7 @@
     </row>
     <row ht="15.75" r="1051" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1051" s="7" t="s">
-        <v>1278</v>
+        <v>1254</v>
       </c>
       <c r="B1051" s="7"/>
       <c r="C1051" s="3" t="s">
@@ -38282,14 +38296,14 @@
     </row>
     <row ht="15.75" r="1052" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1052" s="7" t="s">
-        <v>1279</v>
+        <v>1255</v>
       </c>
       <c r="B1052" s="7"/>
       <c r="C1052" s="3" t="s">
-        <v>974</v>
+        <v>7</v>
       </c>
       <c r="D1052" t="s">
-        <v>1283</v>
+        <v>8</v>
       </c>
       <c r="E1052" s="22" t="s">
         <v>9</v>
@@ -44010,7 +44024,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C2:C894" type="list" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C2:C1052" type="list" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -44132,8 +44146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44333,10 +44347,10 @@
         <v>939</v>
       </c>
       <c r="D8" t="s">
-        <v>1232</v>
+        <v>1262</v>
       </c>
       <c r="E8" t="s">
-        <v>1231</v>
+        <v>1261</v>
       </c>
       <c r="F8" t="s">
         <v>27</v>
@@ -44359,10 +44373,10 @@
         <v>942</v>
       </c>
       <c r="D9" t="s">
-        <v>1234</v>
+        <v>1264</v>
       </c>
       <c r="E9" t="s">
-        <v>1233</v>
+        <v>1263</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -44381,20 +44395,20 @@
       <c r="B10" s="10" t="s">
         <v>944</v>
       </c>
-      <c r="C10" t="s">
-        <v>1252</v>
+      <c r="C10" s="36" t="s">
+        <v>1257</v>
       </c>
       <c r="D10" t="s">
-        <v>1253</v>
+        <v>1266</v>
       </c>
       <c r="E10" t="s">
-        <v>1235</v>
+        <v>1265</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>954</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>955</v>
       </c>
       <c r="J10" t="s">
         <v>978</v>
@@ -44411,16 +44425,16 @@
         <v>947</v>
       </c>
       <c r="D11" t="s">
-        <v>1237</v>
+        <v>1268</v>
       </c>
       <c r="E11" t="s">
-        <v>1236</v>
+        <v>1267</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>954</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>955</v>
       </c>
       <c r="J11" t="s">
         <v>979</v>
@@ -44437,10 +44451,10 @@
         <v>950</v>
       </c>
       <c r="D12" t="s">
-        <v>1239</v>
+        <v>1270</v>
       </c>
       <c r="E12" t="s">
-        <v>1238</v>
+        <v>1269</v>
       </c>
       <c r="F12" t="s">
         <v>930</v>
@@ -44463,10 +44477,10 @@
         <v>953</v>
       </c>
       <c r="D13" t="s">
-        <v>1241</v>
+        <v>1272</v>
       </c>
       <c r="E13" t="s">
-        <v>1240</v>
+        <v>1271</v>
       </c>
       <c r="F13" t="s">
         <v>954</v>
@@ -44489,10 +44503,10 @@
         <v>958</v>
       </c>
       <c r="D14" t="s">
-        <v>1243</v>
+        <v>1274</v>
       </c>
       <c r="E14" t="s">
-        <v>1242</v>
+        <v>1273</v>
       </c>
       <c r="F14" t="s">
         <v>954</v>
@@ -44515,10 +44529,10 @@
         <v>961</v>
       </c>
       <c r="D15" t="s">
-        <v>1245</v>
+        <v>1276</v>
       </c>
       <c r="E15" t="s">
-        <v>1244</v>
+        <v>1275</v>
       </c>
       <c r="F15" t="s">
         <v>954</v>
@@ -44541,10 +44555,10 @@
         <v>964</v>
       </c>
       <c r="D16" t="s">
-        <v>1247</v>
+        <v>1278</v>
       </c>
       <c r="E16" t="s">
-        <v>1246</v>
+        <v>1277</v>
       </c>
       <c r="F16" t="s">
         <v>954</v>
@@ -44567,10 +44581,10 @@
         <v>967</v>
       </c>
       <c r="D17" t="s">
-        <v>1249</v>
+        <v>1280</v>
       </c>
       <c r="E17" t="s">
-        <v>1248</v>
+        <v>1279</v>
       </c>
       <c r="F17" t="s">
         <v>954</v>
@@ -44593,10 +44607,10 @@
         <v>970</v>
       </c>
       <c r="D18" t="s">
-        <v>1251</v>
+        <v>1282</v>
       </c>
       <c r="E18" t="s">
-        <v>1250</v>
+        <v>1281</v>
       </c>
       <c r="F18" t="s">
         <v>954</v>
@@ -44676,10 +44690,10 @@
         <v>300</v>
       </c>
       <c r="D25" t="s">
-        <v>1255</v>
+        <v>1232</v>
       </c>
       <c r="E25" t="s">
-        <v>1254</v>
+        <v>1231</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
@@ -44699,10 +44713,10 @@
         <v>124</v>
       </c>
       <c r="D26" t="s">
-        <v>1257</v>
+        <v>1234</v>
       </c>
       <c r="E26" t="s">
-        <v>1256</v>
+        <v>1233</v>
       </c>
       <c r="F26" t="s">
         <v>27</v>
@@ -44722,10 +44736,10 @@
         <v>406</v>
       </c>
       <c r="D27" t="s">
-        <v>1259</v>
+        <v>1236</v>
       </c>
       <c r="E27" t="s">
-        <v>1258</v>
+        <v>1235</v>
       </c>
       <c r="F27" t="s">
         <v>954</v>
@@ -44745,10 +44759,10 @@
         <v>926</v>
       </c>
       <c r="D28" t="s">
-        <v>1261</v>
+        <v>1238</v>
       </c>
       <c r="E28" t="s">
-        <v>1260</v>
+        <v>1237</v>
       </c>
       <c r="F28" t="s">
         <v>954</v>
@@ -44768,10 +44782,10 @@
         <v>1190</v>
       </c>
       <c r="D29" t="s">
-        <v>1263</v>
+        <v>1240</v>
       </c>
       <c r="E29" t="s">
-        <v>1262</v>
+        <v>1239</v>
       </c>
       <c r="F29" t="s">
         <v>954</v>
@@ -44791,10 +44805,10 @@
         <v>1192</v>
       </c>
       <c r="D30" t="s">
-        <v>1265</v>
+        <v>1242</v>
       </c>
       <c r="E30" t="s">
-        <v>1264</v>
+        <v>1241</v>
       </c>
       <c r="F30" t="s">
         <v>954</v>
@@ -44804,6 +44818,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="E23" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
     <hyperlink r:id="rId2" ref="E24" xr:uid="{00000000-0004-0000-0300-000005000000}"/>

</xml_diff>

<commit_message>
update testcase sheet and delete unused file
Signed-off-by: ravi kumar <rkumar1@navatargroup.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Kumar\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412A72DD-73D7-4EA5-AC3A-E12E7F0946B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAE8520-96EC-419D-B975-09781F46CCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5328" uniqueCount="1487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5343" uniqueCount="1486">
   <si>
     <t>Module_Name</t>
   </si>
@@ -2964,9 +2964,6 @@
   </si>
   <si>
     <t>AcuityMeetingNotesNotificationReminder</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>User_Title</t>
@@ -22724,7 +22721,7 @@
   <dimension ref="A1:AMK27"/>
   <sheetViews>
     <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22876,7 +22873,7 @@
         <v>971</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>974</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="8:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -22897,7 +22894,7 @@
     </row>
     <row r="21" spans="8:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H21" s="2" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>7</v>
@@ -22913,7 +22910,7 @@
     </row>
     <row r="23" spans="8:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H23" s="2" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>7</v>
@@ -22921,7 +22918,7 @@
     </row>
     <row r="24" spans="8:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H24" s="2" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>7</v>
@@ -22929,7 +22926,7 @@
     </row>
     <row r="25" spans="8:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H25" s="2" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>7</v>
@@ -22945,7 +22942,7 @@
     </row>
     <row r="27" spans="8:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H27" s="2" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>7</v>
@@ -23207,8 +23204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1256"/>
   <sheetViews>
-    <sheetView topLeftCell="A943" workbookViewId="0">
-      <selection activeCell="A960" sqref="A960"/>
+    <sheetView tabSelected="1" topLeftCell="A1240" workbookViewId="0">
+      <selection activeCell="C1249" sqref="C1249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36016,7 +36013,7 @@
     </row>
     <row r="811" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A811" s="7" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B811" s="7"/>
       <c r="C811" s="3" t="s">
@@ -36031,7 +36028,7 @@
     </row>
     <row r="812" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A812" s="7" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B812" s="7"/>
       <c r="C812" s="3" t="s">
@@ -36046,7 +36043,7 @@
     </row>
     <row r="813" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A813" s="7" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B813" s="7"/>
       <c r="C813" s="3" t="s">
@@ -36061,7 +36058,7 @@
     </row>
     <row r="814" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A814" s="7" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B814" s="7"/>
       <c r="C814" s="3" t="s">
@@ -36076,7 +36073,7 @@
     </row>
     <row r="815" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A815" s="7" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B815" s="7"/>
       <c r="C815" s="3" t="s">
@@ -36091,7 +36088,7 @@
     </row>
     <row r="816" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A816" s="7" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B816" s="7"/>
       <c r="C816" s="3" t="s">
@@ -36106,7 +36103,7 @@
     </row>
     <row r="817" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A817" s="7" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B817" s="7"/>
       <c r="C817" s="3" t="s">
@@ -36121,7 +36118,7 @@
     </row>
     <row r="818" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A818" s="7" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B818" s="7"/>
       <c r="C818" s="3" t="s">
@@ -36136,7 +36133,7 @@
     </row>
     <row r="819" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A819" s="7" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B819" s="7"/>
       <c r="C819" s="3" t="s">
@@ -36151,7 +36148,7 @@
     </row>
     <row r="820" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A820" s="7" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B820" s="7"/>
       <c r="C820" s="3" t="s">
@@ -36166,7 +36163,7 @@
     </row>
     <row r="821" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A821" s="7" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B821" s="7"/>
       <c r="C821" s="3" t="s">
@@ -36181,7 +36178,7 @@
     </row>
     <row r="822" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A822" s="7" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B822" s="7"/>
       <c r="C822" s="3" t="s">
@@ -36196,7 +36193,7 @@
     </row>
     <row r="823" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A823" s="7" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B823" s="7"/>
       <c r="C823" s="3" t="s">
@@ -36211,7 +36208,7 @@
     </row>
     <row r="824" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A824" s="7" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B824" s="7"/>
       <c r="C824" s="3" t="s">
@@ -36226,7 +36223,7 @@
     </row>
     <row r="825" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A825" s="7" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B825" s="7"/>
       <c r="C825" s="3" t="s">
@@ -36241,7 +36238,7 @@
     </row>
     <row r="826" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A826" s="7" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B826" s="7"/>
       <c r="C826" s="3" t="s">
@@ -36256,7 +36253,7 @@
     </row>
     <row r="827" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A827" s="7" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B827" s="7"/>
       <c r="C827" s="3" t="s">
@@ -36271,7 +36268,7 @@
     </row>
     <row r="828" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A828" s="7" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B828" s="7"/>
       <c r="C828" s="3" t="s">
@@ -36286,7 +36283,7 @@
     </row>
     <row r="829" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A829" s="7" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B829" s="7"/>
       <c r="C829" s="3" t="s">
@@ -36301,7 +36298,7 @@
     </row>
     <row r="830" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A830" s="7" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B830" s="7"/>
       <c r="C830" s="3" t="s">
@@ -36316,7 +36313,7 @@
     </row>
     <row r="831" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A831" s="7" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B831" s="7"/>
       <c r="C831" s="3" t="s">
@@ -36331,7 +36328,7 @@
     </row>
     <row r="832" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A832" s="7" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B832" s="7"/>
       <c r="C832" s="3" t="s">
@@ -36346,7 +36343,7 @@
     </row>
     <row r="833" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A833" s="7" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B833" s="7"/>
       <c r="C833" s="3" t="s">
@@ -36361,7 +36358,7 @@
     </row>
     <row r="834" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A834" s="7" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B834" s="7"/>
       <c r="C834" s="3" t="s">
@@ -36376,7 +36373,7 @@
     </row>
     <row r="835" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A835" s="7" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B835" s="7"/>
       <c r="C835" s="3" t="s">
@@ -36391,7 +36388,7 @@
     </row>
     <row r="836" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A836" s="7" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B836" s="7"/>
       <c r="C836" s="3" t="s">
@@ -36406,7 +36403,7 @@
     </row>
     <row r="837" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A837" s="7" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B837" s="7"/>
       <c r="C837" s="3" t="s">
@@ -36421,7 +36418,7 @@
     </row>
     <row r="838" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A838" s="7" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B838" s="7"/>
       <c r="C838" s="3" t="s">
@@ -36436,7 +36433,7 @@
     </row>
     <row r="839" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A839" s="7" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B839" s="7"/>
       <c r="C839" s="3" t="s">
@@ -36451,7 +36448,7 @@
     </row>
     <row r="840" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A840" s="7" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B840" s="7"/>
       <c r="C840" s="3" t="s">
@@ -36466,7 +36463,7 @@
     </row>
     <row r="841" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A841" s="7" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B841" s="7"/>
       <c r="C841" s="3" t="s">
@@ -36481,7 +36478,7 @@
     </row>
     <row r="842" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A842" s="7" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B842" s="7"/>
       <c r="C842" s="3" t="s">
@@ -36496,7 +36493,7 @@
     </row>
     <row r="843" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A843" s="7" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B843" s="7"/>
       <c r="C843" s="3" t="s">
@@ -36511,7 +36508,7 @@
     </row>
     <row r="844" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A844" s="7" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B844" s="7"/>
       <c r="C844" s="3" t="s">
@@ -36526,7 +36523,7 @@
     </row>
     <row r="845" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A845" s="7" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B845" s="7"/>
       <c r="C845" s="3" t="s">
@@ -36541,7 +36538,7 @@
     </row>
     <row r="846" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A846" s="7" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B846" s="7"/>
       <c r="C846" s="3" t="s">
@@ -36556,7 +36553,7 @@
     </row>
     <row r="847" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A847" s="7" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B847" s="7"/>
       <c r="C847" s="3" t="s">
@@ -36571,7 +36568,7 @@
     </row>
     <row r="848" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A848" s="7" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B848" s="7"/>
       <c r="C848" s="3" t="s">
@@ -36586,7 +36583,7 @@
     </row>
     <row r="849" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A849" s="7" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B849" s="7"/>
       <c r="C849" s="3" t="s">
@@ -36601,7 +36598,7 @@
     </row>
     <row r="850" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A850" s="7" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B850" s="7"/>
       <c r="C850" s="3" t="s">
@@ -36616,7 +36613,7 @@
     </row>
     <row r="851" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A851" s="7" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B851" s="7"/>
       <c r="C851" s="3" t="s">
@@ -36631,7 +36628,7 @@
     </row>
     <row r="852" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A852" s="7" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B852" s="7"/>
       <c r="C852" s="3" t="s">
@@ -36646,7 +36643,7 @@
     </row>
     <row r="853" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A853" s="7" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B853" s="7"/>
       <c r="C853" s="3" t="s">
@@ -36661,7 +36658,7 @@
     </row>
     <row r="854" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A854" s="7" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B854" s="7"/>
       <c r="C854" s="3" t="s">
@@ -36676,7 +36673,7 @@
     </row>
     <row r="855" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A855" s="7" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B855" s="7"/>
       <c r="C855" s="3" t="s">
@@ -36691,7 +36688,7 @@
     </row>
     <row r="856" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A856" s="7" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B856" s="7"/>
       <c r="C856" s="3" t="s">
@@ -36706,7 +36703,7 @@
     </row>
     <row r="857" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A857" s="7" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B857" s="7"/>
       <c r="C857" s="3" t="s">
@@ -36721,7 +36718,7 @@
     </row>
     <row r="858" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A858" s="7" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B858" s="7"/>
       <c r="C858" s="3" t="s">
@@ -36736,7 +36733,7 @@
     </row>
     <row r="859" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A859" s="7" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B859" s="7"/>
       <c r="C859" s="3" t="s">
@@ -36751,7 +36748,7 @@
     </row>
     <row r="860" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A860" s="7" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B860" s="7"/>
       <c r="C860" s="3" t="s">
@@ -36766,7 +36763,7 @@
     </row>
     <row r="861" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A861" s="7" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B861" s="7"/>
       <c r="C861" s="3" t="s">
@@ -36781,7 +36778,7 @@
     </row>
     <row r="862" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A862" s="7" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B862" s="7"/>
       <c r="C862" s="3" t="s">
@@ -36796,7 +36793,7 @@
     </row>
     <row r="863" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A863" s="7" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B863" s="7"/>
       <c r="C863" s="3" t="s">
@@ -36811,7 +36808,7 @@
     </row>
     <row r="864" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A864" s="7" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B864" s="7"/>
       <c r="C864" s="3" t="s">
@@ -36826,7 +36823,7 @@
     </row>
     <row r="865" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A865" s="7" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B865" s="7"/>
       <c r="C865" s="3" t="s">
@@ -36841,7 +36838,7 @@
     </row>
     <row r="866" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A866" s="7" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B866" s="7"/>
       <c r="C866" s="3" t="s">
@@ -36856,7 +36853,7 @@
     </row>
     <row r="867" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A867" s="7" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B867" s="7"/>
       <c r="C867" s="3" t="s">
@@ -36871,7 +36868,7 @@
     </row>
     <row r="868" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A868" s="42" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B868" s="42"/>
       <c r="C868" s="3" t="s">
@@ -36886,7 +36883,7 @@
     </row>
     <row r="869" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A869" s="42" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B869" s="42"/>
       <c r="C869" s="3" t="s">
@@ -36901,7 +36898,7 @@
     </row>
     <row r="870" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A870" s="42" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B870" s="42"/>
       <c r="C870" s="3" t="s">
@@ -36916,7 +36913,7 @@
     </row>
     <row r="871" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A871" s="42" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="B871" s="42"/>
       <c r="C871" s="3" t="s">
@@ -36931,7 +36928,7 @@
     </row>
     <row r="872" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A872" s="42" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B872" s="42"/>
       <c r="C872" s="3" t="s">
@@ -36946,7 +36943,7 @@
     </row>
     <row r="873" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A873" s="42" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B873" s="42"/>
       <c r="C873" s="3" t="s">
@@ -36961,14 +36958,14 @@
     </row>
     <row r="874" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A874" s="42" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B874" s="42"/>
       <c r="C874" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D874" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="E874" s="43" t="s">
         <v>9</v>
@@ -36976,7 +36973,7 @@
     </row>
     <row r="875" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A875" s="7" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B875" s="7"/>
       <c r="C875" s="3" t="s">
@@ -36991,7 +36988,7 @@
     </row>
     <row r="876" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A876" s="7" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B876" s="7"/>
       <c r="C876" s="3" t="s">
@@ -37006,7 +37003,7 @@
     </row>
     <row r="877" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A877" s="7" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B877" s="7"/>
       <c r="C877" s="3" t="s">
@@ -37021,7 +37018,7 @@
     </row>
     <row r="878" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A878" s="7" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B878" s="7"/>
       <c r="C878" s="3" t="s">
@@ -37036,7 +37033,7 @@
     </row>
     <row r="879" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A879" s="7" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B879" s="7"/>
       <c r="C879" s="3" t="s">
@@ -37051,7 +37048,7 @@
     </row>
     <row r="880" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A880" s="7" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B880" s="7"/>
       <c r="C880" s="3" t="s">
@@ -37066,7 +37063,7 @@
     </row>
     <row r="881" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A881" s="7" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B881" s="7"/>
       <c r="C881" s="3" t="s">
@@ -37081,7 +37078,7 @@
     </row>
     <row r="882" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A882" s="7" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B882" s="7"/>
       <c r="C882" s="3" t="s">
@@ -37096,7 +37093,7 @@
     </row>
     <row r="883" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A883" s="7" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B883" s="7"/>
       <c r="C883" s="3" t="s">
@@ -37111,7 +37108,7 @@
     </row>
     <row r="884" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A884" s="7" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B884" s="7"/>
       <c r="C884" s="3" t="s">
@@ -37126,7 +37123,7 @@
     </row>
     <row r="885" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A885" s="7" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B885" s="7"/>
       <c r="C885" s="3" t="s">
@@ -37141,7 +37138,7 @@
     </row>
     <row r="886" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A886" s="7" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B886" s="7"/>
       <c r="C886" s="3" t="s">
@@ -37156,7 +37153,7 @@
     </row>
     <row r="887" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A887" s="7" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B887" s="7"/>
       <c r="C887" s="3" t="s">
@@ -37171,7 +37168,7 @@
     </row>
     <row r="888" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A888" s="7" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B888" s="7"/>
       <c r="C888" s="3" t="s">
@@ -37186,7 +37183,7 @@
     </row>
     <row r="889" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A889" s="7" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B889" s="7"/>
       <c r="C889" s="3" t="s">
@@ -37201,7 +37198,7 @@
     </row>
     <row r="890" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A890" s="7" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B890" s="7"/>
       <c r="C890" s="3" t="s">
@@ -37216,7 +37213,7 @@
     </row>
     <row r="891" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A891" s="7" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B891" s="7"/>
       <c r="C891" s="3" t="s">
@@ -37231,7 +37228,7 @@
     </row>
     <row r="892" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A892" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B892" s="7"/>
       <c r="C892" s="3" t="s">
@@ -37246,7 +37243,7 @@
     </row>
     <row r="893" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A893" s="7" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B893" s="7"/>
       <c r="C893" s="3" t="s">
@@ -37261,7 +37258,7 @@
     </row>
     <row r="894" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A894" s="7" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B894" s="7"/>
       <c r="C894" s="3" t="s">
@@ -37276,7 +37273,7 @@
     </row>
     <row r="895" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A895" s="7" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B895" s="7"/>
       <c r="C895" s="3" t="s">
@@ -37291,7 +37288,7 @@
     </row>
     <row r="896" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A896" s="7" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B896" s="7"/>
       <c r="C896" s="3" t="s">
@@ -37306,7 +37303,7 @@
     </row>
     <row r="897" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A897" s="7" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B897" s="7"/>
       <c r="C897" s="3" t="s">
@@ -37321,7 +37318,7 @@
     </row>
     <row r="898" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A898" s="7" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B898" s="7"/>
       <c r="C898" s="3" t="s">
@@ -37336,7 +37333,7 @@
     </row>
     <row r="899" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A899" s="7" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B899" s="7"/>
       <c r="C899" s="3" t="s">
@@ -37351,7 +37348,7 @@
     </row>
     <row r="900" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A900" s="7" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B900" s="7"/>
       <c r="C900" s="3" t="s">
@@ -37366,7 +37363,7 @@
     </row>
     <row r="901" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A901" s="7" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B901" s="7"/>
       <c r="C901" s="3" t="s">
@@ -37381,7 +37378,7 @@
     </row>
     <row r="902" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A902" s="7" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B902" s="7"/>
       <c r="C902" s="3" t="s">
@@ -37396,7 +37393,7 @@
     </row>
     <row r="903" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A903" s="7" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B903" s="7"/>
       <c r="C903" s="3" t="s">
@@ -37411,7 +37408,7 @@
     </row>
     <row r="904" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A904" s="7" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B904" s="7"/>
       <c r="C904" s="3" t="s">
@@ -37426,7 +37423,7 @@
     </row>
     <row r="905" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A905" s="7" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B905" s="7"/>
       <c r="C905" s="3" t="s">
@@ -37441,7 +37438,7 @@
     </row>
     <row r="906" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A906" s="7" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B906" s="7"/>
       <c r="C906" s="3" t="s">
@@ -37456,7 +37453,7 @@
     </row>
     <row r="907" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A907" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B907" s="7"/>
       <c r="C907" s="3" t="s">
@@ -37471,7 +37468,7 @@
     </row>
     <row r="908" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A908" s="7" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B908" s="7"/>
       <c r="C908" s="3" t="s">
@@ -37486,7 +37483,7 @@
     </row>
     <row r="909" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A909" s="7" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B909" s="7"/>
       <c r="C909" s="3" t="s">
@@ -37501,7 +37498,7 @@
     </row>
     <row r="910" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A910" s="7" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B910" s="7"/>
       <c r="C910" s="3" t="s">
@@ -37516,7 +37513,7 @@
     </row>
     <row r="911" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A911" s="7" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B911" s="7"/>
       <c r="C911" s="3" t="s">
@@ -37531,7 +37528,7 @@
     </row>
     <row r="912" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A912" s="7" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B912" s="7"/>
       <c r="C912" s="3" t="s">
@@ -37546,7 +37543,7 @@
     </row>
     <row r="913" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A913" s="7" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B913" s="7"/>
       <c r="C913" s="3" t="s">
@@ -37561,7 +37558,7 @@
     </row>
     <row r="914" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A914" s="7" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B914" s="7"/>
       <c r="C914" s="3" t="s">
@@ -37576,7 +37573,7 @@
     </row>
     <row r="915" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A915" s="7" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B915" s="7"/>
       <c r="C915" s="3" t="s">
@@ -37591,7 +37588,7 @@
     </row>
     <row r="916" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A916" s="7" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B916" s="7"/>
       <c r="C916" s="3" t="s">
@@ -37606,7 +37603,7 @@
     </row>
     <row r="917" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A917" s="7" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B917" s="7"/>
       <c r="C917" s="3" t="s">
@@ -37621,7 +37618,7 @@
     </row>
     <row r="918" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A918" s="7" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B918" s="7"/>
       <c r="C918" s="3" t="s">
@@ -37636,7 +37633,7 @@
     </row>
     <row r="919" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A919" s="7" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B919" s="7"/>
       <c r="C919" s="3" t="s">
@@ -37651,7 +37648,7 @@
     </row>
     <row r="920" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A920" s="7" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B920" s="7"/>
       <c r="C920" s="3" t="s">
@@ -37666,7 +37663,7 @@
     </row>
     <row r="921" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A921" s="7" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B921" s="7"/>
       <c r="C921" s="3" t="s">
@@ -37681,7 +37678,7 @@
     </row>
     <row r="922" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A922" s="7" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B922" s="7"/>
       <c r="C922" s="3" t="s">
@@ -37696,7 +37693,7 @@
     </row>
     <row r="923" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A923" s="7" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B923" s="7"/>
       <c r="C923" s="3" t="s">
@@ -37711,7 +37708,7 @@
     </row>
     <row r="924" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A924" s="7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B924" s="7"/>
       <c r="C924" s="3" t="s">
@@ -37726,7 +37723,7 @@
     </row>
     <row r="925" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A925" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B925" s="7"/>
       <c r="C925" s="3" t="s">
@@ -37741,7 +37738,7 @@
     </row>
     <row r="926" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A926" s="7" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B926" s="7"/>
       <c r="C926" s="3" t="s">
@@ -37756,7 +37753,7 @@
     </row>
     <row r="927" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A927" s="7" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B927" s="7"/>
       <c r="C927" s="3" t="s">
@@ -37771,7 +37768,7 @@
     </row>
     <row r="928" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A928" s="7" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B928" s="7"/>
       <c r="C928" s="3" t="s">
@@ -37786,7 +37783,7 @@
     </row>
     <row r="929" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A929" s="7" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B929" s="7"/>
       <c r="C929" s="3" t="s">
@@ -37801,7 +37798,7 @@
     </row>
     <row r="930" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A930" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B930" s="7"/>
       <c r="C930" s="3" t="s">
@@ -37816,7 +37813,7 @@
     </row>
     <row r="931" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A931" s="7" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B931" s="7"/>
       <c r="C931" s="3" t="s">
@@ -37831,7 +37828,7 @@
     </row>
     <row r="932" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A932" s="7" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B932" s="7"/>
       <c r="C932" s="3" t="s">
@@ -37846,7 +37843,7 @@
     </row>
     <row r="933" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A933" s="7" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B933" s="7"/>
       <c r="C933" s="3" t="s">
@@ -37861,7 +37858,7 @@
     </row>
     <row r="934" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A934" s="7" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B934" s="7"/>
       <c r="C934" s="3" t="s">
@@ -37876,7 +37873,7 @@
     </row>
     <row r="935" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A935" s="7" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B935" s="7"/>
       <c r="C935" s="3" t="s">
@@ -37891,7 +37888,7 @@
     </row>
     <row r="936" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A936" s="7" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B936" s="7"/>
       <c r="C936" s="3" t="s">
@@ -37906,7 +37903,7 @@
     </row>
     <row r="937" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A937" s="7" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B937" s="7"/>
       <c r="C937" s="3" t="s">
@@ -37921,7 +37918,7 @@
     </row>
     <row r="938" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A938" s="7" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B938" s="7"/>
       <c r="C938" s="3" t="s">
@@ -37936,7 +37933,7 @@
     </row>
     <row r="939" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A939" s="7" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B939" s="7"/>
       <c r="C939" s="3" t="s">
@@ -37951,7 +37948,7 @@
     </row>
     <row r="940" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A940" s="7" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B940" s="7"/>
       <c r="C940" s="3" t="s">
@@ -37966,7 +37963,7 @@
     </row>
     <row r="941" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A941" s="7" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B941" s="7"/>
       <c r="C941" s="3" t="s">
@@ -37981,7 +37978,7 @@
     </row>
     <row r="942" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A942" s="7" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B942" s="7"/>
       <c r="C942" s="3" t="s">
@@ -37996,7 +37993,7 @@
     </row>
     <row r="943" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A943" s="7" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B943" s="7"/>
       <c r="C943" s="3" t="s">
@@ -38011,7 +38008,7 @@
     </row>
     <row r="944" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A944" s="7" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B944" s="7"/>
       <c r="C944" s="3" t="s">
@@ -38026,7 +38023,7 @@
     </row>
     <row r="945" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A945" s="7" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B945" s="7"/>
       <c r="C945" s="3" t="s">
@@ -38041,7 +38038,7 @@
     </row>
     <row r="946" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A946" s="7" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B946" s="7"/>
       <c r="C946" s="3" t="s">
@@ -38056,7 +38053,7 @@
     </row>
     <row r="947" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A947" s="7" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B947" s="7"/>
       <c r="C947" s="3" t="s">
@@ -38071,7 +38068,7 @@
     </row>
     <row r="948" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A948" s="7" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B948" s="7"/>
       <c r="C948" s="3" t="s">
@@ -38086,7 +38083,7 @@
     </row>
     <row r="949" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A949" s="7" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B949" s="7"/>
       <c r="C949" s="3" t="s">
@@ -38101,7 +38098,7 @@
     </row>
     <row r="950" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A950" s="7" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B950" s="7"/>
       <c r="C950" s="3" t="s">
@@ -38116,7 +38113,7 @@
     </row>
     <row r="951" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A951" s="7" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B951" s="7"/>
       <c r="C951" s="3" t="s">
@@ -38131,7 +38128,7 @@
     </row>
     <row r="952" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A952" s="7" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B952" s="7"/>
       <c r="C952" s="3" t="s">
@@ -38146,7 +38143,7 @@
     </row>
     <row r="953" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A953" s="7" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B953" s="7"/>
       <c r="C953" s="3" t="s">
@@ -38161,7 +38158,7 @@
     </row>
     <row r="954" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A954" s="7" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B954" s="7"/>
       <c r="C954" s="3" t="s">
@@ -38176,7 +38173,7 @@
     </row>
     <row r="955" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A955" s="7" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B955" s="7"/>
       <c r="C955" s="3" t="s">
@@ -38191,14 +38188,14 @@
     </row>
     <row r="956" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A956" s="7" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B956" s="8"/>
       <c r="C956" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D956" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="E956" s="22" t="s">
         <v>9</v>
@@ -38206,7 +38203,7 @@
     </row>
     <row r="957" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A957" s="7" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B957" s="8"/>
       <c r="C957" s="3" t="s">
@@ -38221,7 +38218,7 @@
     </row>
     <row r="958" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A958" s="7" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B958" s="8"/>
       <c r="C958" s="3" t="s">
@@ -38236,7 +38233,7 @@
     </row>
     <row r="959" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A959" s="7" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B959" s="8"/>
       <c r="C959" s="3" t="s">
@@ -38251,7 +38248,7 @@
     </row>
     <row r="960" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A960" s="7" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B960" s="8"/>
       <c r="C960" s="3" t="s">
@@ -38311,7 +38308,7 @@
     </row>
     <row r="964" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A964" s="7" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B964" s="8"/>
       <c r="C964" s="3" t="s">
@@ -38326,7 +38323,7 @@
     </row>
     <row r="965" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A965" s="7" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B965" s="8"/>
       <c r="C965" s="3" t="s">
@@ -38356,7 +38353,7 @@
     </row>
     <row r="967" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A967" s="7" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B967" s="8"/>
       <c r="C967" s="3" t="s">
@@ -38371,7 +38368,7 @@
     </row>
     <row r="968" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A968" s="7" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B968" s="8"/>
       <c r="C968" s="3" t="s">
@@ -38401,7 +38398,7 @@
     </row>
     <row r="970" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A970" s="7" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B970" s="8"/>
       <c r="C970" s="3" t="s">
@@ -38416,7 +38413,7 @@
     </row>
     <row r="971" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A971" s="7" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B971" s="8"/>
       <c r="C971" s="3" t="s">
@@ -38431,7 +38428,7 @@
     </row>
     <row r="972" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A972" s="7" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B972" s="8"/>
       <c r="C972" s="3" t="s">
@@ -38446,7 +38443,7 @@
     </row>
     <row r="973" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A973" s="7" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B973" s="8"/>
       <c r="C973" s="3" t="s">
@@ -38461,7 +38458,7 @@
     </row>
     <row r="974" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A974" s="7" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B974" s="8"/>
       <c r="C974" s="3" t="s">
@@ -38476,7 +38473,7 @@
     </row>
     <row r="975" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A975" s="7" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B975" s="8"/>
       <c r="C975" s="3" t="s">
@@ -38491,7 +38488,7 @@
     </row>
     <row r="976" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A976" s="7" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B976" s="8"/>
       <c r="C976" s="3" t="s">
@@ -38506,7 +38503,7 @@
     </row>
     <row r="977" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A977" s="7" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B977" s="8"/>
       <c r="C977" s="3" t="s">
@@ -38521,7 +38518,7 @@
     </row>
     <row r="978" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A978" s="7" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B978" s="17"/>
       <c r="C978" s="3" t="s">
@@ -38536,7 +38533,7 @@
     </row>
     <row r="979" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A979" s="7" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B979" s="17"/>
       <c r="C979" s="3" t="s">
@@ -38551,7 +38548,7 @@
     </row>
     <row r="980" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A980" s="7" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B980" s="17"/>
       <c r="C980" s="3" t="s">
@@ -38566,7 +38563,7 @@
     </row>
     <row r="981" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A981" s="7" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B981" s="17"/>
       <c r="C981" s="3" t="s">
@@ -38581,7 +38578,7 @@
     </row>
     <row r="982" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A982" s="33" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B982" s="17"/>
       <c r="C982" s="3" t="s">
@@ -38596,7 +38593,7 @@
     </row>
     <row r="983" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A983" s="34" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B983" s="17"/>
       <c r="C983" s="3" t="s">
@@ -38611,7 +38608,7 @@
     </row>
     <row r="984" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A984" s="34" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B984" s="17"/>
       <c r="C984" s="3" t="s">
@@ -38626,7 +38623,7 @@
     </row>
     <row r="985" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A985" s="34" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B985" s="17"/>
       <c r="C985" s="3" t="s">
@@ -38641,7 +38638,7 @@
     </row>
     <row r="986" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A986" s="34" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B986" s="8"/>
       <c r="C986" s="3" t="s">
@@ -38656,7 +38653,7 @@
     </row>
     <row r="987" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A987" s="34" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B987" s="8"/>
       <c r="C987" s="3" t="s">
@@ -38671,7 +38668,7 @@
     </row>
     <row r="988" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A988" s="34" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B988" s="8"/>
       <c r="C988" s="3" t="s">
@@ -38686,7 +38683,7 @@
     </row>
     <row r="989" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A989" s="34" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B989" s="8"/>
       <c r="C989" s="3" t="s">
@@ -38701,7 +38698,7 @@
     </row>
     <row r="990" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A990" s="34" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B990" s="8"/>
       <c r="C990" s="3" t="s">
@@ -38716,7 +38713,7 @@
     </row>
     <row r="991" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A991" s="7" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B991" s="8"/>
       <c r="C991" s="3" t="s">
@@ -38731,7 +38728,7 @@
     </row>
     <row r="992" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A992" s="7" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B992" s="8"/>
       <c r="C992" s="3" t="s">
@@ -38746,7 +38743,7 @@
     </row>
     <row r="993" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A993" s="7" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B993" s="8"/>
       <c r="C993" s="3" t="s">
@@ -38761,7 +38758,7 @@
     </row>
     <row r="994" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A994" s="7" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B994" s="8"/>
       <c r="C994" s="3" t="s">
@@ -38776,7 +38773,7 @@
     </row>
     <row r="995" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A995" s="7" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B995" s="8"/>
       <c r="C995" s="3" t="s">
@@ -38791,7 +38788,7 @@
     </row>
     <row r="996" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A996" s="7" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B996" s="8"/>
       <c r="C996" s="3" t="s">
@@ -38806,7 +38803,7 @@
     </row>
     <row r="997" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A997" s="7" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B997" s="8"/>
       <c r="C997" s="3" t="s">
@@ -38821,7 +38818,7 @@
     </row>
     <row r="998" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A998" s="7" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B998" s="8"/>
       <c r="C998" s="3" t="s">
@@ -38836,7 +38833,7 @@
     </row>
     <row r="999" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A999" s="7" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B999" s="8"/>
       <c r="C999" s="3" t="s">
@@ -38851,7 +38848,7 @@
     </row>
     <row r="1000" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1000" s="7" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B1000" s="8"/>
       <c r="C1000" s="3" t="s">
@@ -38866,7 +38863,7 @@
     </row>
     <row r="1001" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1001" s="7" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B1001" s="8"/>
       <c r="C1001" s="3" t="s">
@@ -38881,7 +38878,7 @@
     </row>
     <row r="1002" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1002" s="7" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B1002" s="8"/>
       <c r="C1002" s="3" t="s">
@@ -38896,7 +38893,7 @@
     </row>
     <row r="1003" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1003" s="7" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B1003" s="8"/>
       <c r="C1003" s="3" t="s">
@@ -38911,7 +38908,7 @@
     </row>
     <row r="1004" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1004" s="7" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B1004" s="8"/>
       <c r="C1004" s="3" t="s">
@@ -38926,7 +38923,7 @@
     </row>
     <row r="1005" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1005" s="7" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B1005" s="8"/>
       <c r="C1005" s="3" t="s">
@@ -38941,7 +38938,7 @@
     </row>
     <row r="1006" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1006" s="7" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B1006" s="7"/>
       <c r="C1006" s="3" t="s">
@@ -38956,7 +38953,7 @@
     </row>
     <row r="1007" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1007" s="7" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B1007" s="7"/>
       <c r="C1007" s="3" t="s">
@@ -38971,7 +38968,7 @@
     </row>
     <row r="1008" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1008" s="7" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B1008" s="7"/>
       <c r="C1008" s="3" t="s">
@@ -38986,7 +38983,7 @@
     </row>
     <row r="1009" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1009" s="7" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B1009" s="7"/>
       <c r="C1009" s="3" t="s">
@@ -39001,7 +38998,7 @@
     </row>
     <row r="1010" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1010" s="7" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B1010" s="7"/>
       <c r="C1010" s="3" t="s">
@@ -39016,7 +39013,7 @@
     </row>
     <row r="1011" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1011" s="7" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B1011" s="7"/>
       <c r="C1011" s="3" t="s">
@@ -39031,7 +39028,7 @@
     </row>
     <row r="1012" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1012" s="7" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B1012" s="7"/>
       <c r="C1012" s="3" t="s">
@@ -39046,7 +39043,7 @@
     </row>
     <row r="1013" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1013" s="7" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B1013" s="7"/>
       <c r="C1013" s="3" t="s">
@@ -39061,7 +39058,7 @@
     </row>
     <row r="1014" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1014" s="7" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B1014" s="7"/>
       <c r="C1014" s="3" t="s">
@@ -39076,7 +39073,7 @@
     </row>
     <row r="1015" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1015" s="7" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B1015" s="7"/>
       <c r="C1015" s="3" t="s">
@@ -39091,7 +39088,7 @@
     </row>
     <row r="1016" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1016" s="7" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B1016" s="7"/>
       <c r="C1016" s="3" t="s">
@@ -39106,7 +39103,7 @@
     </row>
     <row r="1017" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1017" s="7" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B1017" s="7"/>
       <c r="C1017" s="3" t="s">
@@ -39121,7 +39118,7 @@
     </row>
     <row r="1018" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1018" s="7" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B1018" s="7"/>
       <c r="C1018" s="3" t="s">
@@ -39136,7 +39133,7 @@
     </row>
     <row r="1019" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1019" s="7" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B1019" s="7"/>
       <c r="C1019" s="3" t="s">
@@ -39151,7 +39148,7 @@
     </row>
     <row r="1020" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1020" s="7" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B1020" s="7"/>
       <c r="C1020" s="3" t="s">
@@ -39166,7 +39163,7 @@
     </row>
     <row r="1021" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1021" s="7" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B1021" s="7"/>
       <c r="C1021" s="3" t="s">
@@ -39181,7 +39178,7 @@
     </row>
     <row r="1022" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1022" s="7" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B1022" s="7"/>
       <c r="C1022" s="3" t="s">
@@ -39196,7 +39193,7 @@
     </row>
     <row r="1023" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1023" s="7" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B1023" s="7"/>
       <c r="C1023" s="3" t="s">
@@ -39211,7 +39208,7 @@
     </row>
     <row r="1024" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1024" s="7" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B1024" s="7"/>
       <c r="C1024" s="3" t="s">
@@ -39226,7 +39223,7 @@
     </row>
     <row r="1025" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1025" s="7" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B1025" s="7"/>
       <c r="C1025" s="3" t="s">
@@ -39241,7 +39238,7 @@
     </row>
     <row r="1026" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1026" s="7" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B1026" s="7"/>
       <c r="C1026" s="3" t="s">
@@ -39256,7 +39253,7 @@
     </row>
     <row r="1027" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1027" s="7" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B1027" s="7"/>
       <c r="C1027" s="3" t="s">
@@ -39271,7 +39268,7 @@
     </row>
     <row r="1028" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1028" s="7" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B1028" s="7"/>
       <c r="C1028" s="3" t="s">
@@ -39286,7 +39283,7 @@
     </row>
     <row r="1029" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1029" s="7" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B1029" s="7"/>
       <c r="C1029" s="3" t="s">
@@ -39301,7 +39298,7 @@
     </row>
     <row r="1030" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1030" s="7" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B1030" s="7"/>
       <c r="C1030" s="3" t="s">
@@ -39316,7 +39313,7 @@
     </row>
     <row r="1031" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1031" s="7" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B1031" s="7"/>
       <c r="C1031" s="3" t="s">
@@ -39331,7 +39328,7 @@
     </row>
     <row r="1032" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1032" s="7" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B1032" s="7"/>
       <c r="C1032" s="3" t="s">
@@ -39346,7 +39343,7 @@
     </row>
     <row r="1033" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1033" s="7" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B1033" s="7"/>
       <c r="C1033" s="3" t="s">
@@ -39361,7 +39358,7 @@
     </row>
     <row r="1034" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1034" s="7" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B1034" s="7"/>
       <c r="C1034" s="3" t="s">
@@ -39376,7 +39373,7 @@
     </row>
     <row r="1035" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1035" s="7" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B1035" s="7"/>
       <c r="C1035" s="3" t="s">
@@ -39391,7 +39388,7 @@
     </row>
     <row r="1036" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1036" s="7" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B1036" s="7"/>
       <c r="C1036" s="3" t="s">
@@ -39406,7 +39403,7 @@
     </row>
     <row r="1037" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1037" s="7" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B1037" s="7"/>
       <c r="C1037" s="3" t="s">
@@ -39421,7 +39418,7 @@
     </row>
     <row r="1038" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1038" s="7" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B1038" s="7"/>
       <c r="C1038" s="3" t="s">
@@ -39436,7 +39433,7 @@
     </row>
     <row r="1039" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1039" s="7" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B1039" s="7"/>
       <c r="C1039" s="3" t="s">
@@ -39451,7 +39448,7 @@
     </row>
     <row r="1040" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1040" s="7" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="B1040" s="7"/>
       <c r="C1040" s="3" t="s">
@@ -39466,7 +39463,7 @@
     </row>
     <row r="1041" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1041" s="7" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B1041" s="7"/>
       <c r="C1041" s="3" t="s">
@@ -39481,7 +39478,7 @@
     </row>
     <row r="1042" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1042" s="7" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="B1042" s="7"/>
       <c r="C1042" s="3" t="s">
@@ -39496,7 +39493,7 @@
     </row>
     <row r="1043" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1043" s="7" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B1043" s="7"/>
       <c r="C1043" s="3" t="s">
@@ -39511,7 +39508,7 @@
     </row>
     <row r="1044" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1044" s="7" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B1044" s="7"/>
       <c r="C1044" s="3" t="s">
@@ -39526,7 +39523,7 @@
     </row>
     <row r="1045" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1045" s="7" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B1045" s="7"/>
       <c r="C1045" s="3" t="s">
@@ -39541,7 +39538,7 @@
     </row>
     <row r="1046" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1046" s="7" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B1046" s="7"/>
       <c r="C1046" s="3" t="s">
@@ -39556,7 +39553,7 @@
     </row>
     <row r="1047" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1047" s="7" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B1047" s="7"/>
       <c r="C1047" s="3" t="s">
@@ -39571,7 +39568,7 @@
     </row>
     <row r="1048" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1048" s="7" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B1048" s="7"/>
       <c r="C1048" s="3" t="s">
@@ -39586,7 +39583,7 @@
     </row>
     <row r="1049" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1049" s="7" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B1049" s="7"/>
       <c r="C1049" s="3" t="s">
@@ -39601,7 +39598,7 @@
     </row>
     <row r="1050" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1050" s="7" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B1050" s="7"/>
       <c r="C1050" s="3" t="s">
@@ -39616,7 +39613,7 @@
     </row>
     <row r="1051" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1051" s="7" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B1051" s="7"/>
       <c r="C1051" s="3" t="s">
@@ -39631,7 +39628,7 @@
     </row>
     <row r="1052" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1052" s="7" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B1052" s="7"/>
       <c r="C1052" s="3" t="s">
@@ -39646,7 +39643,7 @@
     </row>
     <row r="1053" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1053" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B1053" s="7"/>
       <c r="C1053" s="3" t="s">
@@ -39661,7 +39658,7 @@
     </row>
     <row r="1054" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1054" s="7" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B1054" s="7"/>
       <c r="C1054" s="3" t="s">
@@ -39676,7 +39673,7 @@
     </row>
     <row r="1055" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1055" s="7" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B1055" s="7"/>
       <c r="C1055" s="3" t="s">
@@ -39691,7 +39688,7 @@
     </row>
     <row r="1056" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1056" s="7" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B1056" s="7"/>
       <c r="C1056" s="3" t="s">
@@ -39706,7 +39703,7 @@
     </row>
     <row r="1057" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1057" s="7" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B1057" s="7"/>
       <c r="C1057" s="3" t="s">
@@ -39721,7 +39718,7 @@
     </row>
     <row r="1058" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1058" s="7" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B1058" s="7"/>
       <c r="C1058" s="3" t="s">
@@ -39736,7 +39733,7 @@
     </row>
     <row r="1059" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1059" s="7" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B1059" s="7"/>
       <c r="C1059" s="3" t="s">
@@ -39751,7 +39748,7 @@
     </row>
     <row r="1060" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1060" s="7" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B1060" s="7"/>
       <c r="C1060" s="3" t="s">
@@ -39766,7 +39763,7 @@
     </row>
     <row r="1061" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1061" s="7" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B1061" s="7"/>
       <c r="C1061" s="3" t="s">
@@ -39781,7 +39778,7 @@
     </row>
     <row r="1062" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1062" s="7" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B1062" s="7"/>
       <c r="C1062" s="3" t="s">
@@ -39796,7 +39793,7 @@
     </row>
     <row r="1063" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1063" s="7" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B1063" s="7"/>
       <c r="C1063" s="3" t="s">
@@ -39811,7 +39808,7 @@
     </row>
     <row r="1064" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1064" s="7" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B1064" s="7"/>
       <c r="C1064" s="3" t="s">
@@ -39826,7 +39823,7 @@
     </row>
     <row r="1065" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1065" s="7" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B1065" s="7"/>
       <c r="C1065" s="3" t="s">
@@ -39841,7 +39838,7 @@
     </row>
     <row r="1066" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1066" s="7" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B1066" s="7"/>
       <c r="C1066" s="3" t="s">
@@ -39856,7 +39853,7 @@
     </row>
     <row r="1067" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1067" s="7" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B1067" s="7"/>
       <c r="C1067" s="3" t="s">
@@ -39871,7 +39868,7 @@
     </row>
     <row r="1068" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1068" s="7" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B1068" s="7"/>
       <c r="C1068" s="3" t="s">
@@ -39886,7 +39883,7 @@
     </row>
     <row r="1069" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1069" s="7" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B1069" s="7"/>
       <c r="C1069" s="3" t="s">
@@ -39901,7 +39898,7 @@
     </row>
     <row r="1070" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1070" s="7" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B1070" s="7"/>
       <c r="C1070" s="3" t="s">
@@ -39916,7 +39913,7 @@
     </row>
     <row r="1071" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1071" s="7" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B1071" s="7"/>
       <c r="C1071" s="3" t="s">
@@ -39931,7 +39928,7 @@
     </row>
     <row r="1072" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1072" s="7" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B1072" s="7"/>
       <c r="C1072" s="3" t="s">
@@ -39946,7 +39943,7 @@
     </row>
     <row r="1073" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1073" s="7" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B1073" s="7"/>
       <c r="C1073" s="3" t="s">
@@ -39961,7 +39958,7 @@
     </row>
     <row r="1074" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1074" s="7" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B1074" s="7"/>
       <c r="C1074" s="3" t="s">
@@ -39976,7 +39973,7 @@
     </row>
     <row r="1075" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1075" s="7" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B1075" s="7"/>
       <c r="C1075" s="3" t="s">
@@ -39991,7 +39988,7 @@
     </row>
     <row r="1076" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1076" s="7" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B1076" s="7"/>
       <c r="C1076" s="3" t="s">
@@ -40006,7 +40003,7 @@
     </row>
     <row r="1077" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1077" s="7" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B1077" s="7"/>
       <c r="C1077" s="3" t="s">
@@ -40021,7 +40018,7 @@
     </row>
     <row r="1078" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1078" s="7" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B1078" s="7"/>
       <c r="C1078" s="3" t="s">
@@ -40036,7 +40033,7 @@
     </row>
     <row r="1079" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1079" s="7" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B1079" s="38"/>
       <c r="C1079" s="3" t="s">
@@ -40051,7 +40048,7 @@
     </row>
     <row r="1080" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1080" s="7" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B1080" s="38"/>
       <c r="C1080" s="3" t="s">
@@ -40066,7 +40063,7 @@
     </row>
     <row r="1081" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1081" s="7" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B1081" s="38"/>
       <c r="C1081" s="3" t="s">
@@ -40081,7 +40078,7 @@
     </row>
     <row r="1082" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1082" s="7" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B1082" s="38"/>
       <c r="C1082" s="3" t="s">
@@ -40096,7 +40093,7 @@
     </row>
     <row r="1083" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1083" s="7" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B1083" s="38"/>
       <c r="C1083" s="3" t="s">
@@ -40111,7 +40108,7 @@
     </row>
     <row r="1084" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1084" s="37" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B1084" s="38"/>
       <c r="C1084" s="3" t="s">
@@ -40126,7 +40123,7 @@
     </row>
     <row r="1085" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1085" s="37" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B1085" s="38"/>
       <c r="C1085" s="3" t="s">
@@ -40141,7 +40138,7 @@
     </row>
     <row r="1086" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1086" s="37" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B1086" s="38"/>
       <c r="C1086" s="3" t="s">
@@ -40156,7 +40153,7 @@
     </row>
     <row r="1087" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1087" s="37" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B1087" s="38"/>
       <c r="C1087" s="3" t="s">
@@ -40171,7 +40168,7 @@
     </row>
     <row r="1088" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1088" s="37" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B1088" s="38"/>
       <c r="C1088" s="3" t="s">
@@ -40186,7 +40183,7 @@
     </row>
     <row r="1089" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1089" s="37" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B1089" s="38"/>
       <c r="C1089" s="3" t="s">
@@ -40201,7 +40198,7 @@
     </row>
     <row r="1090" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1090" s="37" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B1090" s="38"/>
       <c r="C1090" s="3" t="s">
@@ -40216,7 +40213,7 @@
     </row>
     <row r="1091" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1091" s="37" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B1091" s="38"/>
       <c r="C1091" s="3" t="s">
@@ -40231,7 +40228,7 @@
     </row>
     <row r="1092" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1092" s="37" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B1092" s="38"/>
       <c r="C1092" s="3" t="s">
@@ -40246,7 +40243,7 @@
     </row>
     <row r="1093" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1093" s="37" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B1093" s="38"/>
       <c r="C1093" s="3" t="s">
@@ -40261,7 +40258,7 @@
     </row>
     <row r="1094" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1094" s="37" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B1094" s="38"/>
       <c r="C1094" s="3" t="s">
@@ -40276,7 +40273,7 @@
     </row>
     <row r="1095" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1095" s="37" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B1095" s="38"/>
       <c r="C1095" s="3" t="s">
@@ -40291,7 +40288,7 @@
     </row>
     <row r="1096" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1096" s="37" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B1096" s="38"/>
       <c r="C1096" s="3" t="s">
@@ -40306,7 +40303,7 @@
     </row>
     <row r="1097" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1097" s="37" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B1097" s="38"/>
       <c r="C1097" s="3" t="s">
@@ -40321,7 +40318,7 @@
     </row>
     <row r="1098" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1098" s="37" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B1098" s="38"/>
       <c r="C1098" s="3" t="s">
@@ -40336,7 +40333,7 @@
     </row>
     <row r="1099" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1099" s="37" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B1099" s="38"/>
       <c r="C1099" s="3" t="s">
@@ -40351,7 +40348,7 @@
     </row>
     <row r="1100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1100" s="37" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B1100" s="38"/>
       <c r="C1100" s="3" t="s">
@@ -40366,7 +40363,7 @@
     </row>
     <row r="1101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1101" s="37" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B1101" s="38"/>
       <c r="C1101" s="3" t="s">
@@ -40381,7 +40378,7 @@
     </row>
     <row r="1102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1102" s="37" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B1102" s="38"/>
       <c r="C1102" s="3" t="s">
@@ -40396,7 +40393,7 @@
     </row>
     <row r="1103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1103" s="37" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B1103" s="38"/>
       <c r="C1103" s="3" t="s">
@@ -40411,7 +40408,7 @@
     </row>
     <row r="1104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1104" s="37" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B1104" s="38"/>
       <c r="C1104" s="3" t="s">
@@ -40426,7 +40423,7 @@
     </row>
     <row r="1105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1105" s="37" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B1105" s="38"/>
       <c r="C1105" s="3" t="s">
@@ -40441,7 +40438,7 @@
     </row>
     <row r="1106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1106" s="37" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B1106" s="38"/>
       <c r="C1106" s="3" t="s">
@@ -40456,7 +40453,7 @@
     </row>
     <row r="1107" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1107" s="37" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B1107" s="38"/>
       <c r="C1107" s="3" t="s">
@@ -40471,7 +40468,7 @@
     </row>
     <row r="1108" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1108" s="37" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B1108" s="38"/>
       <c r="C1108" s="3" t="s">
@@ -40486,7 +40483,7 @@
     </row>
     <row r="1109" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1109" s="37" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B1109" s="38"/>
       <c r="C1109" s="3" t="s">
@@ -40501,7 +40498,7 @@
     </row>
     <row r="1110" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1110" s="37" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B1110" s="38"/>
       <c r="C1110" s="3" t="s">
@@ -40516,7 +40513,7 @@
     </row>
     <row r="1111" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1111" s="37" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B1111" s="38"/>
       <c r="C1111" s="3" t="s">
@@ -40531,7 +40528,7 @@
     </row>
     <row r="1112" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1112" s="37" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B1112" s="38"/>
       <c r="C1112" s="3" t="s">
@@ -40546,7 +40543,7 @@
     </row>
     <row r="1113" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1113" s="37" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B1113" s="38"/>
       <c r="C1113" s="3" t="s">
@@ -40561,7 +40558,7 @@
     </row>
     <row r="1114" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1114" s="37" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B1114" s="38"/>
       <c r="C1114" s="3" t="s">
@@ -40576,7 +40573,7 @@
     </row>
     <row r="1115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1115" s="37" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B1115" s="38"/>
       <c r="C1115" s="3" t="s">
@@ -40591,7 +40588,7 @@
     </row>
     <row r="1116" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1116" s="37" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B1116" s="38"/>
       <c r="C1116" s="3" t="s">
@@ -40606,7 +40603,7 @@
     </row>
     <row r="1117" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1117" s="37" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B1117" s="38"/>
       <c r="C1117" s="3" t="s">
@@ -40621,7 +40618,7 @@
     </row>
     <row r="1118" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1118" s="37" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B1118" s="38"/>
       <c r="C1118" s="3" t="s">
@@ -40636,7 +40633,7 @@
     </row>
     <row r="1119" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1119" s="37" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B1119" s="38"/>
       <c r="C1119" s="3" t="s">
@@ -40651,7 +40648,7 @@
     </row>
     <row r="1120" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1120" s="37" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B1120" s="38"/>
       <c r="C1120" s="3" t="s">
@@ -40666,7 +40663,7 @@
     </row>
     <row r="1121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1121" s="37" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B1121" s="40"/>
       <c r="C1121" s="3" t="s">
@@ -40681,7 +40678,7 @@
     </row>
     <row r="1122" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1122" s="37" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B1122" s="40"/>
       <c r="C1122" s="3" t="s">
@@ -40696,7 +40693,7 @@
     </row>
     <row r="1123" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1123" s="37" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B1123" s="40"/>
       <c r="C1123" s="3" t="s">
@@ -40711,7 +40708,7 @@
     </row>
     <row r="1124" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1124" s="37" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B1124" s="40"/>
       <c r="C1124" s="3" t="s">
@@ -40726,7 +40723,7 @@
     </row>
     <row r="1125" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1125" s="37" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B1125" s="40"/>
       <c r="C1125" s="3" t="s">
@@ -40741,7 +40738,7 @@
     </row>
     <row r="1126" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1126" s="37" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B1126" s="40"/>
       <c r="C1126" s="3" t="s">
@@ -40756,7 +40753,7 @@
     </row>
     <row r="1127" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1127" s="37" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B1127" s="40"/>
       <c r="C1127" s="3" t="s">
@@ -40771,7 +40768,7 @@
     </row>
     <row r="1128" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1128" s="37" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B1128" s="40"/>
       <c r="C1128" s="3" t="s">
@@ -40786,7 +40783,7 @@
     </row>
     <row r="1129" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1129" s="37" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B1129" s="40"/>
       <c r="C1129" s="3" t="s">
@@ -40801,7 +40798,7 @@
     </row>
     <row r="1130" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1130" s="37" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B1130" s="40"/>
       <c r="C1130" s="3" t="s">
@@ -40816,7 +40813,7 @@
     </row>
     <row r="1131" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1131" s="37" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B1131" s="40"/>
       <c r="C1131" s="3" t="s">
@@ -40831,7 +40828,7 @@
     </row>
     <row r="1132" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1132" s="37" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B1132" s="40"/>
       <c r="C1132" s="3" t="s">
@@ -40846,7 +40843,7 @@
     </row>
     <row r="1133" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1133" s="37" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B1133" s="40"/>
       <c r="C1133" s="3" t="s">
@@ -40861,7 +40858,7 @@
     </row>
     <row r="1134" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1134" s="37" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B1134" s="40"/>
       <c r="C1134" s="3" t="s">
@@ -40876,7 +40873,7 @@
     </row>
     <row r="1135" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1135" s="37" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B1135" s="40"/>
       <c r="C1135" s="3" t="s">
@@ -40891,7 +40888,7 @@
     </row>
     <row r="1136" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1136" s="37" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B1136" s="40"/>
       <c r="C1136" s="3" t="s">
@@ -40906,7 +40903,7 @@
     </row>
     <row r="1137" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1137" s="37" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B1137" s="40"/>
       <c r="C1137" s="3" t="s">
@@ -40921,7 +40918,7 @@
     </row>
     <row r="1138" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1138" s="37" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B1138" s="40"/>
       <c r="C1138" s="3" t="s">
@@ -40936,7 +40933,7 @@
     </row>
     <row r="1139" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1139" s="37" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B1139" s="40"/>
       <c r="C1139" s="3" t="s">
@@ -40951,7 +40948,7 @@
     </row>
     <row r="1140" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1140" s="37" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B1140" s="40"/>
       <c r="C1140" s="3" t="s">
@@ -40966,7 +40963,7 @@
     </row>
     <row r="1141" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1141" s="37" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B1141" s="40"/>
       <c r="C1141" s="3" t="s">
@@ -40981,7 +40978,7 @@
     </row>
     <row r="1142" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1142" s="37" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B1142" s="40"/>
       <c r="C1142" s="3" t="s">
@@ -40996,7 +40993,7 @@
     </row>
     <row r="1143" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1143" s="37" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B1143" s="40"/>
       <c r="C1143" s="3" t="s">
@@ -41011,7 +41008,7 @@
     </row>
     <row r="1144" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1144" s="37" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B1144" s="40"/>
       <c r="C1144" s="3" t="s">
@@ -41026,7 +41023,7 @@
     </row>
     <row r="1145" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1145" s="37" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B1145" s="40"/>
       <c r="C1145" s="3" t="s">
@@ -41041,7 +41038,7 @@
     </row>
     <row r="1146" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1146" s="37" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B1146" s="40"/>
       <c r="C1146" s="3" t="s">
@@ -41056,7 +41053,7 @@
     </row>
     <row r="1147" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1147" s="37" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B1147" s="40"/>
       <c r="C1147" s="3" t="s">
@@ -41071,7 +41068,7 @@
     </row>
     <row r="1148" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1148" s="37" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B1148" s="40"/>
       <c r="C1148" s="3" t="s">
@@ -41086,7 +41083,7 @@
     </row>
     <row r="1149" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1149" s="37" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B1149" s="40"/>
       <c r="C1149" s="3" t="s">
@@ -41101,7 +41098,7 @@
     </row>
     <row r="1150" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1150" s="37" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B1150" s="40"/>
       <c r="C1150" s="3" t="s">
@@ -41116,7 +41113,7 @@
     </row>
     <row r="1151" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1151" s="37" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="B1151" s="40"/>
       <c r="C1151" s="3" t="s">
@@ -41131,7 +41128,7 @@
     </row>
     <row r="1152" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1152" s="37" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="B1152" s="40"/>
       <c r="C1152" s="3" t="s">
@@ -41146,7 +41143,7 @@
     </row>
     <row r="1153" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1153" s="37" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="B1153" s="40"/>
       <c r="C1153" s="3" t="s">
@@ -41161,7 +41158,7 @@
     </row>
     <row r="1154" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1154" s="37" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="B1154" s="40"/>
       <c r="C1154" s="3" t="s">
@@ -41176,7 +41173,7 @@
     </row>
     <row r="1155" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1155" s="37" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B1155" s="40"/>
       <c r="C1155" s="3" t="s">
@@ -41191,7 +41188,7 @@
     </row>
     <row r="1156" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1156" s="37" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="B1156" s="40"/>
       <c r="C1156" s="3" t="s">
@@ -41206,7 +41203,7 @@
     </row>
     <row r="1157" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1157" s="37" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="B1157" s="40"/>
       <c r="C1157" s="3" t="s">
@@ -41221,7 +41218,7 @@
     </row>
     <row r="1158" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1158" s="37" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="B1158" s="40"/>
       <c r="C1158" s="3" t="s">
@@ -41236,7 +41233,7 @@
     </row>
     <row r="1159" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1159" s="37" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B1159" s="40"/>
       <c r="C1159" s="3" t="s">
@@ -41251,7 +41248,7 @@
     </row>
     <row r="1160" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1160" s="37" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="B1160" s="40"/>
       <c r="C1160" s="3" t="s">
@@ -41266,7 +41263,7 @@
     </row>
     <row r="1161" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1161" s="37" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B1161" s="40"/>
       <c r="C1161" s="3" t="s">
@@ -41281,7 +41278,7 @@
     </row>
     <row r="1162" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1162" s="37" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="B1162" s="40"/>
       <c r="C1162" s="3" t="s">
@@ -41296,7 +41293,7 @@
     </row>
     <row r="1163" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1163" s="37" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="B1163" s="40"/>
       <c r="C1163" s="3" t="s">
@@ -41311,7 +41308,7 @@
     </row>
     <row r="1164" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1164" s="37" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B1164" s="40"/>
       <c r="C1164" s="3" t="s">
@@ -41326,7 +41323,7 @@
     </row>
     <row r="1165" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1165" s="37" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B1165" s="40"/>
       <c r="C1165" s="3" t="s">
@@ -41341,7 +41338,7 @@
     </row>
     <row r="1166" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1166" s="37" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B1166" s="40"/>
       <c r="C1166" s="3" t="s">
@@ -41356,7 +41353,7 @@
     </row>
     <row r="1167" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1167" s="37" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="B1167" s="40"/>
       <c r="C1167" s="3" t="s">
@@ -41371,7 +41368,7 @@
     </row>
     <row r="1168" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1168" s="37" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B1168" s="40"/>
       <c r="C1168" s="3" t="s">
@@ -41386,7 +41383,7 @@
     </row>
     <row r="1169" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1169" s="37" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="B1169" s="40"/>
       <c r="C1169" s="3" t="s">
@@ -41401,7 +41398,7 @@
     </row>
     <row r="1170" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1170" s="37" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B1170" s="40"/>
       <c r="C1170" s="3" t="s">
@@ -41416,7 +41413,7 @@
     </row>
     <row r="1171" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1171" s="37" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B1171" s="40"/>
       <c r="C1171" s="3" t="s">
@@ -41431,14 +41428,14 @@
     </row>
     <row r="1172" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1172" s="37" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B1172" s="40"/>
       <c r="C1172" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D1172" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="E1172" s="39" t="s">
         <v>9</v>
@@ -41446,7 +41443,7 @@
     </row>
     <row r="1173" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1173" s="37" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B1173" s="40"/>
       <c r="C1173" s="3" t="s">
@@ -41461,7 +41458,7 @@
     </row>
     <row r="1174" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1174" s="37" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B1174" s="40"/>
       <c r="C1174" s="3" t="s">
@@ -41476,7 +41473,7 @@
     </row>
     <row r="1175" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1175" s="37" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B1175" s="40"/>
       <c r="C1175" s="3" t="s">
@@ -41491,7 +41488,7 @@
     </row>
     <row r="1176" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1176" s="37" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="B1176" s="40"/>
       <c r="C1176" s="3" t="s">
@@ -41506,7 +41503,7 @@
     </row>
     <row r="1177" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1177" s="37" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B1177" s="40"/>
       <c r="C1177" s="3" t="s">
@@ -41521,7 +41518,7 @@
     </row>
     <row r="1178" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1178" s="37" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="B1178" s="40"/>
       <c r="C1178" s="3" t="s">
@@ -41536,7 +41533,7 @@
     </row>
     <row r="1179" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1179" s="37" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B1179" s="40"/>
       <c r="C1179" s="3" t="s">
@@ -41551,7 +41548,7 @@
     </row>
     <row r="1180" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1180" s="37" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B1180" s="40"/>
       <c r="C1180" s="3" t="s">
@@ -41566,7 +41563,7 @@
     </row>
     <row r="1181" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1181" s="37" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B1181" s="40"/>
       <c r="C1181" s="3" t="s">
@@ -41581,7 +41578,7 @@
     </row>
     <row r="1182" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1182" s="37" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B1182" s="40"/>
       <c r="C1182" s="3" t="s">
@@ -41596,7 +41593,7 @@
     </row>
     <row r="1183" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1183" s="37" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="B1183" s="40"/>
       <c r="C1183" s="3" t="s">
@@ -41611,7 +41608,7 @@
     </row>
     <row r="1184" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1184" s="37" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="B1184" s="40"/>
       <c r="C1184" s="3" t="s">
@@ -41626,7 +41623,7 @@
     </row>
     <row r="1185" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1185" s="37" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B1185" s="40"/>
       <c r="C1185" s="3" t="s">
@@ -41641,7 +41638,7 @@
     </row>
     <row r="1186" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1186" s="37" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="B1186" s="40"/>
       <c r="C1186" s="3" t="s">
@@ -41656,7 +41653,7 @@
     </row>
     <row r="1187" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1187" s="37" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="B1187" s="40"/>
       <c r="C1187" s="3" t="s">
@@ -41671,7 +41668,7 @@
     </row>
     <row r="1188" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1188" s="37" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B1188" s="40"/>
       <c r="C1188" s="3" t="s">
@@ -41686,7 +41683,7 @@
     </row>
     <row r="1189" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1189" s="37" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B1189" s="40"/>
       <c r="C1189" s="3" t="s">
@@ -41701,7 +41698,7 @@
     </row>
     <row r="1190" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1190" s="37" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B1190" s="40"/>
       <c r="C1190" s="3" t="s">
@@ -41716,7 +41713,7 @@
     </row>
     <row r="1191" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1191" s="37" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B1191" s="40"/>
       <c r="C1191" s="3" t="s">
@@ -41731,7 +41728,7 @@
     </row>
     <row r="1192" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1192" s="37" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B1192" s="40"/>
       <c r="C1192" s="3" t="s">
@@ -41746,7 +41743,7 @@
     </row>
     <row r="1193" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1193" s="37" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B1193" s="40"/>
       <c r="C1193" s="3" t="s">
@@ -41761,7 +41758,7 @@
     </row>
     <row r="1194" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1194" s="37" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="B1194" s="40"/>
       <c r="C1194" s="3" t="s">
@@ -41776,7 +41773,7 @@
     </row>
     <row r="1195" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1195" s="37" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B1195" s="40"/>
       <c r="C1195" s="3" t="s">
@@ -41791,7 +41788,7 @@
     </row>
     <row r="1196" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1196" s="37" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="B1196" s="40"/>
       <c r="C1196" s="3" t="s">
@@ -41806,7 +41803,7 @@
     </row>
     <row r="1197" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1197" s="37" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B1197" s="40"/>
       <c r="C1197" s="3" t="s">
@@ -41821,7 +41818,7 @@
     </row>
     <row r="1198" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1198" s="37" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B1198" s="40"/>
       <c r="C1198" s="3" t="s">
@@ -41836,7 +41833,7 @@
     </row>
     <row r="1199" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1199" s="37" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B1199" s="40"/>
       <c r="C1199" s="3" t="s">
@@ -41851,7 +41848,7 @@
     </row>
     <row r="1200" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1200" s="37" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B1200" s="40"/>
       <c r="C1200" s="3" t="s">
@@ -41866,7 +41863,7 @@
     </row>
     <row r="1201" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1201" s="37" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="B1201" s="40"/>
       <c r="C1201" s="3" t="s">
@@ -41881,7 +41878,7 @@
     </row>
     <row r="1202" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1202" s="37" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="B1202" s="40"/>
       <c r="C1202" s="3" t="s">
@@ -41896,7 +41893,7 @@
     </row>
     <row r="1203" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1203" s="37" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="B1203" s="40"/>
       <c r="C1203" s="3" t="s">
@@ -41911,7 +41908,7 @@
     </row>
     <row r="1204" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1204" s="37" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B1204" s="40"/>
       <c r="C1204" s="3" t="s">
@@ -41926,7 +41923,7 @@
     </row>
     <row r="1205" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1205" s="37" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="B1205" s="40"/>
       <c r="C1205" s="3" t="s">
@@ -41941,7 +41938,7 @@
     </row>
     <row r="1206" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1206" s="37" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="B1206" s="40"/>
       <c r="C1206" s="3" t="s">
@@ -41956,7 +41953,7 @@
     </row>
     <row r="1207" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1207" s="37" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B1207" s="40"/>
       <c r="C1207" s="3" t="s">
@@ -41971,7 +41968,7 @@
     </row>
     <row r="1208" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1208" s="37" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="B1208" s="40"/>
       <c r="C1208" s="3" t="s">
@@ -41986,7 +41983,7 @@
     </row>
     <row r="1209" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1209" s="37" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="B1209" s="40"/>
       <c r="C1209" s="3" t="s">
@@ -42001,7 +41998,7 @@
     </row>
     <row r="1210" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1210" s="37" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B1210" s="40"/>
       <c r="C1210" s="3" t="s">
@@ -42016,7 +42013,7 @@
     </row>
     <row r="1211" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1211" s="37" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B1211" s="40"/>
       <c r="C1211" s="3" t="s">
@@ -42031,7 +42028,7 @@
     </row>
     <row r="1212" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1212" s="37" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B1212" s="40"/>
       <c r="C1212" s="3" t="s">
@@ -42046,7 +42043,7 @@
     </row>
     <row r="1213" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1213" s="37" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B1213" s="40"/>
       <c r="C1213" s="3" t="s">
@@ -42061,7 +42058,7 @@
     </row>
     <row r="1214" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1214" s="37" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B1214" s="40"/>
       <c r="C1214" s="3" t="s">
@@ -42076,7 +42073,7 @@
     </row>
     <row r="1215" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1215" s="37" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B1215" s="40"/>
       <c r="C1215" s="3" t="s">
@@ -42091,7 +42088,7 @@
     </row>
     <row r="1216" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1216" s="37" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="B1216" s="40"/>
       <c r="C1216" s="3" t="s">
@@ -42106,7 +42103,7 @@
     </row>
     <row r="1217" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1217" s="37" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B1217" s="40"/>
       <c r="C1217" s="3" t="s">
@@ -42121,7 +42118,7 @@
     </row>
     <row r="1218" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1218" s="37" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B1218" s="40"/>
       <c r="C1218" s="3" t="s">
@@ -42136,7 +42133,7 @@
     </row>
     <row r="1219" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1219" s="41" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B1219" s="40"/>
       <c r="C1219" s="3" t="s">
@@ -42151,7 +42148,7 @@
     </row>
     <row r="1220" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1220" s="37" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="B1220" s="40"/>
       <c r="C1220" s="3" t="s">
@@ -42166,7 +42163,7 @@
     </row>
     <row r="1221" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1221" s="37" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B1221" s="40"/>
       <c r="C1221" s="3" t="s">
@@ -42181,7 +42178,7 @@
     </row>
     <row r="1222" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1222" s="37" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="B1222" s="40"/>
       <c r="C1222" s="3" t="s">
@@ -42196,7 +42193,7 @@
     </row>
     <row r="1223" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1223" s="37" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="B1223" s="40"/>
       <c r="C1223" s="3" t="s">
@@ -42211,7 +42208,7 @@
     </row>
     <row r="1224" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1224" s="37" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B1224" s="40"/>
       <c r="C1224" s="3" t="s">
@@ -42226,7 +42223,7 @@
     </row>
     <row r="1225" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1225" s="37" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="B1225" s="40"/>
       <c r="C1225" s="3" t="s">
@@ -42241,7 +42238,7 @@
     </row>
     <row r="1226" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1226" s="37" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="B1226" s="40"/>
       <c r="C1226" s="3" t="s">
@@ -42256,7 +42253,7 @@
     </row>
     <row r="1227" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1227" s="37" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B1227" s="40"/>
       <c r="C1227" s="3" t="s">
@@ -42271,7 +42268,7 @@
     </row>
     <row r="1228" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1228" s="37" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="B1228" s="40"/>
       <c r="C1228" s="3" t="s">
@@ -42286,7 +42283,7 @@
     </row>
     <row r="1229" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1229" s="37" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B1229" s="40"/>
       <c r="C1229" s="3" t="s">
@@ -42301,7 +42298,7 @@
     </row>
     <row r="1230" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1230" s="37" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="B1230" s="40"/>
       <c r="C1230" s="3" t="s">
@@ -42316,7 +42313,7 @@
     </row>
     <row r="1231" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1231" s="37" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B1231" s="40"/>
       <c r="C1231" s="3" t="s">
@@ -42331,7 +42328,7 @@
     </row>
     <row r="1232" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1232" s="37" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B1232" s="40"/>
       <c r="C1232" s="3" t="s">
@@ -42346,7 +42343,7 @@
     </row>
     <row r="1233" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1233" s="37" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B1233" s="40"/>
       <c r="C1233" s="3" t="s">
@@ -42361,7 +42358,7 @@
     </row>
     <row r="1234" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1234" s="37" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B1234" s="40"/>
       <c r="C1234" s="3" t="s">
@@ -42376,7 +42373,7 @@
     </row>
     <row r="1235" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1235" s="37" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="B1235" s="40"/>
       <c r="C1235" s="3" t="s">
@@ -42391,7 +42388,7 @@
     </row>
     <row r="1236" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1236" s="37" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="B1236" s="40"/>
       <c r="C1236" s="3" t="s">
@@ -42406,7 +42403,7 @@
     </row>
     <row r="1237" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1237" s="37" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="B1237" s="40"/>
       <c r="C1237" s="3" t="s">
@@ -42421,7 +42418,7 @@
     </row>
     <row r="1238" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1238" s="37" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B1238" s="40"/>
       <c r="C1238" s="3" t="s">
@@ -42436,7 +42433,7 @@
     </row>
     <row r="1239" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1239" s="37" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="B1239" s="40"/>
       <c r="C1239" s="3" t="s">
@@ -42451,7 +42448,7 @@
     </row>
     <row r="1240" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1240" s="37" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B1240" s="40"/>
       <c r="C1240" s="3" t="s">
@@ -42466,7 +42463,7 @@
     </row>
     <row r="1241" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1241" s="37" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B1241" s="40"/>
       <c r="C1241" s="3" t="s">
@@ -42481,7 +42478,7 @@
     </row>
     <row r="1242" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1242" s="37" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B1242" s="40"/>
       <c r="C1242" s="3" t="s">
@@ -42496,7 +42493,7 @@
     </row>
     <row r="1243" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1243" s="37" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B1243" s="40"/>
       <c r="C1243" s="3" t="s">
@@ -42511,7 +42508,7 @@
     </row>
     <row r="1244" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1244" s="37" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B1244" s="40"/>
       <c r="C1244" s="3" t="s">
@@ -42526,7 +42523,7 @@
     </row>
     <row r="1245" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1245" s="37" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B1245" s="40"/>
       <c r="C1245" s="3" t="s">
@@ -42541,7 +42538,7 @@
     </row>
     <row r="1246" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1246" s="37" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B1246" s="40"/>
       <c r="C1246" s="3" t="s">
@@ -42556,7 +42553,7 @@
     </row>
     <row r="1247" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1247" s="37" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B1247" s="40"/>
       <c r="C1247" s="3" t="s">
@@ -42571,7 +42568,7 @@
     </row>
     <row r="1248" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1248" s="37" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B1248" s="40"/>
       <c r="C1248" s="3" t="s">
@@ -42586,7 +42583,7 @@
     </row>
     <row r="1249" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1249" s="37" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B1249" s="40"/>
       <c r="C1249" s="3" t="s">
@@ -42601,7 +42598,7 @@
     </row>
     <row r="1250" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1250" s="37" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="B1250" s="40"/>
       <c r="C1250" s="3" t="s">
@@ -42616,7 +42613,7 @@
     </row>
     <row r="1251" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1251" s="37" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="B1251" s="40"/>
       <c r="C1251" s="3" t="s">
@@ -42629,29 +42626,79 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1252" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1252" s="37" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B1252" s="40"/>
+      <c r="C1252" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1252" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1252" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1253" s="37" t="s">
         <v>1464</v>
       </c>
-    </row>
-    <row r="1253" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1253" s="37" t="s">
+      <c r="B1253" s="40"/>
+      <c r="C1253" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1253" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1253" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1254" s="37" t="s">
         <v>1465</v>
       </c>
-    </row>
-    <row r="1254" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1254" s="37" t="s">
+      <c r="B1254" s="40"/>
+      <c r="C1254" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1254" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1254" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1255" s="37" t="s">
         <v>1466</v>
       </c>
-    </row>
-    <row r="1255" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1255" s="37" t="s">
+      <c r="B1255" s="40"/>
+      <c r="C1255" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1255" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1255" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1256" s="37" t="s">
         <v>1467</v>
       </c>
-    </row>
-    <row r="1256" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1256" s="37" t="s">
-        <v>1468</v>
+      <c r="B1256" s="40"/>
+      <c r="C1256" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1256" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1256" s="39" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -48342,7 +48389,7 @@
       <formula>NOT(ISERROR(SEARCH("Pass",D876)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1079:E1251">
+  <conditionalFormatting sqref="E1079:E1256">
     <cfRule type="cellIs" dxfId="62" priority="58" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
@@ -48353,7 +48400,7 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1080:D1251">
+  <conditionalFormatting sqref="D1080:D1256">
     <cfRule type="containsText" dxfId="59" priority="61" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D1080)))</formula>
     </cfRule>
@@ -48578,14 +48625,14 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E867 E875:E1251" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E867 E875:E1256" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E868:E874" xr:uid="{7959F95A-A2DF-42E0-AAF4-9D18A0E7517A}">
       <formula1>"High,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1251" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1256" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -48703,8 +48750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48743,7 +48790,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -48760,7 +48807,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -48780,7 +48827,7 @@
         <v>300</v>
       </c>
       <c r="D3" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="E3" t="s">
         <v>874</v>
@@ -48812,10 +48859,10 @@
         <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="E4" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -48841,10 +48888,10 @@
         <v>406</v>
       </c>
       <c r="D5" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="E5" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
@@ -48870,10 +48917,10 @@
         <v>926</v>
       </c>
       <c r="D6" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="E6" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="F6" t="s">
         <v>927</v>
@@ -48907,10 +48954,10 @@
         <v>939</v>
       </c>
       <c r="D8" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E8" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F8" t="s">
         <v>27</v>
@@ -48919,7 +48966,7 @@
         <v>22</v>
       </c>
       <c r="J8" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -48933,10 +48980,10 @@
         <v>942</v>
       </c>
       <c r="D9" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E9" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -48945,7 +48992,7 @@
         <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -48956,13 +49003,13 @@
         <v>944</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D10" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="E10" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F10" t="s">
         <v>954</v>
@@ -48971,7 +49018,7 @@
         <v>955</v>
       </c>
       <c r="J10" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -48985,10 +49032,10 @@
         <v>947</v>
       </c>
       <c r="D11" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E11" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F11" t="s">
         <v>954</v>
@@ -48997,7 +49044,7 @@
         <v>955</v>
       </c>
       <c r="J11" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -49011,10 +49058,10 @@
         <v>950</v>
       </c>
       <c r="D12" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E12" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="F12" t="s">
         <v>930</v>
@@ -49023,7 +49070,7 @@
         <v>22</v>
       </c>
       <c r="J12" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -49037,10 +49084,10 @@
         <v>953</v>
       </c>
       <c r="D13" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E13" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F13" t="s">
         <v>954</v>
@@ -49049,7 +49096,7 @@
         <v>955</v>
       </c>
       <c r="J13" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -49063,10 +49110,10 @@
         <v>958</v>
       </c>
       <c r="D14" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E14" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="F14" t="s">
         <v>954</v>
@@ -49075,7 +49122,7 @@
         <v>955</v>
       </c>
       <c r="J14" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -49089,10 +49136,10 @@
         <v>961</v>
       </c>
       <c r="D15" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E15" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="F15" t="s">
         <v>954</v>
@@ -49101,7 +49148,7 @@
         <v>955</v>
       </c>
       <c r="J15" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -49115,10 +49162,10 @@
         <v>964</v>
       </c>
       <c r="D16" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E16" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="F16" t="s">
         <v>954</v>
@@ -49127,7 +49174,7 @@
         <v>955</v>
       </c>
       <c r="J16" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -49141,10 +49188,10 @@
         <v>967</v>
       </c>
       <c r="D17" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="E17" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="F17" t="s">
         <v>954</v>
@@ -49153,7 +49200,7 @@
         <v>955</v>
       </c>
       <c r="J17" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -49167,10 +49214,10 @@
         <v>970</v>
       </c>
       <c r="D18" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E18" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="F18" t="s">
         <v>954</v>
@@ -49179,7 +49226,7 @@
         <v>955</v>
       </c>
       <c r="J18" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -49188,7 +49235,7 @@
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
@@ -49198,7 +49245,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>20</v>
@@ -49210,7 +49257,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
@@ -49221,16 +49268,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>1177</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="D24" t="s">
         <v>1178</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="30" t="s">
         <v>1179</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>1180</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
@@ -49241,7 +49288,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>24</v>
@@ -49250,10 +49297,10 @@
         <v>300</v>
       </c>
       <c r="D25" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="E25" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
@@ -49264,7 +49311,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>58</v>
@@ -49273,10 +49320,10 @@
         <v>124</v>
       </c>
       <c r="D26" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="E26" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F26" t="s">
         <v>27</v>
@@ -49287,7 +49334,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>405</v>
@@ -49296,10 +49343,10 @@
         <v>406</v>
       </c>
       <c r="D27" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="E27" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="F27" t="s">
         <v>954</v>
@@ -49310,7 +49357,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>925</v>
@@ -49319,10 +49366,10 @@
         <v>926</v>
       </c>
       <c r="D28" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="E28" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="F28" t="s">
         <v>954</v>
@@ -49333,19 +49380,19 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>929</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D29" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="E29" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="F29" t="s">
         <v>954</v>
@@ -49356,19 +49403,19 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>938</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D30" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="E30" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="F30" t="s">
         <v>954</v>

</xml_diff>

<commit_message>
Uploaded the testcase and datasheet file
Signed-off-by: sourabhnavatargroup <sourabh@navatargroup.com>
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin Garg\git\PE4.7Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\File merge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C775877D-061D-49F3-8C35-5B4BA3535598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5691" uniqueCount="1573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5703" uniqueCount="1576">
   <si>
     <t>Module_Name</t>
   </si>
@@ -4523,9 +4522,6 @@
   </si>
   <si>
     <t>ATCETc207_VerifyUIOfFilterSectionOnFundRecordType</t>
-  </si>
-  <si>
-    <t>ATCETc208_VerifyUIOfFilterSectionOnPrivateEquityRecordType</t>
   </si>
   <si>
     <t>ATCETc209_CreateAccountAndContact</t>
@@ -4751,11 +4747,23 @@
   <si>
     <t>Skip: Priority and dependency of ARTc004_CreateCustomFields testcase was high so cannot continue with the execution.</t>
   </si>
+  <si>
+    <t>ATCETc208_VerifyUIOfFilterSectionOnThemeRecordType</t>
+  </si>
+  <si>
+    <t>ATCETc221_ReplaceFirstColumnsWithAnotherColuman</t>
+  </si>
+  <si>
+    <t>ATCETc222_VerifyMetaDataOnAccuntRecord</t>
+  </si>
+  <si>
+    <t>ATCETc223_VerifyTheResultsOnContactsAcuityTab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -5188,9 +5196,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="231">
     <dxf>
@@ -8266,22 +8274,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK26"/>
   <sheetViews>
     <sheetView topLeftCell="C5" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="8.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="1025" width="8.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="7" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="43.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:9" ht="15.6">
+    <row r="1" spans="8:9" ht="15.75">
       <c r="H1" s="35" t="s">
         <v>0</v>
       </c>
@@ -8499,7 +8507,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I26 I2:I25" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I26 I2:I25">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8509,23 +8517,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA1344"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA1347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1003" workbookViewId="0">
-      <selection activeCell="A1018" sqref="A1018:XFD1018"/>
+    <sheetView tabSelected="1" topLeftCell="A1331" workbookViewId="0">
+      <selection activeCell="A1342" sqref="A1342"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="87.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="87.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999">
+    <row r="1" spans="1:5" ht="17.25">
       <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
@@ -23496,7 +23504,7 @@
     </row>
     <row r="956" spans="1:5">
       <c r="A956" s="15" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B956" s="15"/>
       <c r="C956" s="13" t="s">
@@ -23511,7 +23519,7 @@
     </row>
     <row r="957" spans="1:5">
       <c r="A957" s="15" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B957" s="15"/>
       <c r="C957" s="13" t="s">
@@ -23526,7 +23534,7 @@
     </row>
     <row r="958" spans="1:5">
       <c r="A958" s="15" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="B958" s="15"/>
       <c r="C958" s="13" t="s">
@@ -23563,7 +23571,7 @@
         <v>22</v>
       </c>
       <c r="D960" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E960" s="30" t="s">
         <v>36</v>
@@ -23571,7 +23579,7 @@
     </row>
     <row r="961" spans="1:5">
       <c r="A961" s="15" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B961" s="15"/>
       <c r="C961" s="13" t="s">
@@ -23586,7 +23594,7 @@
     </row>
     <row r="962" spans="1:5">
       <c r="A962" s="15" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="B962" s="15"/>
       <c r="C962" s="13" t="s">
@@ -23601,7 +23609,7 @@
     </row>
     <row r="963" spans="1:5">
       <c r="A963" s="15" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B963" s="15"/>
       <c r="C963" s="13" t="s">
@@ -23616,7 +23624,7 @@
     </row>
     <row r="964" spans="1:5">
       <c r="A964" s="15" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B964" s="15"/>
       <c r="C964" s="13" t="s">
@@ -23631,7 +23639,7 @@
     </row>
     <row r="965" spans="1:5">
       <c r="A965" s="15" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B965" s="15"/>
       <c r="C965" s="13" t="s">
@@ -23646,7 +23654,7 @@
     </row>
     <row r="966" spans="1:5">
       <c r="A966" s="15" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B966" s="15"/>
       <c r="C966" s="13" t="s">
@@ -23661,7 +23669,7 @@
     </row>
     <row r="967" spans="1:5">
       <c r="A967" s="15" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="B967" s="15"/>
       <c r="C967" s="13" t="s">
@@ -23856,7 +23864,7 @@
     </row>
     <row r="980" spans="1:5">
       <c r="A980" s="15" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="B980" s="15"/>
       <c r="C980" s="13" t="s">
@@ -23871,7 +23879,7 @@
     </row>
     <row r="981" spans="1:5">
       <c r="A981" s="15" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="B981" s="15"/>
       <c r="C981" s="13" t="s">
@@ -23886,7 +23894,7 @@
     </row>
     <row r="982" spans="1:5">
       <c r="A982" s="15" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B982" s="15"/>
       <c r="C982" s="13" t="s">
@@ -23901,7 +23909,7 @@
     </row>
     <row r="983" spans="1:5">
       <c r="A983" s="15" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="B983" s="15"/>
       <c r="C983" s="13" t="s">
@@ -23916,7 +23924,7 @@
     </row>
     <row r="984" spans="1:5">
       <c r="A984" s="15" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B984" s="15"/>
       <c r="C984" s="13" t="s">
@@ -23931,7 +23939,7 @@
     </row>
     <row r="985" spans="1:5">
       <c r="A985" s="15" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B985" s="15"/>
       <c r="C985" s="13" t="s">
@@ -23961,7 +23969,7 @@
     </row>
     <row r="987" spans="1:5">
       <c r="A987" s="15" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="B987" s="15"/>
       <c r="C987" s="13" t="s">
@@ -23976,7 +23984,7 @@
     </row>
     <row r="988" spans="1:5">
       <c r="A988" s="15" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B988" s="15"/>
       <c r="C988" s="13" t="s">
@@ -24229,7 +24237,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1005" spans="1:5" ht="15" thickBot="1">
+    <row r="1005" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1005" s="15" t="s">
         <v>1055</v>
       </c>
@@ -24244,7 +24252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1006" spans="1:5" ht="15" thickBot="1">
+    <row r="1006" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1006" s="15" t="s">
         <v>1056</v>
       </c>
@@ -24259,7 +24267,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1007" spans="1:5" ht="15" thickBot="1">
+    <row r="1007" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1007" s="15" t="s">
         <v>1057</v>
       </c>
@@ -24274,7 +24282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1008" spans="1:5" ht="15" thickBot="1">
+    <row r="1008" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1008" s="15" t="s">
         <v>1058</v>
       </c>
@@ -24289,7 +24297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1009" spans="1:5" ht="15" thickBot="1">
+    <row r="1009" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1009" s="15" t="s">
         <v>1059</v>
       </c>
@@ -24304,7 +24312,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1010" spans="1:5" ht="15" thickBot="1">
+    <row r="1010" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1010" s="15" t="s">
         <v>1060</v>
       </c>
@@ -24319,7 +24327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1011" spans="1:5" ht="15" thickBot="1">
+    <row r="1011" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1011" s="15" t="s">
         <v>1061</v>
       </c>
@@ -24334,7 +24342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1012" spans="1:5" ht="15" thickBot="1">
+    <row r="1012" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1012" s="15" t="s">
         <v>1062</v>
       </c>
@@ -24349,7 +24357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1013" spans="1:5" ht="15" thickBot="1">
+    <row r="1013" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1013" s="15" t="s">
         <v>1063</v>
       </c>
@@ -24364,7 +24372,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1014" spans="1:5" ht="15" thickBot="1">
+    <row r="1014" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1014" s="15" t="s">
         <v>1064</v>
       </c>
@@ -24379,7 +24387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1015" spans="1:5" ht="15" thickBot="1">
+    <row r="1015" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1015" s="15" t="s">
         <v>1065</v>
       </c>
@@ -24394,7 +24402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1016" spans="1:5" ht="15" thickBot="1">
+    <row r="1016" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1016" s="15" t="s">
         <v>1066</v>
       </c>
@@ -24409,22 +24417,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1017" spans="1:5" ht="15" thickBot="1">
+    <row r="1017" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1017" s="15" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B1017" s="15"/>
       <c r="C1017" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D1017" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="E1017" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="1018" spans="1:5" ht="15" thickBot="1">
+    <row r="1018" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1018" s="15" t="s">
         <v>1067</v>
       </c>
@@ -25624,9 +25632,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1098" spans="1:5" ht="15" thickBot="1">
+    <row r="1098" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1098" s="15" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B1098" s="15"/>
       <c r="C1098" s="13" t="s">
@@ -25639,9 +25647,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1099" spans="1:5" ht="15" thickBot="1">
+    <row r="1099" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1099" s="15" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="B1099" s="15"/>
       <c r="C1099" s="13" t="s">
@@ -25654,9 +25662,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1100" spans="1:5" ht="15" thickBot="1">
+    <row r="1100" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1100" s="15" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B1100" s="15"/>
       <c r="C1100" s="13" t="s">
@@ -25671,7 +25679,7 @@
     </row>
     <row r="1101" spans="1:5">
       <c r="A1101" s="15" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B1101" s="15"/>
       <c r="C1101" s="13" t="s">
@@ -25686,7 +25694,7 @@
     </row>
     <row r="1102" spans="1:5">
       <c r="A1102" s="15" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B1102" s="15"/>
       <c r="C1102" s="13" t="s">
@@ -25701,7 +25709,7 @@
     </row>
     <row r="1103" spans="1:5">
       <c r="A1103" s="15" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B1103" s="15"/>
       <c r="C1103" s="13" t="s">
@@ -25714,9 +25722,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1104" spans="1:5" ht="15" thickBot="1">
+    <row r="1104" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1104" s="15" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B1104" s="15"/>
       <c r="C1104" s="13" t="s">
@@ -25729,39 +25737,39 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1105" spans="1:5" ht="15" thickBot="1">
+    <row r="1105" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1105" s="15" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B1105" s="15"/>
       <c r="C1105" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D1105" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E1105" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1106" s="15" t="s">
         <v>1532</v>
-      </c>
-      <c r="E1105" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="1106" spans="1:5" ht="15" thickBot="1">
-      <c r="A1106" s="15" t="s">
-        <v>1533</v>
       </c>
       <c r="B1106" s="15"/>
       <c r="C1106" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D1106" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="E1106" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="1107" spans="1:5" ht="15" thickBot="1">
+    <row r="1107" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1107" s="15" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B1107" s="15"/>
       <c r="C1107" s="13" t="s">
@@ -25776,7 +25784,7 @@
     </row>
     <row r="1108" spans="1:5">
       <c r="A1108" s="15" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="B1108" s="15"/>
       <c r="C1108" s="13" t="s">
@@ -25791,7 +25799,7 @@
     </row>
     <row r="1109" spans="1:5">
       <c r="A1109" s="15" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="B1109" s="15"/>
       <c r="C1109" s="13" t="s">
@@ -25806,7 +25814,7 @@
     </row>
     <row r="1110" spans="1:5">
       <c r="A1110" s="15" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="B1110" s="15"/>
       <c r="C1110" s="13" t="s">
@@ -25821,7 +25829,7 @@
     </row>
     <row r="1111" spans="1:5">
       <c r="A1111" s="15" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="B1111" s="15"/>
       <c r="C1111" s="13" t="s">
@@ -25836,7 +25844,7 @@
     </row>
     <row r="1112" spans="1:5">
       <c r="A1112" s="15" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="B1112" s="15"/>
       <c r="C1112" s="13" t="s">
@@ -25851,7 +25859,7 @@
     </row>
     <row r="1113" spans="1:5">
       <c r="A1113" s="15" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="B1113" s="15"/>
       <c r="C1113" s="13" t="s">
@@ -25864,9 +25872,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1114" spans="1:5" ht="15" thickBot="1">
+    <row r="1114" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1114" s="15" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="B1114" s="15"/>
       <c r="C1114" s="13" t="s">
@@ -25879,9 +25887,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1115" spans="1:5" ht="15" thickBot="1">
+    <row r="1115" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1115" s="15" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B1115" s="15"/>
       <c r="C1115" s="13" t="s">
@@ -25894,9 +25902,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1116" spans="1:5" ht="15" thickBot="1">
+    <row r="1116" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1116" s="15" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B1116" s="15"/>
       <c r="C1116" s="13" t="s">
@@ -25909,9 +25917,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1117" spans="1:5" ht="15" thickBot="1">
+    <row r="1117" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1117" s="15" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B1117" s="15"/>
       <c r="C1117" s="13" t="s">
@@ -25924,9 +25932,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1118" spans="1:5" ht="15" thickBot="1">
+    <row r="1118" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1118" s="15" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="B1118" s="15"/>
       <c r="C1118" s="13" t="s">
@@ -25939,9 +25947,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1119" spans="1:5" ht="15" thickBot="1">
+    <row r="1119" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1119" s="15" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="B1119" s="15"/>
       <c r="C1119" s="13" t="s">
@@ -25954,9 +25962,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1120" spans="1:5" ht="15" thickBot="1">
+    <row r="1120" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1120" s="15" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="B1120" s="15"/>
       <c r="C1120" s="13" t="s">
@@ -25969,9 +25977,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1121" spans="1:5" ht="15" thickBot="1">
+    <row r="1121" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1121" s="15" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="B1121" s="15"/>
       <c r="C1121" s="13" t="s">
@@ -25984,9 +25992,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1122" spans="1:5" ht="15" thickBot="1">
+    <row r="1122" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1122" s="15" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="B1122" s="15"/>
       <c r="C1122" s="13" t="s">
@@ -25999,9 +26007,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1123" spans="1:5" ht="15" thickBot="1">
+    <row r="1123" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1123" s="41" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="B1123" s="15"/>
       <c r="C1123" s="13" t="s">
@@ -26014,9 +26022,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1124" spans="1:5" ht="15" thickBot="1">
+    <row r="1124" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1124" s="41" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="B1124" s="15"/>
       <c r="C1124" s="13" t="s">
@@ -26029,7 +26037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1125" spans="1:5" ht="15" thickBot="1">
+    <row r="1125" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1125" s="37" t="s">
         <v>1147</v>
       </c>
@@ -26044,7 +26052,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1126" spans="1:5" ht="15" thickBot="1">
+    <row r="1126" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1126" s="37" t="s">
         <v>1148</v>
       </c>
@@ -26059,7 +26067,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1127" spans="1:5" ht="15" thickBot="1">
+    <row r="1127" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1127" s="37" t="s">
         <v>1149</v>
       </c>
@@ -26074,7 +26082,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1128" spans="1:5" ht="15" thickBot="1">
+    <row r="1128" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1128" s="37" t="s">
         <v>1150</v>
       </c>
@@ -26089,7 +26097,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1129" spans="1:5" ht="15" thickBot="1">
+    <row r="1129" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1129" s="37" t="s">
         <v>1151</v>
       </c>
@@ -26104,7 +26112,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1130" spans="1:5" ht="15" thickBot="1">
+    <row r="1130" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1130" s="37" t="s">
         <v>1152</v>
       </c>
@@ -26119,7 +26127,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1131" spans="1:5" ht="15" thickBot="1">
+    <row r="1131" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1131" s="37" t="s">
         <v>1153</v>
       </c>
@@ -26134,7 +26142,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1132" spans="1:5" ht="15" thickBot="1">
+    <row r="1132" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1132" s="37" t="s">
         <v>1154</v>
       </c>
@@ -26149,7 +26157,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1133" spans="1:5" ht="15" thickBot="1">
+    <row r="1133" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1133" s="37" t="s">
         <v>1305</v>
       </c>
@@ -26164,7 +26172,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1134" spans="1:5" ht="15" thickBot="1">
+    <row r="1134" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1134" s="37" t="s">
         <v>1155</v>
       </c>
@@ -26179,7 +26187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1135" spans="1:5" ht="15" thickBot="1">
+    <row r="1135" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1135" s="37" t="s">
         <v>1156</v>
       </c>
@@ -26194,7 +26202,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1136" spans="1:5" ht="15" thickBot="1">
+    <row r="1136" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1136" s="37" t="s">
         <v>1157</v>
       </c>
@@ -26209,7 +26217,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1137" spans="1:5" ht="15" thickBot="1">
+    <row r="1137" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1137" s="37" t="s">
         <v>1158</v>
       </c>
@@ -26224,7 +26232,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1138" spans="1:5" ht="15" thickBot="1">
+    <row r="1138" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1138" s="37" t="s">
         <v>1159</v>
       </c>
@@ -26239,7 +26247,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1139" spans="1:5" ht="15" thickBot="1">
+    <row r="1139" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1139" s="37" t="s">
         <v>1306</v>
       </c>
@@ -26254,7 +26262,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1140" spans="1:5" ht="15" thickBot="1">
+    <row r="1140" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1140" s="37" t="s">
         <v>1307</v>
       </c>
@@ -26269,7 +26277,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1141" spans="1:5" ht="15" thickBot="1">
+    <row r="1141" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1141" s="37" t="s">
         <v>1308</v>
       </c>
@@ -26284,7 +26292,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1142" spans="1:5" ht="15" thickBot="1">
+    <row r="1142" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1142" s="37" t="s">
         <v>1309</v>
       </c>
@@ -26299,7 +26307,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1143" spans="1:5" ht="15" thickBot="1">
+    <row r="1143" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1143" s="37" t="s">
         <v>1310</v>
       </c>
@@ -26314,7 +26322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1144" spans="1:5" ht="15" thickBot="1">
+    <row r="1144" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1144" s="37" t="s">
         <v>1311</v>
       </c>
@@ -26329,7 +26337,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1145" spans="1:5" ht="15" thickBot="1">
+    <row r="1145" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1145" s="37" t="s">
         <v>1312</v>
       </c>
@@ -26344,7 +26352,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1146" spans="1:5" ht="15" thickBot="1">
+    <row r="1146" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1146" s="37" t="s">
         <v>1313</v>
       </c>
@@ -26359,7 +26367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1147" spans="1:5" ht="15" thickBot="1">
+    <row r="1147" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1147" s="37" t="s">
         <v>1314</v>
       </c>
@@ -26374,7 +26382,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1148" spans="1:5" ht="15" thickBot="1">
+    <row r="1148" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1148" s="37" t="s">
         <v>1315</v>
       </c>
@@ -26389,7 +26397,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1149" spans="1:5" ht="15" thickBot="1">
+    <row r="1149" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1149" s="37" t="s">
         <v>1316</v>
       </c>
@@ -26404,7 +26412,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1150" spans="1:5" ht="15" thickBot="1">
+    <row r="1150" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1150" s="37" t="s">
         <v>1317</v>
       </c>
@@ -26419,7 +26427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1151" spans="1:5" ht="15" thickBot="1">
+    <row r="1151" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1151" s="37" t="s">
         <v>1318</v>
       </c>
@@ -26434,7 +26442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1152" spans="1:5" ht="15" thickBot="1">
+    <row r="1152" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1152" s="37" t="s">
         <v>1319</v>
       </c>
@@ -26449,7 +26457,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1153" spans="1:5" ht="15" thickBot="1">
+    <row r="1153" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1153" s="37" t="s">
         <v>1320</v>
       </c>
@@ -26464,7 +26472,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1154" spans="1:5" ht="15" thickBot="1">
+    <row r="1154" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1154" s="37" t="s">
         <v>1321</v>
       </c>
@@ -26479,7 +26487,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1155" spans="1:5" ht="15" thickBot="1">
+    <row r="1155" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1155" s="37" t="s">
         <v>1322</v>
       </c>
@@ -26494,7 +26502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1156" spans="1:5" ht="15" thickBot="1">
+    <row r="1156" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1156" s="37" t="s">
         <v>1323</v>
       </c>
@@ -26509,7 +26517,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1157" spans="1:5" ht="15" thickBot="1">
+    <row r="1157" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1157" s="37" t="s">
         <v>1324</v>
       </c>
@@ -26524,7 +26532,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1158" spans="1:5" ht="15" thickBot="1">
+    <row r="1158" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1158" s="37" t="s">
         <v>1325</v>
       </c>
@@ -26539,7 +26547,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1159" spans="1:5" ht="15" thickBot="1">
+    <row r="1159" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1159" s="37" t="s">
         <v>1326</v>
       </c>
@@ -26554,7 +26562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1160" spans="1:5" ht="15" thickBot="1">
+    <row r="1160" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1160" s="37" t="s">
         <v>1327</v>
       </c>
@@ -26569,7 +26577,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1161" spans="1:5" ht="15" thickBot="1">
+    <row r="1161" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1161" s="37" t="s">
         <v>1328</v>
       </c>
@@ -26584,7 +26592,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1162" spans="1:5" ht="15" thickBot="1">
+    <row r="1162" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1162" s="37" t="s">
         <v>1329</v>
       </c>
@@ -26599,7 +26607,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1163" spans="1:5" ht="15" thickBot="1">
+    <row r="1163" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1163" s="37" t="s">
         <v>1330</v>
       </c>
@@ -26614,7 +26622,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1164" spans="1:5" ht="15" thickBot="1">
+    <row r="1164" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1164" s="37" t="s">
         <v>1331</v>
       </c>
@@ -26629,7 +26637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1165" spans="1:5" ht="15" thickBot="1">
+    <row r="1165" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1165" s="37" t="s">
         <v>1332</v>
       </c>
@@ -26644,7 +26652,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1166" spans="1:5" ht="15" thickBot="1">
+    <row r="1166" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1166" s="37" t="s">
         <v>1333</v>
       </c>
@@ -26659,7 +26667,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1167" spans="1:5" ht="15" thickBot="1">
+    <row r="1167" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1167" s="37" t="s">
         <v>1334</v>
       </c>
@@ -26674,7 +26682,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1168" spans="1:5" ht="15" thickBot="1">
+    <row r="1168" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1168" s="37" t="s">
         <v>1335</v>
       </c>
@@ -26689,7 +26697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1169" spans="1:5" ht="15" thickBot="1">
+    <row r="1169" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1169" s="37" t="s">
         <v>1336</v>
       </c>
@@ -26704,7 +26712,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1170" spans="1:5" ht="15" thickBot="1">
+    <row r="1170" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1170" s="37" t="s">
         <v>1337</v>
       </c>
@@ -26719,7 +26727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1171" spans="1:5" ht="15" thickBot="1">
+    <row r="1171" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1171" s="37" t="s">
         <v>1338</v>
       </c>
@@ -26734,7 +26742,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1172" spans="1:5" ht="15" thickBot="1">
+    <row r="1172" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1172" s="37" t="s">
         <v>1339</v>
       </c>
@@ -26749,7 +26757,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1173" spans="1:5" ht="15" thickBot="1">
+    <row r="1173" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1173" s="37" t="s">
         <v>1340</v>
       </c>
@@ -26764,7 +26772,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1174" spans="1:5" ht="15" thickBot="1">
+    <row r="1174" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1174" s="37" t="s">
         <v>1341</v>
       </c>
@@ -26779,7 +26787,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1175" spans="1:5" ht="15" thickBot="1">
+    <row r="1175" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1175" s="37" t="s">
         <v>1342</v>
       </c>
@@ -26794,7 +26802,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1176" spans="1:5" ht="15" thickBot="1">
+    <row r="1176" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1176" s="37" t="s">
         <v>1343</v>
       </c>
@@ -26809,7 +26817,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1177" spans="1:5" ht="15" thickBot="1">
+    <row r="1177" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1177" s="37" t="s">
         <v>1344</v>
       </c>
@@ -26824,7 +26832,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1178" spans="1:5" ht="15" thickBot="1">
+    <row r="1178" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1178" s="37" t="s">
         <v>1345</v>
       </c>
@@ -26839,7 +26847,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1179" spans="1:5" ht="15" thickBot="1">
+    <row r="1179" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1179" s="37" t="s">
         <v>1346</v>
       </c>
@@ -26854,7 +26862,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1180" spans="1:5" ht="15" thickBot="1">
+    <row r="1180" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1180" s="37" t="s">
         <v>1347</v>
       </c>
@@ -26869,7 +26877,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1181" spans="1:5" ht="15" thickBot="1">
+    <row r="1181" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1181" s="37" t="s">
         <v>1348</v>
       </c>
@@ -26884,7 +26892,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1182" spans="1:5" ht="15" thickBot="1">
+    <row r="1182" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1182" s="37" t="s">
         <v>1349</v>
       </c>
@@ -26899,7 +26907,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1183" spans="1:5" ht="15" thickBot="1">
+    <row r="1183" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1183" s="37" t="s">
         <v>1350</v>
       </c>
@@ -26914,7 +26922,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1184" spans="1:5" ht="15" thickBot="1">
+    <row r="1184" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1184" s="37" t="s">
         <v>1351</v>
       </c>
@@ -26929,7 +26937,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1185" spans="1:5" ht="15" thickBot="1">
+    <row r="1185" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1185" s="37" t="s">
         <v>1352</v>
       </c>
@@ -26944,7 +26952,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1186" spans="1:5" ht="15" thickBot="1">
+    <row r="1186" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1186" s="37" t="s">
         <v>1353</v>
       </c>
@@ -26959,7 +26967,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1187" spans="1:5" ht="15" thickBot="1">
+    <row r="1187" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1187" s="37" t="s">
         <v>1354</v>
       </c>
@@ -26974,7 +26982,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1188" spans="1:5" ht="15" thickBot="1">
+    <row r="1188" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1188" s="37" t="s">
         <v>1355</v>
       </c>
@@ -26989,7 +26997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1189" spans="1:5" ht="15" thickBot="1">
+    <row r="1189" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1189" s="37" t="s">
         <v>1356</v>
       </c>
@@ -27004,7 +27012,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1190" spans="1:5" ht="15" thickBot="1">
+    <row r="1190" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1190" s="37" t="s">
         <v>1357</v>
       </c>
@@ -27019,7 +27027,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1191" spans="1:5" ht="15" thickBot="1">
+    <row r="1191" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1191" s="37" t="s">
         <v>1358</v>
       </c>
@@ -27034,7 +27042,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1192" spans="1:5" ht="15" thickBot="1">
+    <row r="1192" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1192" s="37" t="s">
         <v>1359</v>
       </c>
@@ -27049,7 +27057,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1193" spans="1:5" ht="15" thickBot="1">
+    <row r="1193" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1193" s="37" t="s">
         <v>1360</v>
       </c>
@@ -27064,7 +27072,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1194" spans="1:5" ht="15" thickBot="1">
+    <row r="1194" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1194" s="37" t="s">
         <v>1361</v>
       </c>
@@ -27079,7 +27087,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1195" spans="1:5" ht="15" thickBot="1">
+    <row r="1195" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1195" s="37" t="s">
         <v>1362</v>
       </c>
@@ -27094,7 +27102,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1196" spans="1:5" ht="15" thickBot="1">
+    <row r="1196" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1196" s="37" t="s">
         <v>1363</v>
       </c>
@@ -27109,7 +27117,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1197" spans="1:5" ht="15" thickBot="1">
+    <row r="1197" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1197" s="37" t="s">
         <v>1364</v>
       </c>
@@ -27124,7 +27132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1198" spans="1:5" ht="15" thickBot="1">
+    <row r="1198" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1198" s="37" t="s">
         <v>1365</v>
       </c>
@@ -27139,7 +27147,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1199" spans="1:5" ht="15" thickBot="1">
+    <row r="1199" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1199" s="37" t="s">
         <v>1366</v>
       </c>
@@ -27154,7 +27162,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1200" spans="1:5" ht="15" thickBot="1">
+    <row r="1200" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1200" s="37" t="s">
         <v>1367</v>
       </c>
@@ -27169,7 +27177,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1201" spans="1:5" ht="15" thickBot="1">
+    <row r="1201" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1201" s="37" t="s">
         <v>1368</v>
       </c>
@@ -27184,7 +27192,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1202" spans="1:5" ht="15" thickBot="1">
+    <row r="1202" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1202" s="37" t="s">
         <v>1369</v>
       </c>
@@ -27199,7 +27207,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1203" spans="1:5" ht="15" thickBot="1">
+    <row r="1203" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1203" s="37" t="s">
         <v>1370</v>
       </c>
@@ -27214,7 +27222,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1204" spans="1:5" ht="15" thickBot="1">
+    <row r="1204" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1204" s="37" t="s">
         <v>1371</v>
       </c>
@@ -27229,7 +27237,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1205" spans="1:5" ht="15" thickBot="1">
+    <row r="1205" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1205" s="37" t="s">
         <v>1372</v>
       </c>
@@ -27244,7 +27252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1206" spans="1:5" ht="15" thickBot="1">
+    <row r="1206" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1206" s="37" t="s">
         <v>1373</v>
       </c>
@@ -27259,7 +27267,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1207" spans="1:5" ht="15" thickBot="1">
+    <row r="1207" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1207" s="37" t="s">
         <v>1374</v>
       </c>
@@ -27274,7 +27282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1208" spans="1:5" ht="15" thickBot="1">
+    <row r="1208" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1208" s="37" t="s">
         <v>1375</v>
       </c>
@@ -27289,7 +27297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1209" spans="1:5" ht="15" thickBot="1">
+    <row r="1209" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1209" s="37" t="s">
         <v>1376</v>
       </c>
@@ -27304,7 +27312,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1210" spans="1:5" ht="15" thickBot="1">
+    <row r="1210" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1210" s="37" t="s">
         <v>1377</v>
       </c>
@@ -27319,7 +27327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1211" spans="1:5" ht="15" thickBot="1">
+    <row r="1211" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1211" s="37" t="s">
         <v>1378</v>
       </c>
@@ -27334,7 +27342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1212" spans="1:5" ht="15" thickBot="1">
+    <row r="1212" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1212" s="37" t="s">
         <v>1379</v>
       </c>
@@ -27349,7 +27357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1213" spans="1:5" ht="15" thickBot="1">
+    <row r="1213" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1213" s="37" t="s">
         <v>1380</v>
       </c>
@@ -27364,7 +27372,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1214" spans="1:5" ht="15" thickBot="1">
+    <row r="1214" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1214" s="37" t="s">
         <v>1381</v>
       </c>
@@ -27379,7 +27387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1215" spans="1:5" ht="15" thickBot="1">
+    <row r="1215" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1215" s="37" t="s">
         <v>1382</v>
       </c>
@@ -27394,7 +27402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1216" spans="1:5" ht="15" thickBot="1">
+    <row r="1216" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1216" s="37" t="s">
         <v>1383</v>
       </c>
@@ -27409,7 +27417,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1217" spans="1:5" ht="15" thickBot="1">
+    <row r="1217" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1217" s="37" t="s">
         <v>1384</v>
       </c>
@@ -27424,7 +27432,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1218" spans="1:5" ht="15" thickBot="1">
+    <row r="1218" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1218" s="37" t="s">
         <v>1385</v>
       </c>
@@ -27439,7 +27447,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1219" spans="1:5" ht="15" thickBot="1">
+    <row r="1219" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1219" s="37" t="s">
         <v>1386</v>
       </c>
@@ -27454,7 +27462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1220" spans="1:5" ht="15" thickBot="1">
+    <row r="1220" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1220" s="37" t="s">
         <v>1387</v>
       </c>
@@ -27469,7 +27477,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1221" spans="1:5" ht="15" thickBot="1">
+    <row r="1221" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1221" s="37" t="s">
         <v>1388</v>
       </c>
@@ -27484,7 +27492,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1222" spans="1:5" ht="15" thickBot="1">
+    <row r="1222" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1222" s="37" t="s">
         <v>1389</v>
       </c>
@@ -27499,7 +27507,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1223" spans="1:5" ht="15" thickBot="1">
+    <row r="1223" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1223" s="37" t="s">
         <v>1390</v>
       </c>
@@ -27514,7 +27522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1224" spans="1:5" ht="15" thickBot="1">
+    <row r="1224" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1224" s="37" t="s">
         <v>1391</v>
       </c>
@@ -27529,7 +27537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1225" spans="1:5" ht="15" thickBot="1">
+    <row r="1225" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1225" s="37" t="s">
         <v>1392</v>
       </c>
@@ -27544,7 +27552,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1226" spans="1:5" ht="15" thickBot="1">
+    <row r="1226" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1226" s="37" t="s">
         <v>1393</v>
       </c>
@@ -27559,7 +27567,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1227" spans="1:5" ht="15" thickBot="1">
+    <row r="1227" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1227" s="37" t="s">
         <v>1394</v>
       </c>
@@ -27574,7 +27582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1228" spans="1:5" ht="15" thickBot="1">
+    <row r="1228" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1228" s="37" t="s">
         <v>1395</v>
       </c>
@@ -27589,7 +27597,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1229" spans="1:5" ht="15" thickBot="1">
+    <row r="1229" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1229" s="37" t="s">
         <v>1396</v>
       </c>
@@ -27604,7 +27612,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1230" spans="1:5" ht="15" thickBot="1">
+    <row r="1230" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1230" s="37" t="s">
         <v>1397</v>
       </c>
@@ -27619,7 +27627,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1231" spans="1:5" ht="15" thickBot="1">
+    <row r="1231" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1231" s="37" t="s">
         <v>1398</v>
       </c>
@@ -27634,7 +27642,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1232" spans="1:5" ht="15" thickBot="1">
+    <row r="1232" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1232" s="37" t="s">
         <v>1399</v>
       </c>
@@ -27649,7 +27657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1233" spans="1:5" ht="15" thickBot="1">
+    <row r="1233" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1233" s="37" t="s">
         <v>1400</v>
       </c>
@@ -27664,7 +27672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1234" spans="1:5" ht="15" thickBot="1">
+    <row r="1234" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1234" s="37" t="s">
         <v>1401</v>
       </c>
@@ -27679,7 +27687,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1235" spans="1:5" ht="15" thickBot="1">
+    <row r="1235" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1235" s="37" t="s">
         <v>1402</v>
       </c>
@@ -27694,7 +27702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1236" spans="1:5" ht="15" thickBot="1">
+    <row r="1236" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1236" s="37" t="s">
         <v>1403</v>
       </c>
@@ -27709,7 +27717,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1237" spans="1:5" ht="15" thickBot="1">
+    <row r="1237" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1237" s="37" t="s">
         <v>1404</v>
       </c>
@@ -27724,7 +27732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1238" spans="1:5" ht="15" thickBot="1">
+    <row r="1238" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1238" s="37" t="s">
         <v>1405</v>
       </c>
@@ -27739,7 +27747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1239" spans="1:5" ht="15" thickBot="1">
+    <row r="1239" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1239" s="37" t="s">
         <v>1406</v>
       </c>
@@ -27754,7 +27762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1240" spans="1:5" ht="15" thickBot="1">
+    <row r="1240" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1240" s="37" t="s">
         <v>1407</v>
       </c>
@@ -27769,7 +27777,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1241" spans="1:5" ht="15" thickBot="1">
+    <row r="1241" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1241" s="37" t="s">
         <v>1408</v>
       </c>
@@ -27784,7 +27792,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1242" spans="1:5" ht="15" thickBot="1">
+    <row r="1242" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1242" s="37" t="s">
         <v>1409</v>
       </c>
@@ -27799,7 +27807,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1243" spans="1:5" ht="15" thickBot="1">
+    <row r="1243" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1243" s="37" t="s">
         <v>1410</v>
       </c>
@@ -27814,7 +27822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1244" spans="1:5" ht="15" thickBot="1">
+    <row r="1244" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1244" s="37" t="s">
         <v>1411</v>
       </c>
@@ -27829,7 +27837,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1245" spans="1:5" ht="15" thickBot="1">
+    <row r="1245" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1245" s="37" t="s">
         <v>1412</v>
       </c>
@@ -27844,7 +27852,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1246" spans="1:5" ht="15" thickBot="1">
+    <row r="1246" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1246" s="37" t="s">
         <v>1413</v>
       </c>
@@ -27859,7 +27867,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1247" spans="1:5" ht="15" thickBot="1">
+    <row r="1247" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1247" s="37" t="s">
         <v>1414</v>
       </c>
@@ -27874,7 +27882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1248" spans="1:5" ht="15" thickBot="1">
+    <row r="1248" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1248" s="37" t="s">
         <v>1415</v>
       </c>
@@ -27889,7 +27897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1249" spans="1:5" ht="15" thickBot="1">
+    <row r="1249" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1249" s="37" t="s">
         <v>1416</v>
       </c>
@@ -27904,7 +27912,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1250" spans="1:5" ht="15" thickBot="1">
+    <row r="1250" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1250" s="37" t="s">
         <v>1417</v>
       </c>
@@ -27919,7 +27927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1251" spans="1:5" ht="15" thickBot="1">
+    <row r="1251" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1251" s="37" t="s">
         <v>1418</v>
       </c>
@@ -27934,7 +27942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1252" spans="1:5" ht="15" thickBot="1">
+    <row r="1252" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1252" s="37" t="s">
         <v>1419</v>
       </c>
@@ -27949,7 +27957,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1253" spans="1:5" ht="15" thickBot="1">
+    <row r="1253" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1253" s="37" t="s">
         <v>1420</v>
       </c>
@@ -27964,7 +27972,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1254" spans="1:5" ht="15" thickBot="1">
+    <row r="1254" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1254" s="37" t="s">
         <v>1421</v>
       </c>
@@ -27979,7 +27987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1255" spans="1:5" ht="15" thickBot="1">
+    <row r="1255" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1255" s="37" t="s">
         <v>1422</v>
       </c>
@@ -27994,7 +28002,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1256" spans="1:5" ht="15" thickBot="1">
+    <row r="1256" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1256" s="37" t="s">
         <v>1423</v>
       </c>
@@ -28009,7 +28017,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1257" spans="1:5" ht="15" thickBot="1">
+    <row r="1257" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1257" s="37" t="s">
         <v>1424</v>
       </c>
@@ -28024,7 +28032,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1258" spans="1:5" ht="15" thickBot="1">
+    <row r="1258" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1258" s="37" t="s">
         <v>1425</v>
       </c>
@@ -28039,7 +28047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1259" spans="1:5" ht="15" thickBot="1">
+    <row r="1259" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1259" s="37" t="s">
         <v>1426</v>
       </c>
@@ -28054,7 +28062,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1260" spans="1:5" ht="15" thickBot="1">
+    <row r="1260" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1260" s="37" t="s">
         <v>1427</v>
       </c>
@@ -28069,7 +28077,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1261" spans="1:5" ht="15" thickBot="1">
+    <row r="1261" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1261" s="37" t="s">
         <v>1428</v>
       </c>
@@ -28084,7 +28092,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1262" spans="1:5" ht="15" thickBot="1">
+    <row r="1262" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1262" s="37" t="s">
         <v>1429</v>
       </c>
@@ -28099,7 +28107,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1263" spans="1:5" ht="15" thickBot="1">
+    <row r="1263" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1263" s="37" t="s">
         <v>1430</v>
       </c>
@@ -28114,7 +28122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1264" spans="1:5" ht="15" thickBot="1">
+    <row r="1264" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1264" s="37" t="s">
         <v>1431</v>
       </c>
@@ -28129,7 +28137,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1265" spans="1:5" ht="15" thickBot="1">
+    <row r="1265" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1265" s="37" t="s">
         <v>1432</v>
       </c>
@@ -28144,7 +28152,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1266" spans="1:5" ht="15" thickBot="1">
+    <row r="1266" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1266" s="37" t="s">
         <v>1433</v>
       </c>
@@ -28159,7 +28167,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1267" spans="1:5" ht="15" thickBot="1">
+    <row r="1267" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1267" s="37" t="s">
         <v>1434</v>
       </c>
@@ -28174,7 +28182,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1268" spans="1:5" ht="15" thickBot="1">
+    <row r="1268" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1268" s="37" t="s">
         <v>1435</v>
       </c>
@@ -28189,7 +28197,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1269" spans="1:5" ht="15" thickBot="1">
+    <row r="1269" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1269" s="37" t="s">
         <v>1436</v>
       </c>
@@ -28204,7 +28212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1270" spans="1:5" ht="15" thickBot="1">
+    <row r="1270" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1270" s="37" t="s">
         <v>1437</v>
       </c>
@@ -28219,7 +28227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1271" spans="1:5" ht="15" thickBot="1">
+    <row r="1271" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1271" s="37" t="s">
         <v>1438</v>
       </c>
@@ -28234,7 +28242,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1272" spans="1:5" ht="15" thickBot="1">
+    <row r="1272" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1272" s="37" t="s">
         <v>1439</v>
       </c>
@@ -28249,7 +28257,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1273" spans="1:5" ht="15" thickBot="1">
+    <row r="1273" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1273" s="37" t="s">
         <v>1440</v>
       </c>
@@ -28264,7 +28272,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1274" spans="1:5" ht="15" thickBot="1">
+    <row r="1274" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1274" s="37" t="s">
         <v>1441</v>
       </c>
@@ -28279,7 +28287,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1275" spans="1:5" ht="15" thickBot="1">
+    <row r="1275" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1275" s="37" t="s">
         <v>1442</v>
       </c>
@@ -28294,7 +28302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1276" spans="1:5" ht="15" thickBot="1">
+    <row r="1276" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1276" s="37" t="s">
         <v>1443</v>
       </c>
@@ -28309,7 +28317,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1277" spans="1:5" ht="15" thickBot="1">
+    <row r="1277" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1277" s="37" t="s">
         <v>1444</v>
       </c>
@@ -28324,7 +28332,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1278" spans="1:5" ht="15" thickBot="1">
+    <row r="1278" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1278" s="37" t="s">
         <v>1445</v>
       </c>
@@ -28339,7 +28347,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1279" spans="1:5" ht="15" thickBot="1">
+    <row r="1279" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1279" s="37" t="s">
         <v>1446</v>
       </c>
@@ -28354,7 +28362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1280" spans="1:5" ht="15" thickBot="1">
+    <row r="1280" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1280" s="37" t="s">
         <v>1447</v>
       </c>
@@ -28369,7 +28377,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1281" spans="1:5" ht="15" thickBot="1">
+    <row r="1281" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1281" s="37" t="s">
         <v>1448</v>
       </c>
@@ -28384,7 +28392,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1282" spans="1:5" ht="15" thickBot="1">
+    <row r="1282" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1282" s="37" t="s">
         <v>1449</v>
       </c>
@@ -28399,7 +28407,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1283" spans="1:5" ht="15" thickBot="1">
+    <row r="1283" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1283" s="37" t="s">
         <v>1450</v>
       </c>
@@ -28414,7 +28422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1284" spans="1:5" ht="15" thickBot="1">
+    <row r="1284" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1284" s="37" t="s">
         <v>1451</v>
       </c>
@@ -28429,7 +28437,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1285" spans="1:5" ht="15" thickBot="1">
+    <row r="1285" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1285" s="37" t="s">
         <v>1452</v>
       </c>
@@ -28444,7 +28452,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1286" spans="1:5" ht="15" thickBot="1">
+    <row r="1286" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1286" s="37" t="s">
         <v>1453</v>
       </c>
@@ -28459,7 +28467,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1287" spans="1:5" ht="15" thickBot="1">
+    <row r="1287" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1287" s="37" t="s">
         <v>1454</v>
       </c>
@@ -28474,7 +28482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1288" spans="1:5" ht="15" thickBot="1">
+    <row r="1288" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1288" s="37" t="s">
         <v>1455</v>
       </c>
@@ -28489,7 +28497,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1289" spans="1:5" ht="15" thickBot="1">
+    <row r="1289" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1289" s="37" t="s">
         <v>1456</v>
       </c>
@@ -28504,7 +28512,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1290" spans="1:5" ht="15" thickBot="1">
+    <row r="1290" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1290" s="37" t="s">
         <v>1457</v>
       </c>
@@ -28519,7 +28527,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1291" spans="1:5" ht="15" thickBot="1">
+    <row r="1291" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1291" s="37" t="s">
         <v>1458</v>
       </c>
@@ -28534,7 +28542,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1292" spans="1:5" ht="15" thickBot="1">
+    <row r="1292" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1292" s="37" t="s">
         <v>1459</v>
       </c>
@@ -28549,7 +28557,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1293" spans="1:5" ht="15" thickBot="1">
+    <row r="1293" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1293" s="37" t="s">
         <v>1460</v>
       </c>
@@ -28564,7 +28572,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1294" spans="1:5" ht="15" thickBot="1">
+    <row r="1294" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1294" s="37" t="s">
         <v>1461</v>
       </c>
@@ -28579,7 +28587,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1295" spans="1:5" ht="15" thickBot="1">
+    <row r="1295" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1295" s="37" t="s">
         <v>1462</v>
       </c>
@@ -28594,7 +28602,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1296" spans="1:5" ht="15" thickBot="1">
+    <row r="1296" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1296" s="37" t="s">
         <v>1463</v>
       </c>
@@ -28609,7 +28617,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1297" spans="1:5" ht="15" thickBot="1">
+    <row r="1297" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1297" s="37" t="s">
         <v>1464</v>
       </c>
@@ -28624,7 +28632,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1298" spans="1:5" ht="15" thickBot="1">
+    <row r="1298" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1298" s="37" t="s">
         <v>1465</v>
       </c>
@@ -28639,7 +28647,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1299" spans="1:5" ht="15" thickBot="1">
+    <row r="1299" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1299" s="37" t="s">
         <v>1466</v>
       </c>
@@ -28654,7 +28662,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1300" spans="1:5" ht="15" thickBot="1">
+    <row r="1300" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1300" s="37" t="s">
         <v>1467</v>
       </c>
@@ -28669,7 +28677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1301" spans="1:5" ht="15" thickBot="1">
+    <row r="1301" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1301" s="37" t="s">
         <v>1468</v>
       </c>
@@ -28684,7 +28692,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1302" spans="1:5" ht="15" thickBot="1">
+    <row r="1302" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1302" s="37" t="s">
         <v>1469</v>
       </c>
@@ -28699,7 +28707,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1303" spans="1:5" ht="15" thickBot="1">
+    <row r="1303" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1303" s="37" t="s">
         <v>1470</v>
       </c>
@@ -28714,7 +28722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1304" spans="1:5" ht="15" thickBot="1">
+    <row r="1304" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1304" s="37" t="s">
         <v>1471</v>
       </c>
@@ -28729,7 +28737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1305" spans="1:5" ht="15" thickBot="1">
+    <row r="1305" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1305" s="37" t="s">
         <v>1472</v>
       </c>
@@ -28744,7 +28752,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1306" spans="1:5" ht="15" thickBot="1">
+    <row r="1306" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1306" s="37" t="s">
         <v>1473</v>
       </c>
@@ -28759,7 +28767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1307" spans="1:5" ht="15" thickBot="1">
+    <row r="1307" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1307" s="37" t="s">
         <v>1474</v>
       </c>
@@ -28774,7 +28782,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1308" spans="1:5" ht="15" thickBot="1">
+    <row r="1308" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1308" s="37" t="s">
         <v>1475</v>
       </c>
@@ -28789,7 +28797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1309" spans="1:5" ht="15" thickBot="1">
+    <row r="1309" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1309" s="37" t="s">
         <v>1476</v>
       </c>
@@ -28804,7 +28812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1310" spans="1:5" ht="15" thickBot="1">
+    <row r="1310" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1310" s="37" t="s">
         <v>1477</v>
       </c>
@@ -28819,7 +28827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1311" spans="1:5" ht="15" thickBot="1">
+    <row r="1311" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1311" s="37" t="s">
         <v>1478</v>
       </c>
@@ -28834,7 +28842,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1312" spans="1:5" ht="15" thickBot="1">
+    <row r="1312" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1312" s="37" t="s">
         <v>1479</v>
       </c>
@@ -28849,7 +28857,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1313" spans="1:5" ht="15" thickBot="1">
+    <row r="1313" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1313" s="37" t="s">
         <v>1480</v>
       </c>
@@ -28864,7 +28872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1314" spans="1:5" ht="15" thickBot="1">
+    <row r="1314" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1314" s="37" t="s">
         <v>1481</v>
       </c>
@@ -28879,7 +28887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1315" spans="1:5" ht="15" thickBot="1">
+    <row r="1315" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1315" s="37" t="s">
         <v>1482</v>
       </c>
@@ -28894,7 +28902,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1316" spans="1:5" ht="15" thickBot="1">
+    <row r="1316" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1316" s="37" t="s">
         <v>1483</v>
       </c>
@@ -28909,7 +28917,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1317" spans="1:5" ht="15" thickBot="1">
+    <row r="1317" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1317" s="37" t="s">
         <v>1484</v>
       </c>
@@ -28924,7 +28932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1318" spans="1:5" ht="15" thickBot="1">
+    <row r="1318" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1318" s="37" t="s">
         <v>1485</v>
       </c>
@@ -28939,7 +28947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1319" spans="1:5" ht="15" thickBot="1">
+    <row r="1319" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1319" s="37" t="s">
         <v>1486</v>
       </c>
@@ -28954,7 +28962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1320" spans="1:5" ht="15" thickBot="1">
+    <row r="1320" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1320" s="37" t="s">
         <v>1487</v>
       </c>
@@ -28969,7 +28977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1321" spans="1:5" ht="15" thickBot="1">
+    <row r="1321" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1321" s="37" t="s">
         <v>1488</v>
       </c>
@@ -28984,7 +28992,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1322" spans="1:5" ht="15" thickBot="1">
+    <row r="1322" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1322" s="37" t="s">
         <v>1489</v>
       </c>
@@ -28999,7 +29007,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1323" spans="1:5" ht="15" thickBot="1">
+    <row r="1323" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1323" s="37" t="s">
         <v>1490</v>
       </c>
@@ -29014,7 +29022,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1324" spans="1:5" ht="15" thickBot="1">
+    <row r="1324" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1324" s="37" t="s">
         <v>1491</v>
       </c>
@@ -29029,7 +29037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1325" spans="1:5" ht="15" thickBot="1">
+    <row r="1325" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1325" s="37" t="s">
         <v>1492</v>
       </c>
@@ -29044,7 +29052,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1326" spans="1:5" ht="15" thickBot="1">
+    <row r="1326" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1326" s="37" t="s">
         <v>1493</v>
       </c>
@@ -29059,7 +29067,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1327" spans="1:5" ht="15" thickBot="1">
+    <row r="1327" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1327" s="37" t="s">
         <v>1494</v>
       </c>
@@ -29074,7 +29082,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1328" spans="1:5" ht="15" thickBot="1">
+    <row r="1328" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1328" s="37" t="s">
         <v>1495</v>
       </c>
@@ -29089,7 +29097,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1329" spans="1:5" ht="15" thickBot="1">
+    <row r="1329" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1329" s="37" t="s">
         <v>1496</v>
       </c>
@@ -29104,7 +29112,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1330" spans="1:5" ht="15" thickBot="1">
+    <row r="1330" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1330" s="37" t="s">
         <v>1497</v>
       </c>
@@ -29119,7 +29127,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1331" spans="1:5" ht="15" thickBot="1">
+    <row r="1331" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1331" s="37" t="s">
         <v>1498</v>
       </c>
@@ -29134,9 +29142,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1332" spans="1:5" ht="15" thickBot="1">
+    <row r="1332" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1332" s="37" t="s">
-        <v>1499</v>
+        <v>1572</v>
       </c>
       <c r="B1332" s="37"/>
       <c r="C1332" s="13" t="s">
@@ -29149,9 +29157,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1333" spans="1:5" ht="15" thickBot="1">
+    <row r="1333" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1333" s="37" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="B1333" s="37"/>
       <c r="C1333" s="13" t="s">
@@ -29164,9 +29172,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1334" spans="1:5" ht="15" thickBot="1">
+    <row r="1334" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1334" s="37" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B1334" s="37"/>
       <c r="C1334" s="13" t="s">
@@ -29179,9 +29187,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1335" spans="1:5" ht="15" thickBot="1">
+    <row r="1335" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1335" s="37" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B1335" s="37"/>
       <c r="C1335" s="13" t="s">
@@ -29194,9 +29202,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1336" spans="1:5" ht="15" thickBot="1">
+    <row r="1336" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1336" s="37" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B1336" s="37"/>
       <c r="C1336" s="13" t="s">
@@ -29209,9 +29217,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1337" spans="1:5" ht="15" thickBot="1">
+    <row r="1337" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1337" s="37" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B1337" s="37"/>
       <c r="C1337" s="13" t="s">
@@ -29224,9 +29232,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1338" spans="1:5" ht="15" thickBot="1">
+    <row r="1338" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1338" s="37" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B1338" s="37"/>
       <c r="C1338" s="13" t="s">
@@ -29239,9 +29247,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1339" spans="1:5" ht="15" thickBot="1">
+    <row r="1339" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1339" s="37" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="B1339" s="37"/>
       <c r="C1339" s="13" t="s">
@@ -29254,9 +29262,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1340" spans="1:5" ht="15" thickBot="1">
+    <row r="1340" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1340" s="37" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B1340" s="37"/>
       <c r="C1340" s="13" t="s">
@@ -29269,9 +29277,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1341" spans="1:5" ht="15" thickBot="1">
+    <row r="1341" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1341" s="37" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B1341" s="37"/>
       <c r="C1341" s="13" t="s">
@@ -29284,9 +29292,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1342" spans="1:5" ht="15" thickBot="1">
+    <row r="1342" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1342" s="37" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B1342" s="37"/>
       <c r="C1342" s="13" t="s">
@@ -29299,9 +29307,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1343" spans="1:5" ht="15" thickBot="1">
+    <row r="1343" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1343" s="37" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B1343" s="37"/>
       <c r="C1343" s="13" t="s">
@@ -29314,9 +29322,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1344" spans="1:5" ht="15" thickBot="1">
+    <row r="1344" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1344" s="37" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B1344" s="37"/>
       <c r="C1344" s="13" t="s">
@@ -29326,6 +29334,51 @@
         <v>35</v>
       </c>
       <c r="E1344" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1345" s="37" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B1345" s="37"/>
+      <c r="C1345" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1345" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1345" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1346" s="37" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B1346" s="37"/>
+      <c r="C1346" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1346" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1346" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1347" s="37" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B1347" s="37"/>
+      <c r="C1347" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1347" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1347" s="40" t="s">
         <v>36</v>
       </c>
     </row>
@@ -30145,7 +30198,7 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1125:D1344">
+  <conditionalFormatting sqref="D1125:D1347">
     <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Skip:">
       <formula>NOT(ISERROR(SEARCH("Skip:",D1125)))</formula>
     </cfRule>
@@ -30156,7 +30209,7 @@
       <formula>NOT(ISERROR(SEARCH("Pass",D1125)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1125:E1344">
+  <conditionalFormatting sqref="E1125:E1347">
     <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"LOW"</formula>
     </cfRule>
@@ -30190,15 +30243,15 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1125:E1344" xr:uid="{06C3568A-7D93-48FB-88C0-C2CF3E220F24}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1125:E1347">
       <formula1>"High,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1344" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1347">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1124" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1124">
       <formula1>"High,Low"</formula1>
     </dataValidation>
   </dataValidations>
@@ -30208,14 +30261,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:22" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
@@ -30312,17 +30365,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="19" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1" collapsed="1"/>
     <col min="6" max="1025" width="19" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -30865,10 +30918,10 @@
         <v>1204</v>
       </c>
       <c r="D25" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="F25" t="s">
         <v>1200</v>
@@ -30888,10 +30941,10 @@
         <v>1211</v>
       </c>
       <c r="D26" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>1515</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>1516</v>
       </c>
       <c r="F26" t="s">
         <v>1200</v>
@@ -30911,10 +30964,10 @@
         <v>1217</v>
       </c>
       <c r="D27" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="F27" t="s">
         <v>1245</v>
@@ -30934,10 +30987,10 @@
         <v>1221</v>
       </c>
       <c r="D28" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>1518</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>1519</v>
       </c>
       <c r="F28" t="s">
         <v>1245</v>
@@ -30957,10 +31010,10 @@
         <v>1301</v>
       </c>
       <c r="D29" t="s">
+        <v>1519</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>1520</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>1521</v>
       </c>
       <c r="F29" t="s">
         <v>1245</v>
@@ -30980,10 +31033,10 @@
         <v>1303</v>
       </c>
       <c r="D30" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>1522</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>1523</v>
       </c>
       <c r="F30" t="s">
         <v>1245</v>
@@ -30994,14 +31047,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E24" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E25" r:id="rId3" xr:uid="{7806A812-C6F5-4A7B-992F-0BEA7A5F470D}"/>
-    <hyperlink ref="E26" r:id="rId4" xr:uid="{FC4568AB-971B-4E8C-A06E-A0A45C13A637}"/>
-    <hyperlink ref="E27" r:id="rId5" xr:uid="{25E208B5-38F8-439B-9EFC-59D5E119AB11}"/>
-    <hyperlink ref="E28" r:id="rId6" xr:uid="{E363E46A-48E9-48DF-8230-3E34F64ECC39}"/>
-    <hyperlink ref="E29" r:id="rId7" xr:uid="{E9CE28AE-D08B-46C3-AFE8-8B4817B4493E}"/>
-    <hyperlink ref="E30" r:id="rId8" xr:uid="{0A25DF2B-93D8-44FA-B853-966A18A1BDCA}"/>
+    <hyperlink ref="E23" r:id="rId1"/>
+    <hyperlink ref="E24" r:id="rId2"/>
+    <hyperlink ref="E25" r:id="rId3"/>
+    <hyperlink ref="E26" r:id="rId4"/>
+    <hyperlink ref="E27" r:id="rId5"/>
+    <hyperlink ref="E28" r:id="rId6"/>
+    <hyperlink ref="E29" r:id="rId7"/>
+    <hyperlink ref="E30" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>